<commit_message>
delete garbage Ingredient Types and add usable list of Ingredient Types
</commit_message>
<xml_diff>
--- a/Ingredients and Types.xlsx
+++ b/Ingredients and Types.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Matthew/Documents/Coding/PersonalProjects/recipeConverter/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51DE5B8B-22D3-E544-BB4A-43C97C862631}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B697403-5018-FA48-AA6B-BF1D1C9B233A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4920" yWindow="860" windowWidth="39780" windowHeight="23260" xr2:uid="{2D2F75AA-471C-5F46-928E-911BD0472A90}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="456">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="454">
   <si>
     <t>Baked Goods, Dry</t>
   </si>
@@ -500,9 +500,6 @@
     <t>Vegetables</t>
   </si>
   <si>
-    <t xml:space="preserve">Miscellaneous </t>
-  </si>
-  <si>
     <t>Corn flour</t>
   </si>
   <si>
@@ -1383,9 +1380,6 @@
   </si>
   <si>
     <t>Lime Juice</t>
-  </si>
-  <si>
-    <t>451 total ingredients</t>
   </si>
   <si>
     <t>16 Catagories</t>
@@ -1858,7 +1852,7 @@
   <dimension ref="B1:AC52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1902,7 +1896,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>3</v>
@@ -1920,7 +1914,7 @@
         <v>4</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>152</v>
@@ -1956,43 +1950,43 @@
         <v>14</v>
       </c>
       <c r="G2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="H2" t="s">
         <v>15</v>
       </c>
       <c r="I2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J2" t="s">
         <v>84</v>
       </c>
       <c r="K2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="L2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="M2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="N2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="O2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="P2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="Q2" t="s">
         <v>12</v>
       </c>
       <c r="R2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="S2" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="T2" t="s">
         <v>122</v>
@@ -2007,46 +2001,46 @@
         <v>17</v>
       </c>
       <c r="F3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="G3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="H3" t="s">
         <v>16</v>
       </c>
       <c r="I3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="J3" t="s">
         <v>75</v>
       </c>
       <c r="K3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="L3" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="M3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="N3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="O3" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="P3" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="Q3" t="s">
         <v>145</v>
       </c>
       <c r="R3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="S3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="T3" t="s">
         <v>119</v>
@@ -2054,7 +2048,7 @@
     </row>
     <row r="4" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C4" s="5"/>
       <c r="E4" t="s">
@@ -2064,43 +2058,43 @@
         <v>64</v>
       </c>
       <c r="G4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="H4" t="s">
         <v>19</v>
       </c>
       <c r="I4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J4" t="s">
         <v>91</v>
       </c>
       <c r="K4" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="L4" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="M4" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="N4" t="s">
         <v>72</v>
       </c>
       <c r="O4" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="P4" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="Q4" t="s">
         <v>39</v>
       </c>
       <c r="R4" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="S4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="T4" t="s">
         <v>118</v>
@@ -2112,7 +2106,7 @@
       </c>
       <c r="C5" s="5"/>
       <c r="E5" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F5" t="s">
         <v>63</v>
@@ -2124,37 +2118,37 @@
         <v>62</v>
       </c>
       <c r="I5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J5" t="s">
         <v>79</v>
       </c>
       <c r="K5" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="L5" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="M5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="N5" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="O5" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="P5" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="Q5" t="s">
         <v>40</v>
       </c>
       <c r="R5" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="S5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="T5" t="s">
         <v>106</v>
@@ -2172,43 +2166,43 @@
         <v>66</v>
       </c>
       <c r="G6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H6" t="s">
         <v>49</v>
       </c>
       <c r="I6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J6" t="s">
         <v>87</v>
       </c>
       <c r="K6" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="L6" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="M6" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="N6" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="O6" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="P6" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="Q6" t="s">
         <v>41</v>
       </c>
       <c r="R6" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="S6" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="T6" t="s">
         <v>109</v>
@@ -2220,13 +2214,13 @@
       </c>
       <c r="C7" s="5"/>
       <c r="E7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F7" t="s">
         <v>45</v>
       </c>
       <c r="G7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="H7" t="s">
         <v>20</v>
@@ -2238,31 +2232,31 @@
         <v>23</v>
       </c>
       <c r="K7" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="L7" t="s">
         <v>137</v>
       </c>
       <c r="M7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="N7" t="s">
         <v>69</v>
       </c>
       <c r="O7" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="P7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="Q7" t="s">
         <v>42</v>
       </c>
       <c r="R7" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="S7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="T7" t="s">
         <v>121</v>
@@ -2280,10 +2274,10 @@
         <v>47</v>
       </c>
       <c r="G8" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H8" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="I8" t="s">
         <v>150</v>
@@ -2292,31 +2286,31 @@
         <v>81</v>
       </c>
       <c r="K8" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="L8" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="M8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="N8" t="s">
         <v>70</v>
       </c>
       <c r="O8" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="P8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="Q8" t="s">
         <v>143</v>
       </c>
       <c r="R8" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="S8" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="T8" t="s">
         <v>105</v>
@@ -2334,34 +2328,34 @@
         <v>46</v>
       </c>
       <c r="G9" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H9" t="s">
         <v>22</v>
       </c>
       <c r="I9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J9" t="s">
         <v>95</v>
       </c>
       <c r="K9" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="L9" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="M9" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="N9" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="O9" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="P9" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="Q9" t="s">
         <v>43</v>
@@ -2370,7 +2364,7 @@
         <v>140</v>
       </c>
       <c r="S9" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="T9" t="s">
         <v>113</v>
@@ -2378,7 +2372,7 @@
     </row>
     <row r="10" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B10" s="4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C10" s="5"/>
       <c r="E10" t="s">
@@ -2388,43 +2382,43 @@
         <v>65</v>
       </c>
       <c r="G10" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="H10" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="I10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J10" t="s">
         <v>94</v>
       </c>
       <c r="K10" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="L10" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="M10" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="N10" t="s">
         <v>71</v>
       </c>
       <c r="O10" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="P10" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="Q10" t="s">
         <v>142</v>
       </c>
       <c r="R10" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="S10" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="T10" t="s">
         <v>111</v>
@@ -2432,9 +2426,12 @@
     </row>
     <row r="11" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B11" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C11" s="5"/>
+      <c r="D11">
+        <v>10</v>
+      </c>
       <c r="E11" t="s">
         <v>59</v>
       </c>
@@ -2442,43 +2439,43 @@
         <v>67</v>
       </c>
       <c r="G11" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="H11" t="s">
         <v>48</v>
       </c>
       <c r="I11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="J11" t="s">
         <v>83</v>
       </c>
       <c r="K11" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="L11" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="M11" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="N11" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="O11" t="s">
         <v>136</v>
       </c>
       <c r="P11" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="Q11" t="s">
         <v>146</v>
       </c>
       <c r="R11" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="S11" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="T11" t="s">
         <v>128</v>
@@ -2496,40 +2493,40 @@
         <v>35</v>
       </c>
       <c r="G12" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="H12" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="I12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="J12" t="s">
         <v>88</v>
       </c>
       <c r="K12" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="L12" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="M12" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="O12" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="P12" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="Q12" t="s">
         <v>144</v>
       </c>
       <c r="R12" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="S12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="T12" t="s">
         <v>112</v>
@@ -2544,40 +2541,40 @@
         <v>60</v>
       </c>
       <c r="G13" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="H13" t="s">
         <v>26</v>
       </c>
       <c r="I13" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="J13" t="s">
         <v>92</v>
       </c>
       <c r="K13" t="s">
+        <v>309</v>
+      </c>
+      <c r="L13" t="s">
+        <v>405</v>
+      </c>
+      <c r="M13" t="s">
+        <v>198</v>
+      </c>
+      <c r="O13" t="s">
         <v>310</v>
-      </c>
-      <c r="L13" t="s">
-        <v>406</v>
-      </c>
-      <c r="M13" t="s">
-        <v>199</v>
-      </c>
-      <c r="O13" t="s">
-        <v>311</v>
       </c>
       <c r="P13" t="s">
         <v>13</v>
       </c>
       <c r="Q13" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="R13" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="S13" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="T13" t="s">
         <v>135</v>
@@ -2592,40 +2589,40 @@
         <v>58</v>
       </c>
       <c r="G14" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="H14" t="s">
         <v>27</v>
       </c>
       <c r="I14" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="J14" t="s">
         <v>89</v>
       </c>
       <c r="K14" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="L14" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="M14" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="O14" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="P14" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="Q14" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="R14" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="S14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="T14" t="s">
         <v>137</v>
@@ -2640,40 +2637,40 @@
         <v>61</v>
       </c>
       <c r="G15" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="H15" t="s">
         <v>28</v>
       </c>
       <c r="I15" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J15" t="s">
         <v>90</v>
       </c>
       <c r="K15" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="L15" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="M15" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="O15" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="P15" t="s">
         <v>36</v>
       </c>
       <c r="Q15" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="R15" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="S15" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="T15" t="s">
         <v>126</v>
@@ -2688,10 +2685,10 @@
         <v>54</v>
       </c>
       <c r="G16" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H16" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="I16" t="s">
         <v>149</v>
@@ -2700,28 +2697,28 @@
         <v>97</v>
       </c>
       <c r="K16" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="L16" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="M16" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="O16" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="P16" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="Q16" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="R16" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="S16" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="T16" t="s">
         <v>127</v>
@@ -2729,84 +2726,81 @@
     </row>
     <row r="17" spans="2:20" x14ac:dyDescent="0.2">
       <c r="E17" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="G17" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="H17" t="s">
         <v>51</v>
       </c>
       <c r="I17" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="J17" t="s">
         <v>80</v>
       </c>
       <c r="K17" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="L17" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="M17" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="O17" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="P17" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="Q17" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="R17" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="S17" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="T17" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="18" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B18" t="s">
-        <v>449</v>
-      </c>
       <c r="E18" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="G18" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="H18" t="s">
         <v>29</v>
       </c>
       <c r="I18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J18" t="s">
         <v>93</v>
       </c>
       <c r="K18" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="L18" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="M18" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="P18" t="s">
         <v>90</v>
       </c>
       <c r="R18" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="S18" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="T18" t="s">
         <v>115</v>
@@ -2814,113 +2808,120 @@
     </row>
     <row r="19" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
+        <v>448</v>
+      </c>
+      <c r="E19" t="s">
+        <v>440</v>
+      </c>
+      <c r="G19" t="s">
+        <v>263</v>
+      </c>
+      <c r="H19" t="s">
         <v>450</v>
       </c>
-      <c r="E19" t="s">
-        <v>441</v>
-      </c>
-      <c r="G19" t="s">
-        <v>264</v>
-      </c>
-      <c r="H19" t="s">
-        <v>452</v>
-      </c>
       <c r="I19" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="J19" t="s">
         <v>93</v>
       </c>
       <c r="K19" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L19" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="M19" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="P19" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="R19" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="S19" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="T19" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="20" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B20">
+        <f>SUM(29, 11, 34, 24, 37,31,51, 19, 33, 10, 16, 35, 16, 37, 32, 37)</f>
+        <v>452</v>
+      </c>
       <c r="E20" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="G20" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H20" t="s">
         <v>31</v>
       </c>
       <c r="I20" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="J20" t="s">
         <v>74</v>
       </c>
       <c r="K20" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="L20" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="M20" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="P20" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="R20" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="S20" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="T20" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="21" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="D21">
+        <v>20</v>
+      </c>
       <c r="E21" t="s">
         <v>30</v>
       </c>
       <c r="G21" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H21" t="s">
         <v>32</v>
       </c>
       <c r="I21" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J21" t="s">
         <v>82</v>
       </c>
       <c r="K21" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="M21" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="P21" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="R21" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="S21" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="T21" t="s">
         <v>131</v>
@@ -2928,34 +2929,34 @@
     </row>
     <row r="22" spans="2:20" x14ac:dyDescent="0.2">
       <c r="E22" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G22" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H22" t="s">
         <v>53</v>
       </c>
       <c r="I22" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="J22" t="s">
         <v>82</v>
       </c>
       <c r="K22" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="M22" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="P22" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="R22" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="S22" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="T22" t="s">
         <v>120</v>
@@ -2963,34 +2964,34 @@
     </row>
     <row r="23" spans="2:20" x14ac:dyDescent="0.2">
       <c r="E23" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="G23" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="H23" t="s">
         <v>50</v>
       </c>
       <c r="I23" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J23" t="s">
         <v>76</v>
       </c>
       <c r="K23" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="M23" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="P23" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="R23" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="S23" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="T23" t="s">
         <v>108</v>
@@ -2998,34 +2999,34 @@
     </row>
     <row r="24" spans="2:20" x14ac:dyDescent="0.2">
       <c r="E24" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="G24" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H24" t="s">
         <v>52</v>
       </c>
       <c r="I24" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J24" t="s">
         <v>96</v>
       </c>
       <c r="K24" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="M24" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="P24" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="R24" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="S24" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="T24" t="s">
         <v>124</v>
@@ -3033,16 +3034,16 @@
     </row>
     <row r="25" spans="2:20" x14ac:dyDescent="0.2">
       <c r="E25" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G25" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="H25" t="s">
         <v>33</v>
       </c>
       <c r="I25" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J25" t="s">
         <v>100</v>
@@ -3051,16 +3052,16 @@
         <v>127</v>
       </c>
       <c r="M25" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="P25" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="R25" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="S25" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="T25" t="s">
         <v>125</v>
@@ -3068,31 +3069,31 @@
     </row>
     <row r="26" spans="2:20" x14ac:dyDescent="0.2">
       <c r="E26" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="G26" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="I26" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J26" t="s">
         <v>98</v>
       </c>
       <c r="K26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="M26" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="P26" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="R26" t="s">
         <v>138</v>
       </c>
       <c r="S26" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="T26" t="s">
         <v>101</v>
@@ -3100,31 +3101,31 @@
     </row>
     <row r="27" spans="2:20" x14ac:dyDescent="0.2">
       <c r="E27" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G27" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="I27" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J27" t="s">
         <v>73</v>
       </c>
       <c r="K27" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="M27" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="P27" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="R27" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="S27" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="T27" t="s">
         <v>103</v>
@@ -3135,28 +3136,28 @@
         <v>57</v>
       </c>
       <c r="G28" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="I28" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J28" t="s">
         <v>99</v>
       </c>
       <c r="K28" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="M28" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="P28" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="R28" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="S28" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="T28" t="s">
         <v>117</v>
@@ -3167,48 +3168,51 @@
         <v>34</v>
       </c>
       <c r="G29" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="I29" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J29" t="s">
         <v>78</v>
       </c>
       <c r="K29" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="M29" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="P29" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="R29" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="S29" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="T29" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="30" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="D30">
+        <v>30</v>
+      </c>
       <c r="G30" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="I30" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="J30" t="s">
         <v>85</v>
       </c>
       <c r="K30" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="M30" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="P30" t="s">
         <v>37</v>
@@ -3217,7 +3221,7 @@
         <v>141</v>
       </c>
       <c r="S30" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="T30" t="s">
         <v>136</v>
@@ -3225,28 +3229,28 @@
     </row>
     <row r="31" spans="2:20" x14ac:dyDescent="0.2">
       <c r="G31" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="I31" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J31" t="s">
         <v>86</v>
       </c>
       <c r="K31" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="M31" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="P31" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="R31" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="S31" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="T31" t="s">
         <v>130</v>
@@ -3254,28 +3258,28 @@
     </row>
     <row r="32" spans="2:20" x14ac:dyDescent="0.2">
       <c r="G32" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="I32" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J32" t="s">
         <v>77</v>
       </c>
       <c r="K32" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="M32" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="P32" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="R32" t="s">
         <v>44</v>
       </c>
       <c r="S32" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="T32" t="s">
         <v>107</v>
@@ -3283,25 +3287,25 @@
     </row>
     <row r="33" spans="7:20" x14ac:dyDescent="0.2">
       <c r="G33" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="I33" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="K33" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="M33" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="P33" t="s">
         <v>38</v>
       </c>
       <c r="R33" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="S33" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="T33" t="s">
         <v>116</v>
@@ -3309,22 +3313,22 @@
     </row>
     <row r="34" spans="7:20" x14ac:dyDescent="0.2">
       <c r="G34" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="I34" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="K34" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="M34" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="P34" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="R34" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="T34" t="s">
         <v>132</v>
@@ -3332,16 +3336,16 @@
     </row>
     <row r="35" spans="7:20" x14ac:dyDescent="0.2">
       <c r="I35" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="K35" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P35" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="R35" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="T35" t="s">
         <v>114</v>
@@ -3349,16 +3353,16 @@
     </row>
     <row r="36" spans="7:20" x14ac:dyDescent="0.2">
       <c r="I36" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="K36" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="P36" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="R36" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="T36" t="s">
         <v>104</v>
@@ -3369,7 +3373,7 @@
         <v>147</v>
       </c>
       <c r="K37" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="R37" t="s">
         <v>139</v>
@@ -3383,10 +3387,10 @@
         <v>151</v>
       </c>
       <c r="K38" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="R38" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="T38" t="s">
         <v>110</v>
@@ -3394,72 +3398,72 @@
     </row>
     <row r="39" spans="7:20" x14ac:dyDescent="0.2">
       <c r="K39" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="40" spans="7:20" x14ac:dyDescent="0.2">
       <c r="K40" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="41" spans="7:20" x14ac:dyDescent="0.2">
       <c r="K41" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="42" spans="7:20" x14ac:dyDescent="0.2">
       <c r="K42" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="43" spans="7:20" x14ac:dyDescent="0.2">
       <c r="K43" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="44" spans="7:20" x14ac:dyDescent="0.2">
       <c r="K44" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="45" spans="7:20" x14ac:dyDescent="0.2">
       <c r="K45" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="46" spans="7:20" x14ac:dyDescent="0.2">
       <c r="K46" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="47" spans="7:20" x14ac:dyDescent="0.2">
       <c r="K47" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="48" spans="7:20" x14ac:dyDescent="0.2">
       <c r="K48" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="49" spans="11:11" x14ac:dyDescent="0.2">
       <c r="K49" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="50" spans="11:11" x14ac:dyDescent="0.2">
       <c r="K50" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="51" spans="11:11" x14ac:dyDescent="0.2">
       <c r="K51" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="52" spans="11:11" x14ac:dyDescent="0.2">
       <c r="K52" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update textFiles/*.txt with inputted data for multiple ingredient types
</commit_message>
<xml_diff>
--- a/Ingredients and Types.xlsx
+++ b/Ingredients and Types.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Matthew/Documents/Coding/PersonalProjects/recipeConverter/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74FF55E8-89C5-4345-AB0F-D037236DBF75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2B39DAB-9D0B-8549-95F5-B9FE0305AE3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4920" yWindow="860" windowWidth="39780" windowHeight="23260" xr2:uid="{2D2F75AA-471C-5F46-928E-911BD0472A90}"/>
+    <workbookView xWindow="1060" yWindow="1900" windowWidth="39780" windowHeight="23260" xr2:uid="{2D2F75AA-471C-5F46-928E-911BD0472A90}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="527">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="531">
   <si>
     <t>Baked Goods, Dry</t>
   </si>
@@ -443,9 +443,6 @@
     <t>Cherries</t>
   </si>
   <si>
-    <t>Dragon fruit</t>
-  </si>
-  <si>
     <t>Starfruit</t>
   </si>
   <si>
@@ -695,9 +692,6 @@
     <t>Provolone</t>
   </si>
   <si>
-    <t>Neufchâtel</t>
-  </si>
-  <si>
     <t>Paneer</t>
   </si>
   <si>
@@ -1286,9 +1280,6 @@
     <t>Avocado</t>
   </si>
   <si>
-    <t>Apple</t>
-  </si>
-  <si>
     <t>Apricot, Chopped</t>
   </si>
   <si>
@@ -1496,9 +1487,6 @@
     <t>Coconut, Shredded</t>
   </si>
   <si>
-    <t>Coconut</t>
-  </si>
-  <si>
     <t>Lotus Root</t>
   </si>
   <si>
@@ -1617,6 +1605,30 @@
   </si>
   <si>
     <t>14 Catagories</t>
+  </si>
+  <si>
+    <t>Neufchatel</t>
+  </si>
+  <si>
+    <t>Garlic, Sliced</t>
+  </si>
+  <si>
+    <t>Garlic, Minced</t>
+  </si>
+  <si>
+    <t>Apple, Chopped</t>
+  </si>
+  <si>
+    <t>Banana, Sliced</t>
+  </si>
+  <si>
+    <t>Coconut, Dessicated</t>
+  </si>
+  <si>
+    <t>Coconut, Raw</t>
+  </si>
+  <si>
+    <t>Dragon Fruit</t>
   </si>
 </sst>
 </file>
@@ -1626,7 +1638,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1652,6 +1664,14 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1734,10 +1754,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1756,8 +1777,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2093,10 +2116,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:AS60"/>
+  <dimension ref="B1:AS62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2111,7 +2134,7 @@
     <col min="10" max="10" width="11.5" customWidth="1"/>
     <col min="11" max="11" width="18.83203125" customWidth="1"/>
     <col min="12" max="12" width="11.5" customWidth="1"/>
-    <col min="13" max="13" width="17.5" customWidth="1"/>
+    <col min="13" max="13" width="20.1640625" customWidth="1"/>
     <col min="14" max="14" width="11.5" customWidth="1"/>
     <col min="15" max="15" width="25.1640625" customWidth="1"/>
     <col min="16" max="16" width="11.5" customWidth="1"/>
@@ -2151,97 +2174,97 @@
         <v>0</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="I1" s="13" t="s">
         <v>6</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>384</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>235</v>
+        <v>382</v>
+      </c>
+      <c r="K1" s="14" t="s">
+        <v>233</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="N1" s="8" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="P1" s="8" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="R1" s="9" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="T1" s="8" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="V1" s="8" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="X1" s="8" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="Y1" s="1" t="s">
         <v>132</v>
       </c>
       <c r="Z1" s="8" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="AA1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="AB1" s="8" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="AC1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="AD1" s="9" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="AE1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="AF1" s="9" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="AG1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="AH1" s="8" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="AJ1" s="8" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="AK1" s="1"/>
       <c r="AQ1" s="1"/>
@@ -2263,22 +2286,22 @@
         <v>14</v>
       </c>
       <c r="H2" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="I2" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="J2" s="11">
         <v>112</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="14" t="s">
         <v>15</v>
       </c>
       <c r="L2" s="12">
         <v>130</v>
       </c>
       <c r="M2" t="s">
-        <v>416</v>
+        <v>526</v>
       </c>
       <c r="N2" s="12">
         <v>125</v>
@@ -2290,34 +2313,34 @@
         <v>245</v>
       </c>
       <c r="Q2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="R2" s="11">
         <v>6</v>
       </c>
       <c r="S2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="T2" s="11">
         <v>197</v>
       </c>
       <c r="U2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="W2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="X2" s="11">
         <v>244</v>
       </c>
       <c r="Y2" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="Z2" s="11" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="AA2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="AB2" s="11">
         <v>138</v>
@@ -2329,13 +2352,13 @@
         <v>13.75</v>
       </c>
       <c r="AE2" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="AF2" s="11">
         <v>17</v>
       </c>
       <c r="AG2" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="AH2" s="11"/>
       <c r="AI2" t="s">
@@ -2358,13 +2381,13 @@
         <v>13.8</v>
       </c>
       <c r="G3" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="H3" s="12">
         <v>218</v>
       </c>
       <c r="I3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J3" s="11">
         <v>245.43799999999999</v>
@@ -2376,7 +2399,7 @@
         <v>96</v>
       </c>
       <c r="M3" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="N3" s="12">
         <v>190</v>
@@ -2388,52 +2411,52 @@
         <v>157</v>
       </c>
       <c r="Q3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="R3" s="11">
         <v>6.7</v>
       </c>
       <c r="S3" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="T3" s="11">
         <v>140</v>
       </c>
       <c r="U3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="W3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="X3" s="11">
         <v>244</v>
       </c>
       <c r="Y3" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="Z3" s="11">
         <v>180</v>
       </c>
       <c r="AA3" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="AB3" s="11">
         <v>120</v>
       </c>
       <c r="AC3" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="AD3" s="11">
         <v>13.625</v>
       </c>
       <c r="AE3" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="AF3" s="11">
         <v>14.08</v>
       </c>
       <c r="AG3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AH3" s="11"/>
       <c r="AI3" t="s">
@@ -2445,14 +2468,14 @@
     </row>
     <row r="4" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C4" s="5"/>
       <c r="E4" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="G4" t="s">
         <v>52</v>
@@ -2461,19 +2484,19 @@
         <v>260</v>
       </c>
       <c r="I4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="J4" s="11">
         <v>232</v>
       </c>
       <c r="K4" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="L4" s="12">
         <v>103</v>
       </c>
       <c r="M4" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="N4" s="12">
         <v>150</v>
@@ -2485,19 +2508,19 @@
         <v>170</v>
       </c>
       <c r="Q4" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="R4" s="11">
         <v>2.1</v>
       </c>
       <c r="S4" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="T4" s="11">
         <v>194</v>
       </c>
       <c r="U4" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="W4" t="s">
         <v>60</v>
@@ -2506,31 +2529,31 @@
         <v>248.8</v>
       </c>
       <c r="Y4" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="Z4" s="11" t="s">
+        <v>476</v>
+      </c>
+      <c r="AA4" t="s">
         <v>479</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>482</v>
       </c>
       <c r="AB4" s="11">
         <v>133</v>
       </c>
       <c r="AC4" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="AD4" s="11">
         <v>13.625</v>
       </c>
       <c r="AE4" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="AF4" s="11">
         <v>17</v>
       </c>
       <c r="AG4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="AH4" s="11"/>
       <c r="AI4" t="s">
@@ -2549,7 +2572,7 @@
         <v>21</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="G5" t="s">
         <v>51</v>
@@ -2564,16 +2587,16 @@
         <v>226</v>
       </c>
       <c r="K5" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="L5" s="12">
         <v>128</v>
       </c>
       <c r="M5" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="N5" s="12">
-        <v>225</v>
+        <v>250</v>
       </c>
       <c r="O5" t="s">
         <v>75</v>
@@ -2582,53 +2605,53 @@
         <v>160</v>
       </c>
       <c r="Q5" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="R5" s="11">
         <v>1.5</v>
       </c>
       <c r="S5" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="T5" s="11">
         <v>172</v>
       </c>
       <c r="U5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="W5" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="X5" s="11">
         <v>247</v>
       </c>
       <c r="Y5" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="Z5" s="11">
         <v>80</v>
       </c>
       <c r="AA5" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="AB5" s="11">
         <f>16*16</f>
         <v>256</v>
       </c>
       <c r="AC5" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="AD5" s="11">
         <v>13.456</v>
       </c>
       <c r="AE5" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="AF5" s="11">
         <v>14.1</v>
       </c>
       <c r="AG5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="AH5" s="11"/>
       <c r="AI5" t="s">
@@ -2647,7 +2670,7 @@
         <v>23</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="G6" t="s">
         <v>54</v>
@@ -2656,22 +2679,22 @@
         <v>308</v>
       </c>
       <c r="I6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J6" s="11">
         <v>113</v>
       </c>
       <c r="K6" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="L6" s="12">
         <v>85</v>
       </c>
       <c r="M6" t="s">
-        <v>138</v>
+        <v>527</v>
       </c>
       <c r="N6" s="12">
-        <v>144</v>
+        <v>220</v>
       </c>
       <c r="O6" t="s">
         <v>23</v>
@@ -2680,34 +2703,34 @@
         <v>122</v>
       </c>
       <c r="Q6" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="R6" s="11">
         <v>1.8</v>
       </c>
       <c r="S6" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="T6" s="11">
         <v>202</v>
       </c>
       <c r="U6" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="W6" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="X6" s="11">
         <v>244</v>
       </c>
       <c r="Y6" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="Z6" s="11">
         <v>80</v>
       </c>
       <c r="AA6" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="AB6" s="11">
         <f>16*16</f>
@@ -2720,13 +2743,13 @@
         <v>13.625</v>
       </c>
       <c r="AE6" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="AF6" s="11">
         <v>15</v>
       </c>
       <c r="AG6" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="AH6" s="11"/>
       <c r="AI6" t="s">
@@ -2749,14 +2772,14 @@
         <v>8</v>
       </c>
       <c r="G7" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="H7" s="12">
         <f>H8-H9</f>
         <v>38</v>
       </c>
       <c r="I7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J7" s="11">
         <v>226.667</v>
@@ -2768,10 +2791,10 @@
         <v>139</v>
       </c>
       <c r="M7" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="N7" s="12">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="O7" t="s">
         <v>69</v>
@@ -2780,19 +2803,19 @@
         <v>173</v>
       </c>
       <c r="Q7" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="R7" s="11">
         <v>6.9</v>
       </c>
       <c r="S7" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="T7" s="11">
         <v>179</v>
       </c>
       <c r="U7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="W7" t="s">
         <v>57</v>
@@ -2801,35 +2824,35 @@
         <v>241.2</v>
       </c>
       <c r="Y7" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="Z7" s="11">
         <v>120</v>
       </c>
       <c r="AA7" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="AB7" s="11">
         <v>224</v>
       </c>
       <c r="AC7" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="AD7" s="11">
         <v>13.5</v>
       </c>
       <c r="AE7" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="AF7" s="11">
         <v>15</v>
       </c>
       <c r="AG7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AH7" s="11"/>
       <c r="AI7" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="AJ7" s="11">
         <v>40</v>
@@ -2848,13 +2871,13 @@
         <v>9</v>
       </c>
       <c r="G8" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="H8" s="12">
         <v>56</v>
       </c>
       <c r="I8" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="J8" s="11">
         <v>120</v>
@@ -2866,10 +2889,10 @@
         <v>120</v>
       </c>
       <c r="M8" t="s">
-        <v>413</v>
+        <v>130</v>
       </c>
       <c r="N8" s="12">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="O8" t="s">
         <v>82</v>
@@ -2878,19 +2901,19 @@
         <v>240</v>
       </c>
       <c r="Q8" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="R8" s="11">
         <v>6.7</v>
       </c>
       <c r="S8" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="T8" s="11">
         <v>200</v>
       </c>
       <c r="U8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="W8" t="s">
         <v>58</v>
@@ -2899,13 +2922,13 @@
         <v>240</v>
       </c>
       <c r="Y8" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="Z8" s="11" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="AA8" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="AB8" s="11">
         <v>256</v>
@@ -2917,13 +2940,13 @@
         <v>20.5</v>
       </c>
       <c r="AE8" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="AF8" s="11">
         <v>16.5</v>
       </c>
       <c r="AG8" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AH8" s="11"/>
       <c r="AI8" t="s">
@@ -2946,13 +2969,13 @@
         <v>10</v>
       </c>
       <c r="G9" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="H9" s="12">
         <v>18</v>
       </c>
       <c r="I9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="J9" s="11">
         <v>225</v>
@@ -2964,10 +2987,10 @@
         <v>137</v>
       </c>
       <c r="M9" t="s">
-        <v>134</v>
+        <v>411</v>
       </c>
       <c r="N9" s="12">
-        <v>103</v>
+        <v>156</v>
       </c>
       <c r="O9" t="s">
         <v>81</v>
@@ -2976,40 +2999,40 @@
         <v>176</v>
       </c>
       <c r="Q9" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="R9" s="11">
         <v>5.8</v>
       </c>
       <c r="S9" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="T9" s="11">
         <v>164</v>
       </c>
       <c r="U9" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="W9" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="X9" s="11">
         <v>244</v>
       </c>
       <c r="Y9" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="Z9" s="11">
         <v>80</v>
       </c>
       <c r="AA9" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="AB9" s="11">
         <v>256</v>
       </c>
       <c r="AC9" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="AD9" s="11">
         <v>13.625</v>
@@ -3021,7 +3044,7 @@
         <v>18</v>
       </c>
       <c r="AG9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="AH9" s="11"/>
       <c r="AI9" t="s">
@@ -3033,11 +3056,11 @@
     </row>
     <row r="10" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B10" s="4" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C10" s="5"/>
       <c r="E10" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="F10" s="12">
         <v>7.85</v>
@@ -3049,22 +3072,22 @@
         <v>240</v>
       </c>
       <c r="I10" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="J10" s="11">
         <v>228</v>
       </c>
       <c r="K10" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="L10" s="12">
         <v>92</v>
       </c>
       <c r="M10" t="s">
-        <v>486</v>
+        <v>134</v>
       </c>
       <c r="N10" s="12">
-        <v>80</v>
+        <v>103</v>
       </c>
       <c r="O10" t="s">
         <v>71</v>
@@ -3073,7 +3096,7 @@
         <v>240</v>
       </c>
       <c r="Q10" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="R10" s="11">
         <v>12.6</v>
@@ -3085,7 +3108,7 @@
         <v>155</v>
       </c>
       <c r="U10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="W10" t="s">
         <v>59</v>
@@ -3094,31 +3117,31 @@
         <v>243</v>
       </c>
       <c r="Y10" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="Z10" s="11">
         <v>155</v>
       </c>
       <c r="AA10" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="AB10" s="11">
         <v>137</v>
       </c>
       <c r="AC10" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="AD10" s="11">
         <v>13.625</v>
       </c>
       <c r="AE10" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="AF10" s="11">
         <v>32</v>
       </c>
       <c r="AG10" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="AH10" s="11"/>
       <c r="AI10" t="s">
@@ -3137,20 +3160,20 @@
         <v>10</v>
       </c>
       <c r="E11" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="F11" s="12">
         <f>48/16</f>
         <v>3</v>
       </c>
       <c r="G11" t="s">
-        <v>55</v>
-      </c>
-      <c r="H11" s="12">
-        <v>306</v>
+        <v>488</v>
+      </c>
+      <c r="H11" t="s">
+        <v>398</v>
       </c>
       <c r="I11" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="J11" s="11">
         <v>114</v>
@@ -3162,10 +3185,10 @@
         <v>144</v>
       </c>
       <c r="M11" t="s">
-        <v>411</v>
+        <v>528</v>
       </c>
       <c r="N11" s="12">
-        <v>147</v>
+        <v>90</v>
       </c>
       <c r="O11" t="s">
         <v>76</v>
@@ -3174,28 +3197,28 @@
         <v>243</v>
       </c>
       <c r="Q11" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="R11" s="11">
         <v>6.5</v>
       </c>
       <c r="S11" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="T11" s="11">
         <v>150</v>
       </c>
       <c r="U11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="W11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="X11" s="11">
         <v>244</v>
       </c>
       <c r="Y11" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="Z11" s="11">
         <v>240</v>
@@ -3208,19 +3231,19 @@
         <v>192</v>
       </c>
       <c r="AC11" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="AD11" s="11">
         <v>13.625</v>
       </c>
       <c r="AE11" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="AF11" s="11">
         <v>14.2</v>
       </c>
       <c r="AG11" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AH11" s="11"/>
       <c r="AI11" t="s">
@@ -3236,35 +3259,35 @@
       </c>
       <c r="C12" s="5"/>
       <c r="E12" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="F12" s="12">
         <f>128/16</f>
         <v>8</v>
       </c>
       <c r="G12" t="s">
-        <v>32</v>
-      </c>
-      <c r="H12" s="12" t="s">
-        <v>404</v>
+        <v>55</v>
+      </c>
+      <c r="H12" s="12">
+        <v>306</v>
       </c>
       <c r="I12" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="J12" s="11">
         <v>112</v>
       </c>
       <c r="K12" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="L12" s="12">
         <v>114</v>
       </c>
       <c r="M12" t="s">
-        <v>135</v>
+        <v>529</v>
       </c>
       <c r="N12" s="12">
-        <v>227</v>
+        <v>90</v>
       </c>
       <c r="O12" t="s">
         <v>79</v>
@@ -3273,19 +3296,19 @@
         <v>122</v>
       </c>
       <c r="Q12" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="R12" s="11">
         <v>1.9</v>
       </c>
       <c r="S12" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="T12" s="11">
         <v>150</v>
       </c>
       <c r="U12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="X12" s="11"/>
       <c r="Y12" t="s">
@@ -3295,25 +3318,25 @@
         <v>80</v>
       </c>
       <c r="AA12" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="AB12" s="11">
         <v>93</v>
       </c>
       <c r="AC12" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="AD12" s="11">
         <v>13.625</v>
       </c>
       <c r="AE12" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="AF12" s="11">
         <v>16</v>
       </c>
       <c r="AG12" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AH12" s="11"/>
       <c r="AI12" t="s">
@@ -3329,20 +3352,20 @@
       </c>
       <c r="C13" s="5"/>
       <c r="E13" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="F13" s="12">
         <f>48/16</f>
         <v>3</v>
       </c>
       <c r="G13" t="s">
-        <v>492</v>
-      </c>
-      <c r="H13" t="s">
-        <v>400</v>
+        <v>32</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>402</v>
       </c>
       <c r="I13" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="J13" s="11">
         <v>113</v>
@@ -3354,10 +3377,10 @@
         <v>148</v>
       </c>
       <c r="M13" t="s">
-        <v>140</v>
+        <v>482</v>
       </c>
       <c r="N13" s="12">
-        <v>145</v>
+        <v>75</v>
       </c>
       <c r="O13" t="s">
         <v>77</v>
@@ -3366,23 +3389,23 @@
         <v>156</v>
       </c>
       <c r="Q13" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="R13" s="11">
         <v>5.4</v>
       </c>
       <c r="S13" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="T13" s="11">
         <v>200</v>
       </c>
       <c r="U13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="X13" s="11"/>
       <c r="Y13" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="Z13" s="11">
         <v>257.60000000000002</v>
@@ -3394,19 +3417,19 @@
         <v>168</v>
       </c>
       <c r="AC13" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="AD13" s="11">
         <v>13.625</v>
       </c>
       <c r="AE13" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="AF13" s="11">
         <v>15</v>
       </c>
       <c r="AG13" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="AH13" s="11"/>
       <c r="AI13" t="s">
@@ -3422,28 +3445,28 @@
       </c>
       <c r="C14" s="5"/>
       <c r="E14" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="F14" s="12">
         <v>7.5</v>
       </c>
       <c r="I14" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="J14" s="11">
         <v>216.56299999999999</v>
       </c>
       <c r="K14" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="L14" s="12">
         <v>122</v>
       </c>
       <c r="M14" t="s">
-        <v>419</v>
+        <v>409</v>
       </c>
       <c r="N14" s="12">
-        <v>230</v>
+        <v>147</v>
       </c>
       <c r="O14" t="s">
         <v>78</v>
@@ -3452,29 +3475,29 @@
         <v>160</v>
       </c>
       <c r="Q14" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="R14" s="11">
         <v>8.1</v>
       </c>
       <c r="S14" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="T14" s="11">
         <v>164</v>
       </c>
       <c r="U14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="X14" s="11"/>
       <c r="Y14" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="Z14" s="11">
         <v>120</v>
       </c>
       <c r="AA14" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="AB14" s="11">
         <v>135</v>
@@ -3486,13 +3509,13 @@
         <v>21.117999999999999</v>
       </c>
       <c r="AE14" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="AF14" s="11">
         <v>17</v>
       </c>
       <c r="AG14" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AH14" s="11"/>
       <c r="AI14" t="s">
@@ -3508,28 +3531,28 @@
       </c>
       <c r="C15" s="5"/>
       <c r="E15" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="F15" s="12">
         <v>12</v>
       </c>
       <c r="I15" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="J15" s="11">
         <v>112</v>
       </c>
       <c r="K15" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="L15" s="12">
         <v>114</v>
       </c>
       <c r="M15" t="s">
-        <v>273</v>
+        <v>530</v>
       </c>
       <c r="N15" s="12">
-        <v>92</v>
+        <v>227</v>
       </c>
       <c r="O15" t="s">
         <v>84</v>
@@ -3538,47 +3561,47 @@
         <v>177</v>
       </c>
       <c r="Q15" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="R15" s="11">
         <v>6.9</v>
       </c>
       <c r="S15" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="T15" s="11">
         <v>160</v>
       </c>
       <c r="U15" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="X15" s="11"/>
       <c r="Y15" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="Z15" s="11">
         <v>166</v>
       </c>
       <c r="AA15" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="AB15" s="11">
         <v>115</v>
       </c>
       <c r="AC15" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="AD15" s="11">
         <v>14</v>
       </c>
       <c r="AE15" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="AF15" s="11">
         <v>15</v>
       </c>
       <c r="AG15" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AH15" s="11"/>
       <c r="AI15" t="s">
@@ -3594,28 +3617,28 @@
       </c>
       <c r="C16" s="7"/>
       <c r="E16" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="F16" s="12">
         <v>18.25</v>
       </c>
       <c r="I16" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="J16" s="11">
         <v>238.4</v>
       </c>
       <c r="K16" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L16" s="12">
         <v>119</v>
       </c>
       <c r="M16" t="s">
-        <v>420</v>
+        <v>139</v>
       </c>
       <c r="N16" s="12">
-        <v>165</v>
+        <v>145</v>
       </c>
       <c r="O16" t="s">
         <v>68</v>
@@ -3624,22 +3647,22 @@
         <v>103</v>
       </c>
       <c r="Q16" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="R16" s="11">
         <v>7.8</v>
       </c>
       <c r="S16" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="T16" s="11">
         <v>184</v>
       </c>
       <c r="U16" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="Y16" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="Z16" s="11">
         <v>250</v>
@@ -3657,13 +3680,13 @@
         <v>20.7</v>
       </c>
       <c r="AE16" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="AF16" s="11">
         <v>15</v>
       </c>
       <c r="AG16" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="AH16" s="11"/>
       <c r="AI16" t="s">
@@ -3675,13 +3698,13 @@
     </row>
     <row r="17" spans="2:36" x14ac:dyDescent="0.2">
       <c r="E17" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="I17" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J17" s="11">
         <v>248</v>
@@ -3693,10 +3716,10 @@
         <v>104</v>
       </c>
       <c r="M17" t="s">
-        <v>412</v>
+        <v>416</v>
       </c>
       <c r="N17" s="12">
-        <v>170</v>
+        <v>230</v>
       </c>
       <c r="O17" t="s">
         <v>80</v>
@@ -3705,29 +3728,29 @@
         <v>85</v>
       </c>
       <c r="Q17" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="R17" s="11">
         <v>6.5</v>
       </c>
       <c r="S17" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="T17" s="11">
         <v>177</v>
       </c>
       <c r="U17" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X17" s="11"/>
       <c r="Y17" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="Z17" s="11">
         <v>80</v>
       </c>
       <c r="AA17" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="AB17" s="11">
         <v>32</v>
@@ -3739,17 +3762,17 @@
         <v>19.667999999999999</v>
       </c>
       <c r="AE17" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="AF17" s="11">
         <v>13.8</v>
       </c>
       <c r="AG17" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="AH17" s="11"/>
       <c r="AI17" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="AJ17" s="11">
         <v>87</v>
@@ -3757,13 +3780,13 @@
     </row>
     <row r="18" spans="2:36" x14ac:dyDescent="0.2">
       <c r="E18" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="I18" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="J18" s="11">
         <v>134</v>
@@ -3775,10 +3798,10 @@
         <v>105</v>
       </c>
       <c r="M18" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="N18" s="12">
-        <v>177</v>
+        <v>92</v>
       </c>
       <c r="O18" t="s">
         <v>62</v>
@@ -3787,47 +3810,47 @@
         <v>81</v>
       </c>
       <c r="Q18" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="R18" s="11">
         <v>5</v>
       </c>
       <c r="S18" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="T18" s="11">
         <v>195</v>
       </c>
       <c r="U18" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="X18" s="11"/>
       <c r="Y18" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="Z18" s="11" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="AA18" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="AB18" s="11">
         <v>134</v>
       </c>
       <c r="AC18" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="AD18" s="11">
         <v>14</v>
       </c>
       <c r="AE18" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="AF18" s="11">
         <v>15</v>
       </c>
       <c r="AG18" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AH18" s="11"/>
       <c r="AI18" t="s">
@@ -3839,31 +3862,31 @@
     </row>
     <row r="19" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="E19" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="I19" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J19" s="11">
         <v>240</v>
       </c>
       <c r="K19" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="L19" s="12">
         <v>116</v>
       </c>
       <c r="M19" t="s">
-        <v>414</v>
+        <v>417</v>
       </c>
       <c r="N19" s="12">
-        <v>212</v>
+        <v>165</v>
       </c>
       <c r="O19" t="s">
         <v>70</v>
@@ -3872,24 +3895,24 @@
         <v>163</v>
       </c>
       <c r="Q19" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="R19" s="11">
         <v>6</v>
       </c>
       <c r="S19" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="T19" s="11">
         <v>198</v>
       </c>
       <c r="U19" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="X19" s="11"/>
       <c r="Z19" s="11"/>
       <c r="AA19" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="AB19" s="11">
         <v>120</v>
@@ -3902,13 +3925,13 @@
         <v>21.0625</v>
       </c>
       <c r="AE19" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="AF19" s="11">
         <v>15</v>
       </c>
       <c r="AG19" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="AH19" s="11"/>
       <c r="AI19" t="s">
@@ -3920,16 +3943,16 @@
     </row>
     <row r="20" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="E20" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="I20" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="J20" s="11">
         <v>113</v>
@@ -3941,10 +3964,10 @@
         <v>170</v>
       </c>
       <c r="M20" t="s">
-        <v>274</v>
+        <v>410</v>
       </c>
       <c r="N20" s="12">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="O20" t="s">
         <v>64</v>
@@ -3953,23 +3976,23 @@
         <v>170</v>
       </c>
       <c r="Q20" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="R20" s="11">
         <v>0.375</v>
       </c>
       <c r="S20" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="T20" s="11">
         <v>178</v>
       </c>
       <c r="U20" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="X20" s="11"/>
       <c r="AA20" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="AB20" s="11">
         <v>146</v>
@@ -3981,13 +4004,13 @@
         <v>13.5</v>
       </c>
       <c r="AE20" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="AF20" s="11">
         <v>18</v>
       </c>
       <c r="AG20" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AH20" s="11"/>
       <c r="AI20" t="s">
@@ -4006,28 +4029,28 @@
         <v>20</v>
       </c>
       <c r="E21" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="I21" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="J21" s="11">
         <v>113</v>
       </c>
       <c r="K21" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="L21" s="12">
-        <v>227</v>
+        <v>106</v>
       </c>
       <c r="M21" t="s">
-        <v>421</v>
+        <v>270</v>
       </c>
       <c r="N21" s="12">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="O21" t="s">
         <v>83</v>
@@ -4036,42 +4059,42 @@
         <v>140</v>
       </c>
       <c r="Q21" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="R21" s="11">
         <v>6.3</v>
       </c>
       <c r="S21" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="T21" s="11">
         <v>188</v>
       </c>
       <c r="U21" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="X21" s="11"/>
       <c r="AA21" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="AB21" s="11">
         <v>180</v>
       </c>
       <c r="AC21" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="AD21" s="11">
         <v>13.5</v>
       </c>
       <c r="AE21" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="AF21" s="11">
         <f>244/16</f>
         <v>15.25</v>
       </c>
       <c r="AG21" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AH21" s="11"/>
       <c r="AI21" t="s">
@@ -4086,28 +4109,28 @@
         <v>65</v>
       </c>
       <c r="E22" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="I22" t="s">
-        <v>219</v>
+        <v>523</v>
       </c>
       <c r="J22" s="11">
         <v>240</v>
       </c>
       <c r="K22" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="L22" s="12">
         <v>137</v>
       </c>
       <c r="M22" t="s">
-        <v>431</v>
+        <v>412</v>
       </c>
       <c r="N22" s="12">
-        <v>165</v>
+        <v>212</v>
       </c>
       <c r="O22" t="s">
         <v>86</v>
@@ -4116,42 +4139,42 @@
         <v>190</v>
       </c>
       <c r="Q22" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="R22" s="11">
         <v>6.6</v>
       </c>
       <c r="S22" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="T22" s="11">
         <v>207</v>
       </c>
       <c r="U22" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="X22" s="11"/>
       <c r="AA22" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="AB22" s="11">
         <v>144</v>
       </c>
       <c r="AC22" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="AD22" s="11">
         <f>237/16</f>
         <v>14.8125</v>
       </c>
       <c r="AE22" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="AF22" s="11">
         <v>15</v>
       </c>
       <c r="AG22" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="AH22" s="11"/>
       <c r="AI22" t="s">
@@ -4169,22 +4192,22 @@
         <v>6.9</v>
       </c>
       <c r="I23" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="J23" s="11">
         <v>122</v>
       </c>
       <c r="K23" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="L23" s="12">
         <v>155</v>
       </c>
       <c r="M23" t="s">
-        <v>142</v>
+        <v>272</v>
       </c>
       <c r="N23" s="12">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="O23" t="s">
         <v>61</v>
@@ -4193,41 +4216,41 @@
         <v>185</v>
       </c>
       <c r="Q23" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="R23" s="11">
         <v>3.1</v>
       </c>
       <c r="S23" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="T23" s="11">
         <v>104</v>
       </c>
       <c r="U23" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="X23" s="11"/>
       <c r="AA23" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="AB23" s="11">
         <v>99</v>
       </c>
       <c r="AC23" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="AD23" s="11">
         <v>13.53</v>
       </c>
       <c r="AE23" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="AF23" s="11">
         <v>15</v>
       </c>
       <c r="AG23" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="AH23" s="11"/>
       <c r="AI23" t="s">
@@ -4245,22 +4268,22 @@
         <v>10</v>
       </c>
       <c r="I24" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="J24" s="11">
         <v>100</v>
       </c>
       <c r="K24" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="L24" s="12">
         <v>108</v>
       </c>
       <c r="M24" t="s">
-        <v>139</v>
+        <v>418</v>
       </c>
       <c r="N24" s="12">
-        <v>140</v>
+        <v>190</v>
       </c>
       <c r="O24" t="s">
         <v>85</v>
@@ -4275,39 +4298,39 @@
         <v>5.8</v>
       </c>
       <c r="S24" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="T24" s="11">
         <v>208</v>
       </c>
       <c r="U24" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="X24" s="11"/>
       <c r="AA24" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="AB24" s="11">
         <v>109</v>
       </c>
       <c r="AC24" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="AD24" s="11">
         <v>13.625</v>
       </c>
       <c r="AE24" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="AF24" s="11">
         <v>18</v>
       </c>
       <c r="AG24" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="AH24" s="11"/>
       <c r="AI24" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="AJ24" s="11">
         <v>55</v>
@@ -4315,7 +4338,7 @@
     </row>
     <row r="25" spans="2:36" x14ac:dyDescent="0.2">
       <c r="I25" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J25" s="11">
         <v>245.43799999999999</v>
@@ -4327,10 +4350,10 @@
         <v>125</v>
       </c>
       <c r="M25" t="s">
-        <v>422</v>
+        <v>428</v>
       </c>
       <c r="N25" s="12">
-        <v>143</v>
+        <v>165</v>
       </c>
       <c r="O25" t="s">
         <v>66</v>
@@ -4339,23 +4362,23 @@
         <v>169</v>
       </c>
       <c r="Q25" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="R25" s="11">
         <v>11.1</v>
       </c>
       <c r="S25" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="T25" s="11">
         <v>193</v>
       </c>
       <c r="U25" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="X25" s="11"/>
       <c r="AA25" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="AB25" s="11">
         <v>135</v>
@@ -4367,17 +4390,17 @@
         <v>13.625</v>
       </c>
       <c r="AE25" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="AF25" s="11">
         <v>15</v>
       </c>
       <c r="AG25" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AH25" s="11"/>
       <c r="AI25" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="AJ25" s="11">
         <v>35</v>
@@ -4385,7 +4408,7 @@
     </row>
     <row r="26" spans="2:36" x14ac:dyDescent="0.2">
       <c r="I26" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="J26" s="11">
         <v>118</v>
@@ -4397,10 +4420,10 @@
         <v>167</v>
       </c>
       <c r="M26" t="s">
-        <v>423</v>
+        <v>141</v>
       </c>
       <c r="N26" s="12">
-        <v>217</v>
+        <v>196</v>
       </c>
       <c r="O26" t="s">
         <v>73</v>
@@ -4409,23 +4432,23 @@
         <v>174</v>
       </c>
       <c r="Q26" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="R26" s="11">
         <v>9.6999999999999993</v>
       </c>
       <c r="S26" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="T26" s="11">
         <v>171</v>
       </c>
       <c r="U26" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="X26" s="11"/>
       <c r="AA26" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="AB26" s="11">
         <v>123</v>
@@ -4443,11 +4466,11 @@
         <v>16</v>
       </c>
       <c r="AG26" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="AH26" s="11"/>
       <c r="AI26" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="AJ26" s="11">
         <v>57</v>
@@ -4455,7 +4478,7 @@
     </row>
     <row r="27" spans="2:36" x14ac:dyDescent="0.2">
       <c r="I27" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="J27" s="11">
         <v>122</v>
@@ -4467,7 +4490,7 @@
         <v>121</v>
       </c>
       <c r="M27" t="s">
-        <v>424</v>
+        <v>138</v>
       </c>
       <c r="N27" s="12">
         <v>140</v>
@@ -4479,46 +4502,47 @@
         <v>193</v>
       </c>
       <c r="Q27" t="s">
-        <v>441</v>
+        <v>525</v>
       </c>
       <c r="R27" s="11">
-        <v>5.2</v>
+        <f>149/16</f>
+        <v>9.3125</v>
       </c>
       <c r="S27" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="T27" s="11">
         <v>150</v>
       </c>
       <c r="U27" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="X27" s="11"/>
       <c r="AA27" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="AB27" s="11">
         <v>133</v>
       </c>
       <c r="AC27" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="AD27" s="11">
         <v>14</v>
       </c>
       <c r="AE27" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="AF27" s="11">
         <f>6.5*3</f>
         <v>19.5</v>
       </c>
       <c r="AG27" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="AH27" s="11"/>
       <c r="AI27" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="AJ27" s="11">
         <v>54</v>
@@ -4526,7 +4550,7 @@
     </row>
     <row r="28" spans="2:36" x14ac:dyDescent="0.2">
       <c r="I28" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J28" s="11">
         <v>227</v>
@@ -4538,10 +4562,10 @@
         <v>120</v>
       </c>
       <c r="M28" t="s">
-        <v>141</v>
+        <v>419</v>
       </c>
       <c r="N28" s="12">
-        <v>236</v>
+        <v>143</v>
       </c>
       <c r="O28" t="s">
         <v>65</v>
@@ -4550,19 +4574,19 @@
         <v>192</v>
       </c>
       <c r="Q28" t="s">
-        <v>442</v>
+        <v>524</v>
       </c>
       <c r="R28" s="11">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="S28" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="T28" s="11">
         <v>256</v>
       </c>
       <c r="U28" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="X28" s="11"/>
       <c r="AA28" t="s">
@@ -4578,17 +4602,17 @@
         <v>13.5</v>
       </c>
       <c r="AE28" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="AF28" s="11">
         <v>10</v>
       </c>
       <c r="AG28" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AH28" s="11"/>
       <c r="AI28" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="AJ28" s="11">
         <v>87</v>
@@ -4597,7 +4621,7 @@
     <row r="29" spans="2:36" x14ac:dyDescent="0.2">
       <c r="F29" s="11"/>
       <c r="I29" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="J29" s="11">
         <v>122</v>
@@ -4609,35 +4633,35 @@
         <v>120</v>
       </c>
       <c r="M29" t="s">
-        <v>426</v>
+        <v>420</v>
       </c>
       <c r="N29" s="12">
-        <v>154</v>
+        <v>217</v>
       </c>
       <c r="O29" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="P29" s="12">
         <v>64</v>
       </c>
       <c r="Q29" t="s">
-        <v>258</v>
+        <v>438</v>
       </c>
       <c r="R29" s="11">
-        <v>6.9</v>
+        <v>5.2</v>
       </c>
       <c r="S29" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="T29" s="11">
         <v>197</v>
       </c>
       <c r="U29" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="X29" s="11"/>
       <c r="AA29" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="AB29" s="11">
         <v>122</v>
@@ -4649,17 +4673,17 @@
         <v>13.625</v>
       </c>
       <c r="AE29" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="AF29" s="11">
         <v>18</v>
       </c>
       <c r="AG29" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="AH29" s="11"/>
       <c r="AI29" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="AJ29" s="11">
         <v>66</v>
@@ -4671,7 +4695,7 @@
       </c>
       <c r="F30" s="10"/>
       <c r="I30" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="J30" s="11">
         <v>245</v>
@@ -4680,46 +4704,46 @@
         <v>30</v>
       </c>
       <c r="L30" s="12">
-        <v>120</v>
+        <v>135</v>
       </c>
       <c r="M30" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="N30" s="12">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="O30" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="P30" s="12">
         <f>28*4</f>
         <v>112</v>
       </c>
       <c r="Q30" t="s">
-        <v>265</v>
+        <v>439</v>
       </c>
       <c r="R30" s="11">
-        <v>2.8</v>
+        <v>6</v>
       </c>
       <c r="S30" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="T30" s="11">
         <v>105</v>
       </c>
       <c r="U30" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="X30" s="11"/>
       <c r="AA30" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="AB30" s="11">
         <f>28*4</f>
         <v>112</v>
       </c>
       <c r="AC30" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="AD30" s="11">
         <v>13.625</v>
@@ -4731,11 +4755,11 @@
         <v>16.5</v>
       </c>
       <c r="AG30" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AH30" s="11"/>
       <c r="AI30" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="AJ30" s="11">
         <v>86</v>
@@ -4743,27 +4767,27 @@
     </row>
     <row r="31" spans="2:36" x14ac:dyDescent="0.2">
       <c r="I31" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J31" s="11">
         <v>248</v>
       </c>
       <c r="M31" t="s">
-        <v>428</v>
+        <v>140</v>
       </c>
       <c r="N31" s="12">
-        <v>168</v>
+        <v>236</v>
       </c>
       <c r="P31" s="12"/>
       <c r="Q31" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="R31" s="11">
-        <v>6</v>
+        <v>6.9</v>
       </c>
       <c r="T31" s="11"/>
       <c r="U31" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="X31" s="11"/>
       <c r="AA31" t="s">
@@ -4774,17 +4798,17 @@
       </c>
       <c r="AD31" s="11"/>
       <c r="AE31" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="AF31" s="11">
         <v>15</v>
       </c>
       <c r="AG31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="AH31" s="11"/>
       <c r="AI31" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="AJ31" s="11">
         <v>89</v>
@@ -4792,32 +4816,32 @@
     </row>
     <row r="32" spans="2:36" x14ac:dyDescent="0.2">
       <c r="I32" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="J32" s="11">
         <f>28*8</f>
         <v>224</v>
       </c>
       <c r="M32" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="N32" s="12">
-        <v>173.25</v>
+        <v>154</v>
       </c>
       <c r="P32" s="12"/>
       <c r="Q32" t="s">
-        <v>256</v>
+        <v>263</v>
       </c>
       <c r="R32" s="11">
-        <v>6</v>
+        <v>2.8</v>
       </c>
       <c r="T32" s="11"/>
       <c r="U32" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="X32" s="11"/>
       <c r="AA32" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="AB32" s="11">
         <v>46</v>
@@ -4830,11 +4854,11 @@
         <v>14.9</v>
       </c>
       <c r="AG32" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="AH32" s="11"/>
       <c r="AI32" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="AJ32" s="11">
         <v>96</v>
@@ -4842,13 +4866,13 @@
     </row>
     <row r="33" spans="9:36" x14ac:dyDescent="0.2">
       <c r="I33" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="J33" s="11">
         <v>113</v>
       </c>
       <c r="M33" t="s">
-        <v>429</v>
+        <v>422</v>
       </c>
       <c r="N33" s="12">
         <v>150</v>
@@ -4857,27 +4881,27 @@
         <v>253</v>
       </c>
       <c r="R33" s="11">
-        <v>5.2</v>
+        <v>6</v>
       </c>
       <c r="T33" s="11"/>
       <c r="U33" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="AA33" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="AB33" s="11">
         <v>120</v>
       </c>
       <c r="AD33" s="11"/>
       <c r="AE33" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="AF33" s="11">
         <v>14.938000000000001</v>
       </c>
       <c r="AG33" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="AH33" s="11"/>
       <c r="AI33" t="s">
@@ -4889,36 +4913,36 @@
     </row>
     <row r="34" spans="9:36" x14ac:dyDescent="0.2">
       <c r="I34" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="J34" s="11">
         <v>240</v>
       </c>
       <c r="M34" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="N34" s="12">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="Q34" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="R34" s="11">
-        <v>1.7</v>
+        <v>6</v>
       </c>
       <c r="T34" s="11"/>
       <c r="U34" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AA34" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="AB34" s="11">
         <v>120</v>
       </c>
       <c r="AD34" s="11"/>
       <c r="AE34" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="AF34" s="11">
         <v>15.938000000000001</v>
@@ -4933,33 +4957,33 @@
     </row>
     <row r="35" spans="9:36" x14ac:dyDescent="0.2">
       <c r="I35" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J35" s="11">
         <v>245</v>
       </c>
       <c r="M35" t="s">
-        <v>137</v>
+        <v>424</v>
       </c>
       <c r="N35" s="12">
-        <v>134</v>
+        <v>173.25</v>
       </c>
       <c r="Q35" t="s">
-        <v>271</v>
+        <v>251</v>
       </c>
       <c r="R35" s="11">
-        <v>6</v>
+        <v>5.2</v>
       </c>
       <c r="T35" s="11"/>
       <c r="AA35" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="AB35" s="11">
         <v>62</v>
       </c>
       <c r="AD35" s="11"/>
       <c r="AE35" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="AF35" s="11">
         <v>14.938000000000001</v>
@@ -4974,21 +4998,21 @@
     </row>
     <row r="36" spans="9:36" x14ac:dyDescent="0.2">
       <c r="M36" t="s">
-        <v>136</v>
+        <v>426</v>
       </c>
       <c r="N36" s="12">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="Q36" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="R36" s="11">
-        <v>6.2</v>
+        <v>1.7</v>
       </c>
       <c r="T36" s="11"/>
       <c r="AD36" s="11"/>
       <c r="AE36" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="AF36" s="11">
         <v>14.938000000000001</v>
@@ -5003,16 +5027,16 @@
     </row>
     <row r="37" spans="9:36" x14ac:dyDescent="0.2">
       <c r="M37" t="s">
-        <v>129</v>
+        <v>427</v>
       </c>
       <c r="N37" s="12">
-        <v>152</v>
+        <v>174</v>
       </c>
       <c r="Q37" t="s">
-        <v>243</v>
+        <v>269</v>
       </c>
       <c r="R37" s="11">
-        <v>6.8</v>
+        <v>6</v>
       </c>
       <c r="T37" s="11"/>
       <c r="AD37" s="11"/>
@@ -5031,21 +5055,21 @@
     </row>
     <row r="38" spans="9:36" x14ac:dyDescent="0.2">
       <c r="M38" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="N38" s="12">
-        <v>152</v>
+        <v>134</v>
       </c>
       <c r="Q38" t="s">
-        <v>518</v>
+        <v>249</v>
       </c>
       <c r="R38" s="11">
-        <v>6.9</v>
+        <v>6.2</v>
       </c>
       <c r="T38" s="11"/>
       <c r="AD38" s="11"/>
       <c r="AE38" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="AF38" s="11">
         <v>18</v>
@@ -5058,12 +5082,17 @@
       </c>
     </row>
     <row r="39" spans="9:36" x14ac:dyDescent="0.2">
-      <c r="N39" s="12"/>
+      <c r="M39" t="s">
+        <v>135</v>
+      </c>
+      <c r="N39" s="12">
+        <v>120</v>
+      </c>
       <c r="Q39" t="s">
-        <v>443</v>
+        <v>241</v>
       </c>
       <c r="R39" s="11">
-        <v>5.4</v>
+        <v>6.8</v>
       </c>
       <c r="T39" s="11"/>
       <c r="AD39" s="11"/>
@@ -5076,34 +5105,46 @@
       </c>
     </row>
     <row r="40" spans="9:36" x14ac:dyDescent="0.2">
+      <c r="M40" t="s">
+        <v>129</v>
+      </c>
+      <c r="N40" s="12">
+        <v>152</v>
+      </c>
       <c r="Q40" t="s">
-        <v>444</v>
+        <v>514</v>
       </c>
       <c r="R40" s="11">
-        <v>3</v>
+        <v>6.9</v>
       </c>
       <c r="T40" s="11"/>
       <c r="AD40" s="11"/>
       <c r="AF40" s="11"/>
       <c r="AI40" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="AJ40" s="11">
         <v>140</v>
       </c>
     </row>
     <row r="41" spans="9:36" x14ac:dyDescent="0.2">
+      <c r="M41" t="s">
+        <v>131</v>
+      </c>
+      <c r="N41" s="12">
+        <v>152</v>
+      </c>
       <c r="Q41" t="s">
-        <v>238</v>
+        <v>440</v>
       </c>
       <c r="R41" s="11">
-        <v>6.85</v>
+        <v>5.4</v>
       </c>
       <c r="T41" s="11"/>
       <c r="AD41" s="11"/>
       <c r="AF41" s="11"/>
       <c r="AI41" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="AJ41" s="11">
         <v>140</v>
@@ -5111,16 +5152,16 @@
     </row>
     <row r="42" spans="9:36" x14ac:dyDescent="0.2">
       <c r="Q42" t="s">
-        <v>447</v>
+        <v>441</v>
       </c>
       <c r="R42" s="11">
-        <v>6.9</v>
+        <v>3</v>
       </c>
       <c r="T42" s="11"/>
       <c r="AD42" s="11"/>
       <c r="AF42" s="11"/>
       <c r="AI42" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="AJ42" s="11">
         <v>113</v>
@@ -5128,16 +5169,16 @@
     </row>
     <row r="43" spans="9:36" x14ac:dyDescent="0.2">
       <c r="Q43" t="s">
-        <v>448</v>
+        <v>236</v>
       </c>
       <c r="R43" s="11">
-        <v>5.3</v>
+        <v>6.85</v>
       </c>
       <c r="T43" s="11"/>
       <c r="AD43" s="11"/>
       <c r="AF43" s="11"/>
       <c r="AI43" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="AJ43" s="11">
         <v>101</v>
@@ -5145,16 +5186,16 @@
     </row>
     <row r="44" spans="9:36" x14ac:dyDescent="0.2">
       <c r="Q44" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
       <c r="R44" s="11">
-        <v>7.1</v>
+        <v>6.9</v>
       </c>
       <c r="T44" s="11"/>
       <c r="AD44" s="11"/>
       <c r="AF44" s="11"/>
       <c r="AI44" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="AJ44" s="11">
         <v>145</v>
@@ -5162,14 +5203,14 @@
     </row>
     <row r="45" spans="9:36" x14ac:dyDescent="0.2">
       <c r="Q45" t="s">
-        <v>451</v>
+        <v>445</v>
       </c>
       <c r="R45" s="11">
-        <v>8.6999999999999993</v>
+        <v>5.3</v>
       </c>
       <c r="AF45" s="11"/>
       <c r="AI45" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="AJ45" s="11">
         <v>154</v>
@@ -5177,10 +5218,10 @@
     </row>
     <row r="46" spans="9:36" x14ac:dyDescent="0.2">
       <c r="Q46" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="R46" s="11">
-        <v>10</v>
+        <v>7.1</v>
       </c>
       <c r="AF46" s="11"/>
       <c r="AI46" t="s">
@@ -5192,10 +5233,10 @@
     </row>
     <row r="47" spans="9:36" x14ac:dyDescent="0.2">
       <c r="Q47" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="R47" s="11">
-        <v>3.3</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="AI47" t="s">
         <v>90</v>
@@ -5206,13 +5247,13 @@
     </row>
     <row r="48" spans="9:36" x14ac:dyDescent="0.2">
       <c r="Q48" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="R48" s="11">
-        <v>1.9</v>
+        <v>10</v>
       </c>
       <c r="AI48" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="AJ48" s="11">
         <v>152</v>
@@ -5220,10 +5261,10 @@
     </row>
     <row r="49" spans="17:36" x14ac:dyDescent="0.2">
       <c r="Q49" t="s">
-        <v>246</v>
+        <v>443</v>
       </c>
       <c r="R49" s="11">
-        <v>2.1</v>
+        <v>3.3</v>
       </c>
       <c r="AI49" t="s">
         <v>115</v>
@@ -5234,10 +5275,10 @@
     </row>
     <row r="50" spans="17:36" x14ac:dyDescent="0.2">
       <c r="Q50" t="s">
-        <v>249</v>
+        <v>442</v>
       </c>
       <c r="R50" s="11">
-        <v>2.1</v>
+        <v>1.9</v>
       </c>
       <c r="AI50" t="s">
         <v>95</v>
@@ -5248,13 +5289,13 @@
     </row>
     <row r="51" spans="17:36" x14ac:dyDescent="0.2">
       <c r="Q51" t="s">
-        <v>259</v>
+        <v>244</v>
       </c>
       <c r="R51" s="11">
-        <v>8.1</v>
+        <v>2.1</v>
       </c>
       <c r="AI51" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="AJ51" s="11">
         <v>20</v>
@@ -5262,43 +5303,43 @@
     </row>
     <row r="52" spans="17:36" x14ac:dyDescent="0.2">
       <c r="Q52" t="s">
-        <v>264</v>
+        <v>247</v>
       </c>
       <c r="R52" s="11">
-        <v>7.5</v>
+        <v>2.1</v>
       </c>
       <c r="AJ52" s="11"/>
     </row>
     <row r="53" spans="17:36" x14ac:dyDescent="0.2">
       <c r="Q53" t="s">
-        <v>452</v>
+        <v>257</v>
       </c>
       <c r="R53" s="11">
-        <v>1.8</v>
+        <v>8.1</v>
       </c>
       <c r="AJ53" s="11"/>
     </row>
     <row r="54" spans="17:36" x14ac:dyDescent="0.2">
       <c r="Q54" t="s">
-        <v>453</v>
+        <v>262</v>
       </c>
       <c r="R54" s="11">
-        <v>2.4</v>
+        <v>7.5</v>
       </c>
       <c r="AJ54" s="11"/>
     </row>
     <row r="55" spans="17:36" x14ac:dyDescent="0.2">
       <c r="Q55" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="R55" s="11">
-        <v>4.25</v>
+        <v>1.8</v>
       </c>
       <c r="AJ55" s="11"/>
     </row>
     <row r="56" spans="17:36" x14ac:dyDescent="0.2">
       <c r="Q56" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="R56" s="11">
         <v>2.4</v>
@@ -5307,42 +5348,62 @@
     </row>
     <row r="57" spans="17:36" x14ac:dyDescent="0.2">
       <c r="Q57" t="s">
-        <v>269</v>
+        <v>451</v>
       </c>
       <c r="R57" s="11">
-        <v>9.4</v>
+        <v>4.25</v>
       </c>
       <c r="AJ57" s="11"/>
     </row>
     <row r="58" spans="17:36" x14ac:dyDescent="0.2">
       <c r="Q58" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="R58" s="11">
-        <v>5</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="59" spans="17:36" x14ac:dyDescent="0.2">
       <c r="Q59" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="R59" s="11">
-        <v>6</v>
+        <v>9.4</v>
       </c>
     </row>
     <row r="60" spans="17:36" x14ac:dyDescent="0.2">
       <c r="Q60" t="s">
-        <v>262</v>
+        <v>453</v>
       </c>
       <c r="R60" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="61" spans="17:36" x14ac:dyDescent="0.2">
+      <c r="Q61" t="s">
+        <v>268</v>
+      </c>
+      <c r="R61" s="11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" spans="17:36" x14ac:dyDescent="0.2">
+      <c r="Q62" t="s">
+        <v>260</v>
+      </c>
+      <c r="R62" s="11">
         <v>4.2</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="Q2:R60">
-    <sortCondition ref="Q2:Q60"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="M2:N41">
+    <sortCondition ref="M2:M41"/>
   </sortState>
+  <hyperlinks>
+    <hyperlink ref="K1" r:id="rId1" xr:uid="{03BE3EB4-1121-B34D-96B6-1846C769CE18}"/>
+    <hyperlink ref="K2" r:id="rId2" xr:uid="{8618677F-CB78-E544-8E31-FE8A667EEEF5}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="64" fitToWidth="2" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup scale="41" fitToWidth="2" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update .xlsx and textFiles/*.txt files to include current added ingredients for continued backup
</commit_message>
<xml_diff>
--- a/Ingredients and Types.xlsx
+++ b/Ingredients and Types.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Matthew/Documents/Coding/PersonalProjects/recipeConverter/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2B39DAB-9D0B-8549-95F5-B9FE0305AE3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E2C3FC0-8DFE-1A40-85C3-2B7882AD0D90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1060" yWindow="1900" windowWidth="39780" windowHeight="23260" xr2:uid="{2D2F75AA-471C-5F46-928E-911BD0472A90}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="531">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="532">
   <si>
     <t>Baked Goods, Dry</t>
   </si>
@@ -1629,6 +1629,9 @@
   </si>
   <si>
     <t>Dragon Fruit</t>
+  </si>
+  <si>
+    <t>Water</t>
   </si>
 </sst>
 </file>
@@ -2119,7 +2122,7 @@
   <dimension ref="B1:AS62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="M40" sqref="M40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3450,6 +3453,12 @@
       <c r="F14" s="12">
         <v>7.5</v>
       </c>
+      <c r="G14" t="s">
+        <v>531</v>
+      </c>
+      <c r="H14" s="11">
+        <v>236.58799999999999</v>
+      </c>
       <c r="I14" t="s">
         <v>219</v>
       </c>

</xml_diff>

<commit_message>
update .xlsx and textFiles/*.txt files to include final first pass of added ingredients for continued backup
</commit_message>
<xml_diff>
--- a/Ingredients and Types.xlsx
+++ b/Ingredients and Types.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Matthew/Documents/Coding/PersonalProjects/recipeConverter/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A17C11A-38C8-9E45-9E04-0F3B2CE25136}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FBA2120-66E0-D94C-BD0F-70DD710A93F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1060" yWindow="1900" windowWidth="39780" windowHeight="23260" xr2:uid="{2D2F75AA-471C-5F46-928E-911BD0472A90}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="532">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="547">
   <si>
     <t>Baked Goods, Dry</t>
   </si>
@@ -1022,21 +1022,6 @@
     <t>Walnuts, Chopped</t>
   </si>
   <si>
-    <t>Butter, Almond</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Butter, Cashew </t>
-  </si>
-  <si>
-    <t>Butter, Hazelnut</t>
-  </si>
-  <si>
-    <t>Butter, Peanut</t>
-  </si>
-  <si>
-    <t>Butter, Sunflower</t>
-  </si>
-  <si>
     <t>Navy Beans</t>
   </si>
   <si>
@@ -1632,6 +1617,66 @@
   </si>
   <si>
     <t>17.01 g/tbsp</t>
+  </si>
+  <si>
+    <t>Almond Butter</t>
+  </si>
+  <si>
+    <t>Cashew Butter</t>
+  </si>
+  <si>
+    <t>Hazelnut Butter</t>
+  </si>
+  <si>
+    <t>Peanut Butter</t>
+  </si>
+  <si>
+    <t>Sunflower Butter</t>
+  </si>
+  <si>
+    <t>Chocolate Chips</t>
+  </si>
+  <si>
+    <t>Chocolate Chunks</t>
+  </si>
+  <si>
+    <t>Chocolate, Melted</t>
+  </si>
+  <si>
+    <t>170 g/cup</t>
+  </si>
+  <si>
+    <t>140g/cup</t>
+  </si>
+  <si>
+    <t>Choocolate, Grated</t>
+  </si>
+  <si>
+    <t>180g/cup</t>
+  </si>
+  <si>
+    <t>100g/cup</t>
+  </si>
+  <si>
+    <t>Chocolate, Fine Chop</t>
+  </si>
+  <si>
+    <t>Chocoalte, Rough Chop</t>
+  </si>
+  <si>
+    <t>120g/cup</t>
+  </si>
+  <si>
+    <t>Chocolate Syrup</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>?done</t>
   </si>
 </sst>
 </file>
@@ -1641,7 +1686,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1673,6 +1718,29 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow (Body)"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1761,7 +1829,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1780,6 +1848,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2118,10 +2192,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:AS62"/>
+  <dimension ref="A1:AS62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="Y28" sqref="Y28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2176,97 +2250,97 @@
         <v>0</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="I1" s="12" t="s">
         <v>6</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="K1" s="13" t="s">
         <v>229</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="N1" s="8" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="P1" s="8" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="R1" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="T1" s="8" t="s">
-        <v>375</v>
-      </c>
-      <c r="U1" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="U1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="V1" s="8" t="s">
-        <v>375</v>
+      <c r="V1" s="15" t="s">
+        <v>370</v>
       </c>
       <c r="W1" s="1" t="s">
         <v>228</v>
       </c>
       <c r="X1" s="8" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="Y1" s="1" t="s">
         <v>128</v>
       </c>
       <c r="Z1" s="8" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="AA1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="AB1" s="8" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="AC1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="AD1" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="AE1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="AF1" t="s">
-        <v>376</v>
-      </c>
-      <c r="AG1" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="AG1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="AH1" s="8" t="s">
-        <v>375</v>
+      <c r="AH1" s="15" t="s">
+        <v>370</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="AJ1" s="8" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="AK1" s="1"/>
       <c r="AQ1" s="1"/>
@@ -2288,10 +2362,10 @@
         <v>14</v>
       </c>
       <c r="H2" t="s">
+        <v>385</v>
+      </c>
+      <c r="I2" t="s">
         <v>390</v>
-      </c>
-      <c r="I2" t="s">
-        <v>395</v>
       </c>
       <c r="J2" s="10">
         <v>112</v>
@@ -2303,7 +2377,7 @@
         <v>130</v>
       </c>
       <c r="M2" t="s">
-        <v>514</v>
+        <v>509</v>
       </c>
       <c r="N2" s="11">
         <v>125</v>
@@ -2321,25 +2395,27 @@
         <v>6</v>
       </c>
       <c r="S2" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="T2" s="10">
         <v>197</v>
       </c>
-      <c r="U2" t="s">
+      <c r="U2" s="16" t="s">
         <v>143</v>
       </c>
+      <c r="V2" s="16"/>
       <c r="Y2" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="Z2" s="10" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="AA2" t="s">
-        <v>302</v>
+        <v>527</v>
       </c>
       <c r="AB2" s="10">
-        <v>138</v>
+        <f>16*16</f>
+        <v>256</v>
       </c>
       <c r="AC2" t="s">
         <v>12</v>
@@ -2353,10 +2429,10 @@
       <c r="AF2" s="10">
         <v>17</v>
       </c>
-      <c r="AG2" t="s">
-        <v>365</v>
-      </c>
-      <c r="AH2" s="10"/>
+      <c r="AG2" s="16" t="s">
+        <v>360</v>
+      </c>
+      <c r="AH2" s="17"/>
       <c r="AI2" t="s">
         <v>102</v>
       </c>
@@ -2377,7 +2453,7 @@
         <v>13.8</v>
       </c>
       <c r="G3" t="s">
-        <v>525</v>
+        <v>520</v>
       </c>
       <c r="H3" s="10">
         <v>248.8</v>
@@ -2395,7 +2471,7 @@
         <v>96</v>
       </c>
       <c r="M3" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="N3" s="11">
         <v>190</v>
@@ -2413,28 +2489,29 @@
         <v>6.7</v>
       </c>
       <c r="S3" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="T3" s="10">
         <v>140</v>
       </c>
-      <c r="U3" t="s">
+      <c r="U3" s="16" t="s">
         <v>139</v>
       </c>
+      <c r="V3" s="16"/>
       <c r="Y3" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="Z3" s="10">
         <v>180</v>
       </c>
       <c r="AA3" t="s">
-        <v>321</v>
+        <v>302</v>
       </c>
       <c r="AB3" s="10">
-        <v>120</v>
+        <v>138</v>
       </c>
       <c r="AC3" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
       <c r="AD3" s="10">
         <v>13.625</v>
@@ -2445,15 +2522,15 @@
       <c r="AF3" s="10">
         <v>14.08</v>
       </c>
-      <c r="AG3" t="s">
+      <c r="AG3" s="16" t="s">
         <v>185</v>
       </c>
-      <c r="AH3" s="10"/>
+      <c r="AH3" s="17"/>
       <c r="AI3" t="s">
-        <v>99</v>
+        <v>488</v>
       </c>
       <c r="AJ3" s="10">
-        <v>134</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="2:45" x14ac:dyDescent="0.2">
@@ -2465,10 +2542,10 @@
         <v>316</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="G4" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="H4" s="10">
         <v>247</v>
@@ -2480,13 +2557,13 @@
         <v>232</v>
       </c>
       <c r="K4" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
       <c r="L4" s="11">
         <v>103</v>
       </c>
       <c r="M4" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="N4" s="11">
         <v>150</v>
@@ -2498,34 +2575,35 @@
         <v>170</v>
       </c>
       <c r="Q4" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="R4" s="10">
         <v>2.1</v>
       </c>
       <c r="S4" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
       <c r="T4" s="10">
         <v>194</v>
       </c>
-      <c r="U4" t="s">
+      <c r="U4" s="16" t="s">
         <v>270</v>
       </c>
+      <c r="V4" s="16"/>
       <c r="Y4" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="Z4" s="10" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="AA4" t="s">
-        <v>470</v>
+        <v>321</v>
       </c>
       <c r="AB4" s="10">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="AC4" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="AD4" s="10">
         <v>13.625</v>
@@ -2536,15 +2614,15 @@
       <c r="AF4" s="10">
         <v>17</v>
       </c>
-      <c r="AG4" t="s">
+      <c r="AG4" s="16" t="s">
         <v>177</v>
       </c>
-      <c r="AH4" s="10"/>
+      <c r="AH4" s="17"/>
       <c r="AI4" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AJ4" s="10">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="2:45" x14ac:dyDescent="0.2">
@@ -2553,16 +2631,16 @@
       </c>
       <c r="C5" s="5"/>
       <c r="E5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>383</v>
+        <v>541</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>542</v>
       </c>
       <c r="G5" t="s">
-        <v>318</v>
-      </c>
-      <c r="H5" s="11">
-        <v>218</v>
+        <v>534</v>
+      </c>
+      <c r="H5" s="10">
+        <v>304</v>
       </c>
       <c r="I5" t="s">
         <v>56</v>
@@ -2571,13 +2649,13 @@
         <v>226</v>
       </c>
       <c r="K5" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="L5" s="11">
         <v>128</v>
       </c>
       <c r="M5" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="N5" s="11">
         <v>250</v>
@@ -2589,35 +2667,35 @@
         <v>160</v>
       </c>
       <c r="Q5" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="R5" s="10">
         <v>1.5</v>
       </c>
       <c r="S5" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="T5" s="10">
         <v>172</v>
       </c>
-      <c r="U5" t="s">
+      <c r="U5" s="16" t="s">
         <v>152</v>
       </c>
+      <c r="V5" s="16"/>
       <c r="Y5" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="Z5" s="10">
         <v>80</v>
       </c>
       <c r="AA5" t="s">
-        <v>328</v>
+        <v>465</v>
       </c>
       <c r="AB5" s="10">
-        <f>16*16</f>
-        <v>256</v>
+        <v>133</v>
       </c>
       <c r="AC5" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
       <c r="AD5" s="10">
         <v>13.456</v>
@@ -2628,15 +2706,15 @@
       <c r="AF5" s="10">
         <v>14.1</v>
       </c>
-      <c r="AG5" t="s">
+      <c r="AG5" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="AH5" s="10"/>
+      <c r="AH5" s="17"/>
       <c r="AI5" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="AJ5" s="10">
-        <v>149</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" spans="2:45" x14ac:dyDescent="0.2">
@@ -2645,16 +2723,16 @@
       </c>
       <c r="C6" s="5"/>
       <c r="E6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>524</v>
+        <v>532</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>535</v>
       </c>
       <c r="G6" t="s">
-        <v>52</v>
+        <v>318</v>
       </c>
       <c r="H6" s="11">
-        <v>260</v>
+        <v>218</v>
       </c>
       <c r="I6" t="s">
         <v>211</v>
@@ -2663,13 +2741,13 @@
         <v>244</v>
       </c>
       <c r="K6" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="L6" s="11">
         <v>85</v>
       </c>
       <c r="M6" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
       <c r="N6" s="11">
         <v>220</v>
@@ -2687,32 +2765,34 @@
         <v>1.8</v>
       </c>
       <c r="S6" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="T6" s="10">
         <v>202</v>
       </c>
-      <c r="U6" t="s">
+      <c r="U6" s="16" t="s">
         <v>271</v>
       </c>
+      <c r="V6" s="16"/>
       <c r="Y6" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="Z6" s="10">
         <v>80</v>
       </c>
       <c r="AA6" t="s">
-        <v>329</v>
+        <v>528</v>
       </c>
       <c r="AB6" s="10">
         <f>16*16</f>
         <v>256</v>
       </c>
       <c r="AC6" t="s">
-        <v>123</v>
+        <v>543</v>
       </c>
       <c r="AD6" s="10">
-        <v>13.625</v>
+        <f xml:space="preserve"> 282/16</f>
+        <v>17.625</v>
       </c>
       <c r="AE6" t="s">
         <v>284</v>
@@ -2720,15 +2800,15 @@
       <c r="AF6" s="10">
         <v>15</v>
       </c>
-      <c r="AG6" t="s">
-        <v>366</v>
-      </c>
-      <c r="AH6" s="10"/>
+      <c r="AG6" s="16" t="s">
+        <v>361</v>
+      </c>
+      <c r="AH6" s="17"/>
       <c r="AI6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="AJ6" s="10">
-        <v>88</v>
+        <v>149</v>
       </c>
     </row>
     <row r="7" spans="2:45" x14ac:dyDescent="0.2">
@@ -2737,17 +2817,16 @@
       </c>
       <c r="C7" s="5"/>
       <c r="E7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" s="11">
-        <f>128/16</f>
-        <v>8</v>
+        <v>533</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>536</v>
       </c>
       <c r="G7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H7" s="11">
-        <v>241</v>
+        <v>260</v>
       </c>
       <c r="I7" t="s">
         <v>205</v>
@@ -2780,31 +2859,32 @@
         <v>6.9</v>
       </c>
       <c r="S7" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="T7" s="10">
         <v>179</v>
       </c>
-      <c r="U7" t="s">
+      <c r="U7" s="16" t="s">
         <v>138</v>
       </c>
+      <c r="V7" s="16"/>
       <c r="Y7" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="Z7" s="10">
         <v>120</v>
       </c>
       <c r="AA7" t="s">
-        <v>330</v>
+        <v>303</v>
       </c>
       <c r="AB7" s="10">
-        <v>224</v>
+        <v>137</v>
       </c>
       <c r="AC7" t="s">
-        <v>487</v>
+        <v>123</v>
       </c>
       <c r="AD7" s="10">
-        <v>13.5</v>
+        <v>13.625</v>
       </c>
       <c r="AE7" t="s">
         <v>280</v>
@@ -2812,15 +2892,15 @@
       <c r="AF7" s="10">
         <v>15</v>
       </c>
-      <c r="AG7" t="s">
+      <c r="AG7" s="16" t="s">
         <v>173</v>
       </c>
-      <c r="AH7" s="10"/>
+      <c r="AH7" s="17"/>
       <c r="AI7" t="s">
-        <v>491</v>
+        <v>90</v>
       </c>
       <c r="AJ7" s="10">
-        <v>40</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="2:45" x14ac:dyDescent="0.2">
@@ -2829,17 +2909,16 @@
       </c>
       <c r="C8" s="5"/>
       <c r="E8" t="s">
-        <v>25</v>
-      </c>
-      <c r="F8" s="11">
-        <f>144/16</f>
-        <v>9</v>
+        <v>540</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>538</v>
       </c>
       <c r="G8" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="H8" s="11">
-        <v>308</v>
+        <v>241</v>
       </c>
       <c r="I8" t="s">
         <v>209</v>
@@ -2866,37 +2945,39 @@
         <v>176</v>
       </c>
       <c r="Q8" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="R8" s="10">
         <v>6.7</v>
       </c>
       <c r="S8" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="T8" s="10">
         <v>200</v>
       </c>
-      <c r="U8" t="s">
+      <c r="U8" s="16" t="s">
         <v>146</v>
       </c>
+      <c r="V8" s="16"/>
       <c r="Y8" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="Z8" s="10" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="AA8" t="s">
-        <v>331</v>
+        <v>13</v>
       </c>
       <c r="AB8" s="10">
-        <v>256</v>
+        <f>12*16</f>
+        <v>192</v>
       </c>
       <c r="AC8" t="s">
-        <v>36</v>
+        <v>482</v>
       </c>
       <c r="AD8" s="10">
-        <v>20.5</v>
+        <v>13.5</v>
       </c>
       <c r="AE8" t="s">
         <v>296</v>
@@ -2904,15 +2985,15 @@
       <c r="AF8" s="10">
         <v>16.5</v>
       </c>
-      <c r="AG8" t="s">
+      <c r="AG8" s="16" t="s">
         <v>194</v>
       </c>
-      <c r="AH8" s="10"/>
+      <c r="AH8" s="17"/>
       <c r="AI8" t="s">
-        <v>101</v>
+        <v>486</v>
       </c>
       <c r="AJ8" s="10">
-        <v>88</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="2:45" x14ac:dyDescent="0.2">
@@ -2921,18 +3002,16 @@
       </c>
       <c r="C9" s="5"/>
       <c r="E9" t="s">
-        <v>48</v>
-      </c>
-      <c r="F9" s="11">
-        <f>160/16</f>
-        <v>10</v>
+        <v>537</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>539</v>
       </c>
       <c r="G9" t="s">
-        <v>391</v>
+        <v>54</v>
       </c>
       <c r="H9" s="11">
-        <f>H10-H11</f>
-        <v>38</v>
+        <v>308</v>
       </c>
       <c r="I9" t="s">
         <v>216</v>
@@ -2947,7 +3026,7 @@
         <v>137</v>
       </c>
       <c r="M9" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="N9" s="11">
         <v>156</v>
@@ -2965,31 +3044,32 @@
         <v>5.8</v>
       </c>
       <c r="S9" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="T9" s="10">
         <v>164</v>
       </c>
-      <c r="U9" t="s">
+      <c r="U9" s="16" t="s">
         <v>272</v>
       </c>
+      <c r="V9" s="16"/>
       <c r="Y9" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="Z9" s="10">
         <v>80</v>
       </c>
       <c r="AA9" t="s">
-        <v>332</v>
+        <v>468</v>
       </c>
       <c r="AB9" s="10">
-        <v>256</v>
+        <v>93</v>
       </c>
       <c r="AC9" t="s">
-        <v>482</v>
+        <v>36</v>
       </c>
       <c r="AD9" s="10">
-        <v>13.625</v>
+        <v>20.5</v>
       </c>
       <c r="AE9" t="s">
         <v>118</v>
@@ -2997,15 +3077,15 @@
       <c r="AF9" s="10">
         <v>18</v>
       </c>
-      <c r="AG9" t="s">
+      <c r="AG9" s="16" t="s">
         <v>192</v>
       </c>
-      <c r="AH9" s="10"/>
+      <c r="AH9" s="17"/>
       <c r="AI9" t="s">
-        <v>87</v>
+        <v>101</v>
       </c>
       <c r="AJ9" s="10">
-        <v>110</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="2:45" x14ac:dyDescent="0.2">
@@ -3014,16 +3094,17 @@
       </c>
       <c r="C10" s="5"/>
       <c r="E10" t="s">
-        <v>355</v>
-      </c>
-      <c r="F10" s="11">
-        <v>7.85</v>
+        <v>21</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>378</v>
       </c>
       <c r="G10" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="H10" s="11">
-        <v>56</v>
+        <f>H11-H12</f>
+        <v>38</v>
       </c>
       <c r="I10" t="s">
         <v>200</v>
@@ -3032,7 +3113,7 @@
         <v>225</v>
       </c>
       <c r="K10" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="L10" s="11">
         <v>92</v>
@@ -3061,23 +3142,24 @@
       <c r="T10" s="10">
         <v>155</v>
       </c>
-      <c r="U10" t="s">
+      <c r="U10" s="16" t="s">
         <v>148</v>
       </c>
+      <c r="V10" s="16"/>
       <c r="Y10" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="Z10" s="10">
         <v>155</v>
       </c>
       <c r="AA10" t="s">
-        <v>303</v>
+        <v>33</v>
       </c>
       <c r="AB10" s="10">
-        <v>137</v>
+        <v>168</v>
       </c>
       <c r="AC10" t="s">
-        <v>483</v>
+        <v>477</v>
       </c>
       <c r="AD10" s="10">
         <v>13.625</v>
@@ -3088,15 +3170,15 @@
       <c r="AF10" s="10">
         <v>32</v>
       </c>
-      <c r="AG10" t="s">
+      <c r="AG10" s="16" t="s">
         <v>183</v>
       </c>
-      <c r="AH10" s="10"/>
+      <c r="AH10" s="17"/>
       <c r="AI10" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="AJ10" s="10">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="2:45" x14ac:dyDescent="0.2">
@@ -3108,17 +3190,16 @@
         <v>10</v>
       </c>
       <c r="E11" t="s">
-        <v>378</v>
-      </c>
-      <c r="F11" s="11">
-        <f>48/16</f>
-        <v>3</v>
+        <v>23</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>519</v>
       </c>
       <c r="G11" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
       <c r="H11" s="11">
-        <v>18</v>
+        <v>56</v>
       </c>
       <c r="I11" t="s">
         <v>208</v>
@@ -3133,7 +3214,7 @@
         <v>144</v>
       </c>
       <c r="M11" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
       <c r="N11" s="11">
         <v>90</v>
@@ -3151,29 +3232,29 @@
         <v>6.5</v>
       </c>
       <c r="S11" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="T11" s="10">
         <v>150</v>
       </c>
-      <c r="U11" t="s">
+      <c r="U11" s="16" t="s">
         <v>151</v>
       </c>
+      <c r="V11" s="16"/>
       <c r="Y11" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="Z11" s="10">
         <v>240</v>
       </c>
       <c r="AA11" t="s">
-        <v>13</v>
+        <v>529</v>
       </c>
       <c r="AB11" s="10">
-        <f>12*16</f>
-        <v>192</v>
+        <v>224</v>
       </c>
       <c r="AC11" t="s">
-        <v>484</v>
+        <v>478</v>
       </c>
       <c r="AD11" s="10">
         <v>13.625</v>
@@ -3184,15 +3265,15 @@
       <c r="AF11" s="10">
         <v>14.2</v>
       </c>
-      <c r="AG11" t="s">
+      <c r="AG11" s="16" t="s">
         <v>191</v>
       </c>
-      <c r="AH11" s="10"/>
+      <c r="AH11" s="17"/>
       <c r="AI11" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="AJ11" s="10">
-        <v>120</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="2:45" x14ac:dyDescent="0.2">
@@ -3201,32 +3282,32 @@
       </c>
       <c r="C12" s="5"/>
       <c r="E12" t="s">
-        <v>363</v>
+        <v>24</v>
       </c>
       <c r="F12" s="11">
         <f>128/16</f>
         <v>8</v>
       </c>
       <c r="G12" t="s">
-        <v>53</v>
+        <v>388</v>
       </c>
       <c r="H12" s="11">
-        <v>240</v>
+        <v>18</v>
       </c>
       <c r="I12" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="J12" s="10">
         <v>114</v>
       </c>
       <c r="K12" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="L12" s="11">
         <v>114</v>
       </c>
       <c r="M12" t="s">
-        <v>516</v>
+        <v>511</v>
       </c>
       <c r="N12" s="11">
         <v>90</v>
@@ -3244,14 +3325,15 @@
         <v>1.9</v>
       </c>
       <c r="S12" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="T12" s="10">
         <v>150</v>
       </c>
-      <c r="U12" t="s">
+      <c r="U12" s="16" t="s">
         <v>159</v>
       </c>
+      <c r="V12" s="16"/>
       <c r="X12" s="10"/>
       <c r="Y12" t="s">
         <v>114</v>
@@ -3260,13 +3342,13 @@
         <v>80</v>
       </c>
       <c r="AA12" t="s">
-        <v>473</v>
+        <v>308</v>
       </c>
       <c r="AB12" s="10">
-        <v>93</v>
+        <v>135</v>
       </c>
       <c r="AC12" t="s">
-        <v>311</v>
+        <v>479</v>
       </c>
       <c r="AD12" s="10">
         <v>13.625</v>
@@ -3277,15 +3359,15 @@
       <c r="AF12" s="10">
         <v>16</v>
       </c>
-      <c r="AG12" t="s">
+      <c r="AG12" s="16" t="s">
         <v>178</v>
       </c>
-      <c r="AH12" s="10"/>
+      <c r="AH12" s="17"/>
       <c r="AI12" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="AJ12" s="10">
-        <v>36</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="2:45" x14ac:dyDescent="0.2">
@@ -3294,17 +3376,17 @@
       </c>
       <c r="C13" s="5"/>
       <c r="E13" t="s">
-        <v>356</v>
+        <v>25</v>
       </c>
       <c r="F13" s="11">
-        <f>48/16</f>
-        <v>3</v>
+        <f>144/16</f>
+        <v>9</v>
       </c>
       <c r="G13" t="s">
-        <v>479</v>
-      </c>
-      <c r="H13" t="s">
-        <v>390</v>
+        <v>53</v>
+      </c>
+      <c r="H13" s="11">
+        <v>240</v>
       </c>
       <c r="I13" t="s">
         <v>203</v>
@@ -3319,7 +3401,7 @@
         <v>148</v>
       </c>
       <c r="M13" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="N13" s="11">
         <v>75</v>
@@ -3337,29 +3419,30 @@
         <v>5.4</v>
       </c>
       <c r="S13" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="T13" s="10">
         <v>200</v>
       </c>
-      <c r="U13" t="s">
+      <c r="U13" s="16" t="s">
         <v>157</v>
       </c>
+      <c r="V13" s="16"/>
       <c r="X13" s="10"/>
       <c r="Y13" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="Z13" s="10">
         <v>257.60000000000002</v>
       </c>
       <c r="AA13" t="s">
-        <v>33</v>
+        <v>322</v>
       </c>
       <c r="AB13" s="10">
-        <v>168</v>
+        <v>115</v>
       </c>
       <c r="AC13" t="s">
-        <v>521</v>
+        <v>311</v>
       </c>
       <c r="AD13" s="10">
         <v>13.625</v>
@@ -3370,15 +3453,15 @@
       <c r="AF13" s="10">
         <v>15</v>
       </c>
-      <c r="AG13" t="s">
+      <c r="AG13" s="16" t="s">
         <v>193</v>
       </c>
-      <c r="AH13" s="10"/>
+      <c r="AH13" s="17"/>
       <c r="AI13" t="s">
-        <v>93</v>
+        <v>107</v>
       </c>
       <c r="AJ13" s="10">
-        <v>119</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="2:45" x14ac:dyDescent="0.2">
@@ -3387,31 +3470,32 @@
       </c>
       <c r="C14" s="5"/>
       <c r="E14" t="s">
-        <v>381</v>
+        <v>48</v>
       </c>
       <c r="F14" s="11">
-        <v>7.5</v>
+        <f>160/16</f>
+        <v>10</v>
       </c>
       <c r="G14" t="s">
-        <v>527</v>
-      </c>
-      <c r="H14" s="10">
-        <v>241.2</v>
+        <v>474</v>
+      </c>
+      <c r="H14" t="s">
+        <v>385</v>
       </c>
       <c r="I14" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="J14" s="10">
         <v>113</v>
       </c>
       <c r="K14" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="L14" s="11">
         <v>122</v>
       </c>
       <c r="M14" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="N14" s="11">
         <v>147</v>
@@ -3429,32 +3513,33 @@
         <v>8.1</v>
       </c>
       <c r="S14" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="T14" s="10">
         <v>164</v>
       </c>
-      <c r="U14" t="s">
+      <c r="U14" s="16" t="s">
         <v>154</v>
       </c>
+      <c r="V14" s="16"/>
       <c r="X14" s="10"/>
       <c r="Y14" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="Z14" s="10">
         <v>166</v>
       </c>
       <c r="AA14" t="s">
-        <v>308</v>
+        <v>74</v>
       </c>
       <c r="AB14" s="10">
-        <v>135</v>
+        <v>160</v>
       </c>
       <c r="AC14" t="s">
-        <v>37</v>
+        <v>516</v>
       </c>
       <c r="AD14" s="10">
-        <v>21.117999999999999</v>
+        <v>13.625</v>
       </c>
       <c r="AE14" t="s">
         <v>273</v>
@@ -3462,15 +3547,15 @@
       <c r="AF14" s="10">
         <v>17</v>
       </c>
-      <c r="AG14" t="s">
+      <c r="AG14" s="16" t="s">
         <v>195</v>
       </c>
-      <c r="AH14" s="10"/>
+      <c r="AH14" s="17"/>
       <c r="AI14" t="s">
-        <v>113</v>
+        <v>504</v>
       </c>
       <c r="AJ14" s="10">
-        <v>154</v>
+        <v>145</v>
       </c>
     </row>
     <row r="15" spans="2:45" x14ac:dyDescent="0.2">
@@ -3479,16 +3564,16 @@
       </c>
       <c r="C15" s="5"/>
       <c r="E15" t="s">
-        <v>382</v>
+        <v>350</v>
       </c>
       <c r="F15" s="11">
-        <v>12</v>
+        <v>7.85</v>
       </c>
       <c r="G15" t="s">
-        <v>528</v>
+        <v>522</v>
       </c>
       <c r="H15" s="10">
-        <v>240</v>
+        <v>241.2</v>
       </c>
       <c r="I15" t="s">
         <v>215</v>
@@ -3497,13 +3582,13 @@
         <v>216.56299999999999</v>
       </c>
       <c r="K15" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="L15" s="11">
         <v>114</v>
       </c>
       <c r="M15" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
       <c r="N15" s="11">
         <v>227</v>
@@ -3521,32 +3606,33 @@
         <v>6.9</v>
       </c>
       <c r="S15" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="T15" s="10">
         <v>160</v>
       </c>
-      <c r="U15" t="s">
+      <c r="U15" s="16" t="s">
         <v>165</v>
       </c>
+      <c r="V15" s="16"/>
       <c r="X15" s="10"/>
       <c r="Y15" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="Z15" s="10">
         <v>250</v>
       </c>
       <c r="AA15" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="AB15" s="10">
-        <v>115</v>
+        <v>32</v>
       </c>
       <c r="AC15" t="s">
-        <v>319</v>
+        <v>37</v>
       </c>
       <c r="AD15" s="10">
-        <v>14</v>
+        <v>21.117999999999999</v>
       </c>
       <c r="AE15" t="s">
         <v>285</v>
@@ -3554,15 +3640,15 @@
       <c r="AF15" s="10">
         <v>15</v>
       </c>
-      <c r="AG15" t="s">
+      <c r="AG15" s="16" t="s">
         <v>182</v>
       </c>
-      <c r="AH15" s="10"/>
+      <c r="AH15" s="17"/>
       <c r="AI15" t="s">
-        <v>115</v>
+        <v>503</v>
       </c>
       <c r="AJ15" s="10">
-        <v>93</v>
+        <v>154</v>
       </c>
     </row>
     <row r="16" spans="2:45" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -3571,16 +3657,17 @@
       </c>
       <c r="C16" s="7"/>
       <c r="E16" t="s">
-        <v>380</v>
+        <v>373</v>
       </c>
       <c r="F16" s="11">
-        <v>18.25</v>
+        <f>48/16</f>
+        <v>3</v>
       </c>
       <c r="G16" t="s">
-        <v>529</v>
+        <v>523</v>
       </c>
       <c r="H16" s="10">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="I16" t="s">
         <v>220</v>
@@ -3589,7 +3676,7 @@
         <v>112</v>
       </c>
       <c r="K16" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="L16" s="11">
         <v>119</v>
@@ -3613,61 +3700,63 @@
         <v>7.8</v>
       </c>
       <c r="S16" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
       <c r="T16" s="10">
         <v>184</v>
       </c>
-      <c r="U16" t="s">
+      <c r="U16" s="16" t="s">
         <v>155</v>
       </c>
+      <c r="V16" s="16"/>
       <c r="Y16" t="s">
-        <v>530</v>
+        <v>525</v>
       </c>
       <c r="Z16" s="10" t="s">
-        <v>531</v>
+        <v>526</v>
       </c>
       <c r="AA16" t="s">
-        <v>74</v>
+        <v>309</v>
       </c>
       <c r="AB16" s="10">
-        <v>160</v>
+        <v>134</v>
       </c>
       <c r="AC16" t="s">
-        <v>50</v>
+        <v>319</v>
       </c>
       <c r="AD16" s="10">
-        <v>20.7</v>
+        <v>14</v>
       </c>
       <c r="AE16" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="AF16" s="10">
         <v>15</v>
       </c>
-      <c r="AG16" t="s">
+      <c r="AG16" s="16" t="s">
         <v>169</v>
       </c>
-      <c r="AH16" s="10"/>
+      <c r="AH16" s="17"/>
       <c r="AI16" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="AJ16" s="10">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="17" spans="2:36" x14ac:dyDescent="0.2">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="17" spans="1:36" x14ac:dyDescent="0.2">
       <c r="E17" t="s">
-        <v>359</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>386</v>
+        <v>358</v>
+      </c>
+      <c r="F17" s="11">
+        <f>128/16</f>
+        <v>8</v>
       </c>
       <c r="G17" t="s">
-        <v>55</v>
-      </c>
-      <c r="H17" s="11">
-        <v>306</v>
+        <v>524</v>
+      </c>
+      <c r="H17" s="10">
+        <v>243</v>
       </c>
       <c r="I17" t="s">
         <v>226</v>
@@ -3682,7 +3771,7 @@
         <v>104</v>
       </c>
       <c r="M17" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="N17" s="11">
         <v>230</v>
@@ -3700,32 +3789,33 @@
         <v>6.5</v>
       </c>
       <c r="S17" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
       <c r="T17" s="10">
         <v>177</v>
       </c>
-      <c r="U17" t="s">
+      <c r="U17" s="16" t="s">
         <v>145</v>
       </c>
+      <c r="V17" s="16"/>
       <c r="X17" s="10"/>
       <c r="Y17" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="Z17" s="10">
         <v>80</v>
       </c>
       <c r="AA17" t="s">
-        <v>314</v>
+        <v>323</v>
       </c>
       <c r="AB17" s="10">
-        <v>32</v>
+        <v>120</v>
       </c>
       <c r="AC17" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="AD17" s="10">
-        <v>19.667999999999999</v>
+        <v>20.7</v>
       </c>
       <c r="AE17" t="s">
         <v>275</v>
@@ -3733,29 +3823,30 @@
       <c r="AF17" s="10">
         <v>13.8</v>
       </c>
-      <c r="AG17" t="s">
+      <c r="AG17" s="16" t="s">
         <v>187</v>
       </c>
-      <c r="AH17" s="10"/>
+      <c r="AH17" s="17"/>
       <c r="AI17" t="s">
-        <v>492</v>
+        <v>113</v>
       </c>
       <c r="AJ17" s="10">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="18" spans="2:36" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="18" spans="1:36" x14ac:dyDescent="0.2">
       <c r="E18" t="s">
-        <v>362</v>
-      </c>
-      <c r="F18" s="11" t="s">
-        <v>387</v>
+        <v>351</v>
+      </c>
+      <c r="F18" s="11">
+        <f>48/16</f>
+        <v>3</v>
       </c>
       <c r="G18" t="s">
-        <v>32</v>
-      </c>
-      <c r="H18" s="11" t="s">
-        <v>394</v>
+        <v>55</v>
+      </c>
+      <c r="H18" s="11">
+        <v>306</v>
       </c>
       <c r="I18" t="s">
         <v>210</v>
@@ -3788,32 +3879,33 @@
         <v>5</v>
       </c>
       <c r="S18" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="T18" s="10">
         <v>195</v>
       </c>
-      <c r="U18" t="s">
+      <c r="U18" s="16" t="s">
         <v>153</v>
       </c>
+      <c r="V18" s="16"/>
       <c r="X18" s="10"/>
       <c r="Y18" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="Z18" s="10" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
       <c r="AA18" t="s">
-        <v>309</v>
+        <v>530</v>
       </c>
       <c r="AB18" s="10">
-        <v>134</v>
+        <v>256</v>
       </c>
       <c r="AC18" t="s">
-        <v>485</v>
+        <v>38</v>
       </c>
       <c r="AD18" s="10">
-        <v>14</v>
+        <v>19.667999999999999</v>
       </c>
       <c r="AE18" t="s">
         <v>292</v>
@@ -3821,32 +3913,32 @@
       <c r="AF18" s="10">
         <v>15</v>
       </c>
-      <c r="AG18" t="s">
+      <c r="AG18" s="16" t="s">
         <v>171</v>
       </c>
-      <c r="AH18" s="10"/>
+      <c r="AH18" s="17"/>
       <c r="AI18" t="s">
-        <v>84</v>
+        <v>105</v>
       </c>
       <c r="AJ18" s="10">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="19" spans="2:36" x14ac:dyDescent="0.2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>522</v>
+        <v>517</v>
       </c>
       <c r="E19" t="s">
-        <v>361</v>
-      </c>
-      <c r="F19" s="11" t="s">
-        <v>388</v>
+        <v>376</v>
+      </c>
+      <c r="F19" s="11">
+        <v>7.5</v>
       </c>
       <c r="G19" t="s">
-        <v>518</v>
-      </c>
-      <c r="H19" s="10">
-        <v>236.58799999999999</v>
+        <v>32</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>389</v>
       </c>
       <c r="I19" t="s">
         <v>218</v>
@@ -3855,13 +3947,13 @@
         <v>134</v>
       </c>
       <c r="K19" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="L19" s="11">
         <v>116</v>
       </c>
       <c r="M19" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="N19" s="11">
         <v>165</v>
@@ -3879,137 +3971,148 @@
         <v>6</v>
       </c>
       <c r="S19" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
       <c r="T19" s="10">
         <v>198</v>
       </c>
-      <c r="U19" t="s">
+      <c r="U19" s="16" t="s">
         <v>269</v>
       </c>
+      <c r="V19" s="16"/>
       <c r="X19" s="10"/>
       <c r="AA19" t="s">
-        <v>323</v>
+        <v>310</v>
       </c>
       <c r="AB19" s="10">
-        <v>120</v>
+        <v>146</v>
       </c>
       <c r="AC19" t="s">
+        <v>480</v>
+      </c>
+      <c r="AD19" s="10">
+        <v>14</v>
+      </c>
+      <c r="AE19" t="s">
+        <v>274</v>
+      </c>
+      <c r="AF19" s="10">
+        <v>15</v>
+      </c>
+      <c r="AG19" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="AH19" s="17"/>
+      <c r="AI19" t="s">
+        <v>487</v>
+      </c>
+      <c r="AJ19" s="10">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="20" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>518</v>
+      </c>
+      <c r="E20" t="s">
+        <v>377</v>
+      </c>
+      <c r="F20" s="11">
+        <v>12</v>
+      </c>
+      <c r="G20" t="s">
+        <v>513</v>
+      </c>
+      <c r="H20" s="10">
+        <v>236.58799999999999</v>
+      </c>
+      <c r="I20" t="s">
+        <v>212</v>
+      </c>
+      <c r="J20" s="10">
+        <v>240</v>
+      </c>
+      <c r="K20" t="s">
+        <v>45</v>
+      </c>
+      <c r="L20" s="11">
+        <v>170</v>
+      </c>
+      <c r="M20" t="s">
+        <v>397</v>
+      </c>
+      <c r="N20" s="11">
+        <v>170</v>
+      </c>
+      <c r="O20" t="s">
+        <v>79</v>
+      </c>
+      <c r="P20" s="11">
+        <v>140</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>262</v>
+      </c>
+      <c r="R20" s="10">
+        <v>0.375</v>
+      </c>
+      <c r="S20" t="s">
+        <v>458</v>
+      </c>
+      <c r="T20" s="10">
+        <v>178</v>
+      </c>
+      <c r="U20" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="V20" s="16"/>
+      <c r="X20" s="10"/>
+      <c r="AA20" t="s">
+        <v>470</v>
+      </c>
+      <c r="AB20" s="10">
+        <v>180</v>
+      </c>
+      <c r="AC20" t="s">
         <v>39</v>
       </c>
-      <c r="AD19" s="10">
+      <c r="AD20" s="10">
         <f>337/16</f>
         <v>21.0625</v>
       </c>
-      <c r="AE19" t="s">
-        <v>274</v>
-      </c>
-      <c r="AF19" s="10">
-        <v>15</v>
-      </c>
-      <c r="AG19" t="s">
-        <v>180</v>
-      </c>
-      <c r="AH19" s="10"/>
-      <c r="AI19" t="s">
-        <v>96</v>
-      </c>
-      <c r="AJ19" s="10">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="20" spans="2:36" x14ac:dyDescent="0.2">
-      <c r="B20" t="s">
-        <v>523</v>
-      </c>
-      <c r="E20" t="s">
-        <v>358</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>389</v>
-      </c>
-      <c r="I20" t="s">
-        <v>212</v>
-      </c>
-      <c r="J20" s="10">
-        <v>240</v>
-      </c>
-      <c r="K20" t="s">
-        <v>45</v>
-      </c>
-      <c r="L20" s="11">
-        <v>170</v>
-      </c>
-      <c r="M20" t="s">
-        <v>402</v>
-      </c>
-      <c r="N20" s="11">
-        <v>170</v>
-      </c>
-      <c r="O20" t="s">
-        <v>79</v>
-      </c>
-      <c r="P20" s="11">
-        <v>140</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>262</v>
-      </c>
-      <c r="R20" s="10">
-        <v>0.375</v>
-      </c>
-      <c r="S20" t="s">
-        <v>463</v>
-      </c>
-      <c r="T20" s="10">
-        <v>178</v>
-      </c>
-      <c r="U20" t="s">
-        <v>158</v>
-      </c>
-      <c r="X20" s="10"/>
-      <c r="AA20" t="s">
-        <v>310</v>
-      </c>
-      <c r="AB20" s="10">
-        <v>146</v>
-      </c>
-      <c r="AC20" t="s">
-        <v>121</v>
-      </c>
-      <c r="AD20" s="10">
-        <v>13.5</v>
-      </c>
       <c r="AE20" t="s">
         <v>289</v>
       </c>
       <c r="AF20" s="10">
         <v>18</v>
       </c>
-      <c r="AG20" t="s">
+      <c r="AG20" s="16" t="s">
         <v>174</v>
       </c>
-      <c r="AH20" s="10"/>
+      <c r="AH20" s="17"/>
       <c r="AI20" t="s">
-        <v>108</v>
+        <v>84</v>
       </c>
       <c r="AJ20" s="10">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="21" spans="2:36" x14ac:dyDescent="0.2">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="21" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>544</v>
+      </c>
       <c r="B21">
-        <f>SUM(23, 12, 34, 29, 37, 29, 59, 29, 10, 17, 35, 29, 37, 50)</f>
-        <v>430</v>
+        <f>SUM(28, 19, 38, 29, 40, 28, 61, 29, 17, 34, 30, 37)</f>
+        <v>390</v>
       </c>
       <c r="D21">
         <v>20</v>
       </c>
       <c r="E21" t="s">
-        <v>369</v>
-      </c>
-      <c r="F21" s="11" t="s">
-        <v>385</v>
+        <v>375</v>
+      </c>
+      <c r="F21" s="11">
+        <v>18.25</v>
       </c>
       <c r="I21" t="s">
         <v>198</v>
@@ -4018,7 +4121,7 @@
         <v>244</v>
       </c>
       <c r="K21" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
       <c r="L21" s="11">
         <v>106</v>
@@ -4042,23 +4145,24 @@
         <v>6.3</v>
       </c>
       <c r="S21" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="T21" s="10">
         <v>188</v>
       </c>
-      <c r="U21" t="s">
+      <c r="U21" s="16" t="s">
         <v>141</v>
       </c>
+      <c r="V21" s="16"/>
       <c r="X21" s="10"/>
       <c r="AA21" t="s">
-        <v>475</v>
+        <v>324</v>
       </c>
       <c r="AB21" s="10">
-        <v>180</v>
+        <v>144</v>
       </c>
       <c r="AC21" t="s">
-        <v>489</v>
+        <v>121</v>
       </c>
       <c r="AD21" s="10">
         <v>13.5</v>
@@ -4070,26 +4174,30 @@
         <f>244/16</f>
         <v>15.25</v>
       </c>
-      <c r="AG21" t="s">
+      <c r="AG21" s="16" t="s">
         <v>184</v>
       </c>
-      <c r="AH21" s="10"/>
+      <c r="AH21" s="17"/>
       <c r="AI21" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="AJ21" s="10">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="2:36" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>545</v>
+      </c>
       <c r="B22">
+        <f>33 + 32</f>
         <v>65</v>
       </c>
       <c r="E22" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="I22" t="s">
         <v>196</v>
@@ -4098,13 +4206,13 @@
         <v>244</v>
       </c>
       <c r="K22" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="L22" s="11">
         <v>137</v>
       </c>
       <c r="M22" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="N22" s="11">
         <v>212</v>
@@ -4122,127 +4230,136 @@
         <v>6.6</v>
       </c>
       <c r="S22" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="T22" s="10">
         <v>207</v>
       </c>
-      <c r="U22" t="s">
+      <c r="U22" s="16" t="s">
         <v>163</v>
       </c>
+      <c r="V22" s="16"/>
       <c r="X22" s="10"/>
       <c r="AA22" t="s">
-        <v>324</v>
+        <v>307</v>
       </c>
       <c r="AB22" s="10">
-        <v>144</v>
+        <v>99</v>
       </c>
       <c r="AC22" t="s">
+        <v>484</v>
+      </c>
+      <c r="AD22" s="10">
+        <v>13.5</v>
+      </c>
+      <c r="AE22" t="s">
+        <v>283</v>
+      </c>
+      <c r="AF22" s="10">
+        <v>15</v>
+      </c>
+      <c r="AG22" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="AH22" s="17"/>
+      <c r="AI22" t="s">
+        <v>108</v>
+      </c>
+      <c r="AJ22" s="10">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="23" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>546</v>
+      </c>
+      <c r="B23">
+        <f>B21+B22</f>
+        <v>455</v>
+      </c>
+      <c r="E23" t="s">
+        <v>357</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>382</v>
+      </c>
+      <c r="I23" t="s">
+        <v>197</v>
+      </c>
+      <c r="J23" s="10">
+        <v>244</v>
+      </c>
+      <c r="K23" t="s">
+        <v>394</v>
+      </c>
+      <c r="L23" s="11">
+        <v>155</v>
+      </c>
+      <c r="M23" t="s">
+        <v>268</v>
+      </c>
+      <c r="N23" s="11">
+        <v>180</v>
+      </c>
+      <c r="O23" t="s">
+        <v>81</v>
+      </c>
+      <c r="P23" s="11">
+        <v>160</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>423</v>
+      </c>
+      <c r="R23" s="10">
+        <v>3.1</v>
+      </c>
+      <c r="S23" t="s">
+        <v>442</v>
+      </c>
+      <c r="T23" s="10">
+        <v>104</v>
+      </c>
+      <c r="U23" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="V23" s="16"/>
+      <c r="X23" s="10"/>
+      <c r="AA23" t="s">
+        <v>325</v>
+      </c>
+      <c r="AB23" s="10">
+        <v>109</v>
+      </c>
+      <c r="AC23" t="s">
         <v>317</v>
       </c>
-      <c r="AD22" s="10">
+      <c r="AD23" s="10">
         <f>237/16</f>
         <v>14.8125</v>
       </c>
-      <c r="AE22" t="s">
-        <v>283</v>
-      </c>
-      <c r="AF22" s="10">
-        <v>15</v>
-      </c>
-      <c r="AG22" t="s">
-        <v>167</v>
-      </c>
-      <c r="AH22" s="10"/>
-      <c r="AI22" t="s">
-        <v>110</v>
-      </c>
-      <c r="AJ22" s="10">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="23" spans="2:36" x14ac:dyDescent="0.2">
-      <c r="E23" t="s">
-        <v>49</v>
-      </c>
-      <c r="F23" s="11">
-        <v>6.9</v>
-      </c>
-      <c r="I23" t="s">
-        <v>197</v>
-      </c>
-      <c r="J23" s="10">
-        <v>244</v>
-      </c>
-      <c r="K23" t="s">
-        <v>399</v>
-      </c>
-      <c r="L23" s="11">
-        <v>155</v>
-      </c>
-      <c r="M23" t="s">
-        <v>268</v>
-      </c>
-      <c r="N23" s="11">
-        <v>180</v>
-      </c>
-      <c r="O23" t="s">
-        <v>81</v>
-      </c>
-      <c r="P23" s="11">
-        <v>160</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>428</v>
-      </c>
-      <c r="R23" s="10">
-        <v>3.1</v>
-      </c>
-      <c r="S23" t="s">
-        <v>447</v>
-      </c>
-      <c r="T23" s="10">
-        <v>104</v>
-      </c>
-      <c r="U23" t="s">
-        <v>164</v>
-      </c>
-      <c r="X23" s="10"/>
-      <c r="AA23" t="s">
-        <v>307</v>
-      </c>
-      <c r="AB23" s="10">
-        <v>99</v>
-      </c>
-      <c r="AC23" t="s">
-        <v>476</v>
-      </c>
-      <c r="AD23" s="10">
-        <v>13.53</v>
-      </c>
       <c r="AE23" t="s">
         <v>288</v>
       </c>
       <c r="AF23" s="10">
         <v>15</v>
       </c>
-      <c r="AG23" t="s">
+      <c r="AG23" s="16" t="s">
         <v>170</v>
       </c>
-      <c r="AH23" s="10"/>
+      <c r="AH23" s="17"/>
       <c r="AI23" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="AJ23" s="10">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="24" spans="2:36" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:36" x14ac:dyDescent="0.2">
       <c r="E24" t="s">
-        <v>31</v>
-      </c>
-      <c r="F24" s="11">
-        <v>10</v>
+        <v>356</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>383</v>
       </c>
       <c r="I24" t="s">
         <v>219</v>
@@ -4251,13 +4368,13 @@
         <v>113</v>
       </c>
       <c r="K24" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="L24" s="11">
         <v>108</v>
       </c>
       <c r="M24" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="N24" s="11">
         <v>190</v>
@@ -4275,26 +4392,27 @@
         <v>5.8</v>
       </c>
       <c r="S24" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="T24" s="10">
         <v>208</v>
       </c>
-      <c r="U24" t="s">
+      <c r="U24" s="16" t="s">
         <v>140</v>
       </c>
+      <c r="V24" s="16"/>
       <c r="X24" s="10"/>
       <c r="AA24" t="s">
-        <v>325</v>
+        <v>313</v>
       </c>
       <c r="AB24" s="10">
-        <v>109</v>
+        <v>135</v>
       </c>
       <c r="AC24" t="s">
-        <v>488</v>
+        <v>471</v>
       </c>
       <c r="AD24" s="10">
-        <v>13.625</v>
+        <v>13.53</v>
       </c>
       <c r="AE24" t="s">
         <v>287</v>
@@ -4302,18 +4420,24 @@
       <c r="AF24" s="10">
         <v>18</v>
       </c>
-      <c r="AG24" t="s">
+      <c r="AG24" s="16" t="s">
         <v>175</v>
       </c>
-      <c r="AH24" s="10"/>
+      <c r="AH24" s="17"/>
       <c r="AI24" t="s">
-        <v>494</v>
+        <v>110</v>
       </c>
       <c r="AJ24" s="10">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="25" spans="2:36" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="25" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="E25" t="s">
+        <v>353</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>384</v>
+      </c>
       <c r="I25" t="s">
         <v>204</v>
       </c>
@@ -4327,7 +4451,7 @@
         <v>125</v>
       </c>
       <c r="M25" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="N25" s="11">
         <v>165</v>
@@ -4345,23 +4469,24 @@
         <v>11.1</v>
       </c>
       <c r="S25" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="T25" s="10">
         <v>193</v>
       </c>
-      <c r="U25" t="s">
+      <c r="U25" s="16" t="s">
         <v>160</v>
       </c>
+      <c r="V25" s="16"/>
       <c r="X25" s="10"/>
       <c r="AA25" t="s">
-        <v>313</v>
+        <v>304</v>
       </c>
       <c r="AB25" s="10">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="AC25" t="s">
-        <v>40</v>
+        <v>483</v>
       </c>
       <c r="AD25" s="10">
         <v>13.625</v>
@@ -4372,20 +4497,26 @@
       <c r="AF25" s="10">
         <v>15</v>
       </c>
-      <c r="AG25" t="s">
+      <c r="AG25" s="16" t="s">
         <v>181</v>
       </c>
-      <c r="AH25" s="10"/>
+      <c r="AH25" s="17"/>
       <c r="AI25" t="s">
-        <v>495</v>
+        <v>100</v>
       </c>
       <c r="AJ25" s="10">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="26" spans="2:36" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="26" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="E26" t="s">
+        <v>364</v>
+      </c>
+      <c r="F26" s="11" t="s">
+        <v>380</v>
+      </c>
       <c r="I26" t="s">
-        <v>511</v>
+        <v>506</v>
       </c>
       <c r="J26" s="10">
         <v>240</v>
@@ -4409,32 +4540,33 @@
         <v>193</v>
       </c>
       <c r="Q26" t="s">
-        <v>503</v>
+        <v>498</v>
       </c>
       <c r="R26" s="10">
         <v>9.6999999999999993</v>
       </c>
       <c r="S26" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="T26" s="10">
         <v>171</v>
       </c>
-      <c r="U26" t="s">
+      <c r="U26" s="16" t="s">
         <v>150</v>
       </c>
+      <c r="V26" s="16"/>
       <c r="X26" s="10"/>
       <c r="AA26" t="s">
-        <v>304</v>
+        <v>326</v>
       </c>
       <c r="AB26" s="10">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="AC26" t="s">
-        <v>120</v>
+        <v>40</v>
       </c>
       <c r="AD26" s="10">
-        <v>13.5</v>
+        <v>13.625</v>
       </c>
       <c r="AE26" t="s">
         <v>116</v>
@@ -4442,18 +4574,24 @@
       <c r="AF26" s="10">
         <v>16</v>
       </c>
-      <c r="AG26" t="s">
+      <c r="AG26" s="16" t="s">
         <v>186</v>
       </c>
-      <c r="AH26" s="10"/>
+      <c r="AH26" s="17"/>
       <c r="AI26" t="s">
-        <v>496</v>
+        <v>489</v>
       </c>
       <c r="AJ26" s="10">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="27" spans="2:36" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="E27" t="s">
+        <v>355</v>
+      </c>
+      <c r="F27" s="11" t="s">
+        <v>383</v>
+      </c>
       <c r="I27" t="s">
         <v>214</v>
       </c>
@@ -4479,33 +4617,34 @@
         <v>192</v>
       </c>
       <c r="Q27" t="s">
-        <v>513</v>
+        <v>508</v>
       </c>
       <c r="R27" s="10">
         <f>149/16</f>
         <v>9.3125</v>
       </c>
       <c r="S27" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="T27" s="10">
         <v>150</v>
       </c>
-      <c r="U27" t="s">
+      <c r="U27" s="16" t="s">
         <v>166</v>
       </c>
+      <c r="V27" s="16"/>
       <c r="X27" s="10"/>
       <c r="AA27" t="s">
-        <v>326</v>
+        <v>34</v>
       </c>
       <c r="AB27" s="10">
-        <v>133</v>
+        <v>140.80000000000001</v>
       </c>
       <c r="AC27" t="s">
-        <v>471</v>
+        <v>120</v>
       </c>
       <c r="AD27" s="10">
-        <v>14</v>
+        <v>13.5</v>
       </c>
       <c r="AE27" t="s">
         <v>279</v>
@@ -4514,20 +4653,26 @@
         <f>6.5*3</f>
         <v>19.5</v>
       </c>
-      <c r="AG27" t="s">
-        <v>367</v>
-      </c>
-      <c r="AH27" s="10"/>
+      <c r="AG27" s="16" t="s">
+        <v>362</v>
+      </c>
+      <c r="AH27" s="17"/>
       <c r="AI27" t="s">
-        <v>497</v>
+        <v>491</v>
       </c>
       <c r="AJ27" s="10">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="28" spans="2:36" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="E28" t="s">
+        <v>49</v>
+      </c>
+      <c r="F28" s="11">
+        <v>6.9</v>
+      </c>
       <c r="I28" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="J28" s="10">
         <v>100</v>
@@ -4539,44 +4684,45 @@
         <v>120</v>
       </c>
       <c r="M28" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="N28" s="11">
         <v>143</v>
       </c>
       <c r="O28" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="P28" s="11">
         <v>64</v>
       </c>
       <c r="Q28" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
       <c r="R28" s="10">
         <v>14</v>
       </c>
       <c r="S28" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="T28" s="10">
         <v>256</v>
       </c>
-      <c r="U28" t="s">
+      <c r="U28" s="16" t="s">
         <v>161</v>
       </c>
+      <c r="V28" s="16"/>
       <c r="X28" s="10"/>
       <c r="AA28" t="s">
-        <v>34</v>
+        <v>306</v>
       </c>
       <c r="AB28" s="10">
-        <v>140.80000000000001</v>
+        <v>122</v>
       </c>
       <c r="AC28" t="s">
-        <v>124</v>
+        <v>466</v>
       </c>
       <c r="AD28" s="10">
-        <v>13.5</v>
+        <v>14</v>
       </c>
       <c r="AE28" t="s">
         <v>290</v>
@@ -4584,19 +4730,24 @@
       <c r="AF28" s="10">
         <v>10</v>
       </c>
-      <c r="AG28" t="s">
+      <c r="AG28" s="16" t="s">
         <v>188</v>
       </c>
-      <c r="AH28" s="10"/>
+      <c r="AH28" s="17"/>
       <c r="AI28" t="s">
-        <v>498</v>
+        <v>490</v>
       </c>
       <c r="AJ28" s="10">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="29" spans="2:36" x14ac:dyDescent="0.2">
-      <c r="F29" s="10"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="E29" t="s">
+        <v>31</v>
+      </c>
+      <c r="F29" s="11">
+        <v>10</v>
+      </c>
       <c r="I29" t="s">
         <v>213</v>
       </c>
@@ -4610,45 +4761,47 @@
         <v>120</v>
       </c>
       <c r="M29" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="N29" s="11">
         <v>217</v>
       </c>
       <c r="O29" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="P29" s="11">
         <f>28*4</f>
         <v>112</v>
       </c>
       <c r="Q29" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="R29" s="10">
         <v>5.2</v>
       </c>
       <c r="S29" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="T29" s="10">
         <v>197</v>
       </c>
-      <c r="U29" t="s">
+      <c r="U29" s="16" t="s">
         <v>149</v>
       </c>
+      <c r="V29" s="16"/>
       <c r="X29" s="10"/>
       <c r="AA29" t="s">
-        <v>306</v>
+        <v>315</v>
       </c>
       <c r="AB29" s="10">
-        <v>122</v>
+        <f>28*4</f>
+        <v>112</v>
       </c>
       <c r="AC29" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="AD29" s="10">
-        <v>13.625</v>
+        <v>13.5</v>
       </c>
       <c r="AE29" t="s">
         <v>278</v>
@@ -4656,18 +4809,18 @@
       <c r="AF29" s="10">
         <v>18</v>
       </c>
-      <c r="AG29" t="s">
+      <c r="AG29" s="16" t="s">
         <v>189</v>
       </c>
-      <c r="AH29" s="10"/>
+      <c r="AH29" s="17"/>
       <c r="AI29" t="s">
-        <v>499</v>
+        <v>493</v>
       </c>
       <c r="AJ29" s="10">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="30" spans="2:36" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="30" spans="1:36" x14ac:dyDescent="0.2">
       <c r="D30">
         <v>30</v>
       </c>
@@ -4685,37 +4838,37 @@
         <v>135</v>
       </c>
       <c r="M30" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="N30" s="11">
         <v>140</v>
       </c>
       <c r="P30" s="11"/>
       <c r="Q30" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="R30" s="10">
         <v>6</v>
       </c>
       <c r="S30" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="T30" s="10">
         <v>105</v>
       </c>
-      <c r="U30" t="s">
+      <c r="U30" s="16" t="s">
         <v>144</v>
       </c>
+      <c r="V30" s="16"/>
       <c r="X30" s="10"/>
       <c r="AA30" t="s">
-        <v>315</v>
+        <v>35</v>
       </c>
       <c r="AB30" s="10">
-        <f>28*4</f>
-        <v>112</v>
+        <v>128</v>
       </c>
       <c r="AC30" t="s">
-        <v>312</v>
+        <v>122</v>
       </c>
       <c r="AD30" s="10">
         <v>13.625</v>
@@ -4726,18 +4879,18 @@
       <c r="AF30" s="10">
         <v>16.5</v>
       </c>
-      <c r="AG30" t="s">
+      <c r="AG30" s="16" t="s">
         <v>179</v>
       </c>
-      <c r="AH30" s="10"/>
+      <c r="AH30" s="17"/>
       <c r="AI30" t="s">
-        <v>500</v>
+        <v>492</v>
       </c>
       <c r="AJ30" s="10">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="31" spans="2:36" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="1:36" x14ac:dyDescent="0.2">
       <c r="I31" t="s">
         <v>223</v>
       </c>
@@ -4758,35 +4911,41 @@
         <v>6.9</v>
       </c>
       <c r="T31" s="10"/>
-      <c r="U31" t="s">
+      <c r="U31" s="16" t="s">
         <v>147</v>
       </c>
+      <c r="V31" s="16"/>
       <c r="X31" s="10"/>
       <c r="AA31" t="s">
-        <v>35</v>
+        <v>531</v>
       </c>
       <c r="AB31" s="10">
-        <v>128</v>
-      </c>
-      <c r="AD31" s="10"/>
+        <v>256</v>
+      </c>
+      <c r="AC31" t="s">
+        <v>312</v>
+      </c>
+      <c r="AD31" s="10">
+        <v>13.625</v>
+      </c>
       <c r="AE31" t="s">
         <v>286</v>
       </c>
       <c r="AF31" s="10">
         <v>15</v>
       </c>
-      <c r="AG31" t="s">
+      <c r="AG31" s="16" t="s">
         <v>176</v>
       </c>
-      <c r="AH31" s="10"/>
+      <c r="AH31" s="17"/>
       <c r="AI31" t="s">
-        <v>501</v>
+        <v>494</v>
       </c>
       <c r="AJ31" s="10">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="32" spans="2:36" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="32" spans="1:36" x14ac:dyDescent="0.2">
       <c r="I32" t="s">
         <v>202</v>
       </c>
@@ -4794,7 +4953,7 @@
         <v>227</v>
       </c>
       <c r="M32" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="N32" s="11">
         <v>154</v>
@@ -4806,9 +4965,10 @@
         <v>2.8</v>
       </c>
       <c r="T32" s="10"/>
-      <c r="U32" t="s">
+      <c r="U32" s="16" t="s">
         <v>142</v>
       </c>
+      <c r="V32" s="16"/>
       <c r="X32" s="10"/>
       <c r="AA32" t="s">
         <v>305</v>
@@ -4823,15 +4983,15 @@
       <c r="AF32" s="10">
         <v>14.9</v>
       </c>
-      <c r="AG32" t="s">
+      <c r="AG32" s="16" t="s">
         <v>190</v>
       </c>
-      <c r="AH32" s="10"/>
+      <c r="AH32" s="17"/>
       <c r="AI32" t="s">
-        <v>502</v>
+        <v>495</v>
       </c>
       <c r="AJ32" s="10">
-        <v>96</v>
+        <v>86</v>
       </c>
     </row>
     <row r="33" spans="9:36" x14ac:dyDescent="0.2">
@@ -4842,7 +5002,7 @@
         <v>122</v>
       </c>
       <c r="M33" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="N33" s="11">
         <v>150</v>
@@ -4854,9 +5014,10 @@
         <v>6</v>
       </c>
       <c r="T33" s="10"/>
-      <c r="U33" t="s">
+      <c r="U33" s="16" t="s">
         <v>162</v>
       </c>
+      <c r="V33" s="16"/>
       <c r="AA33" t="s">
         <v>320</v>
       </c>
@@ -4870,15 +5031,15 @@
       <c r="AF33" s="10">
         <v>14.938000000000001</v>
       </c>
-      <c r="AG33" t="s">
+      <c r="AG33" s="16" t="s">
         <v>168</v>
       </c>
-      <c r="AH33" s="10"/>
+      <c r="AH33" s="17"/>
       <c r="AI33" t="s">
-        <v>104</v>
+        <v>496</v>
       </c>
       <c r="AJ33" s="10">
-        <v>100</v>
+        <v>89</v>
       </c>
     </row>
     <row r="34" spans="9:36" x14ac:dyDescent="0.2">
@@ -4889,7 +5050,7 @@
         <v>245</v>
       </c>
       <c r="M34" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="N34" s="11">
         <v>168</v>
@@ -4901,9 +5062,10 @@
         <v>6</v>
       </c>
       <c r="T34" s="10"/>
-      <c r="U34" t="s">
+      <c r="U34" s="16" t="s">
         <v>156</v>
       </c>
+      <c r="V34" s="16"/>
       <c r="AA34" t="s">
         <v>327</v>
       </c>
@@ -4919,10 +5081,10 @@
       </c>
       <c r="AH34" s="10"/>
       <c r="AI34" t="s">
-        <v>83</v>
+        <v>497</v>
       </c>
       <c r="AJ34" s="10">
-        <v>142</v>
+        <v>96</v>
       </c>
     </row>
     <row r="35" spans="9:36" x14ac:dyDescent="0.2">
@@ -4933,7 +5095,7 @@
         <v>248</v>
       </c>
       <c r="M35" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="N35" s="11">
         <v>173.25</v>
@@ -4946,24 +5108,24 @@
       </c>
       <c r="T35" s="10"/>
       <c r="AA35" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="AB35" s="10">
         <v>62</v>
       </c>
       <c r="AD35" s="10"/>
       <c r="AE35" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="AF35" s="10">
         <v>14.938000000000001</v>
       </c>
       <c r="AH35" s="10"/>
       <c r="AI35" t="s">
-        <v>85</v>
+        <v>104</v>
       </c>
       <c r="AJ35" s="10">
-        <v>150</v>
+        <v>100</v>
       </c>
     </row>
     <row r="36" spans="9:36" x14ac:dyDescent="0.2">
@@ -4975,7 +5137,7 @@
         <v>224</v>
       </c>
       <c r="M36" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="N36" s="11">
         <v>150</v>
@@ -4989,17 +5151,17 @@
       <c r="T36" s="10"/>
       <c r="AD36" s="10"/>
       <c r="AE36" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="AF36" s="10">
         <v>14.938000000000001</v>
       </c>
       <c r="AH36" s="10"/>
       <c r="AI36" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="AJ36" s="10">
-        <v>116</v>
+        <v>142</v>
       </c>
     </row>
     <row r="37" spans="9:36" x14ac:dyDescent="0.2">
@@ -5010,7 +5172,7 @@
         <v>113</v>
       </c>
       <c r="M37" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="N37" s="11">
         <v>174</v>
@@ -5030,10 +5192,10 @@
         <v>17.117999999999999</v>
       </c>
       <c r="AI37" t="s">
-        <v>112</v>
+        <v>85</v>
       </c>
       <c r="AJ37" s="10">
-        <v>140</v>
+        <v>150</v>
       </c>
     </row>
     <row r="38" spans="9:36" x14ac:dyDescent="0.2">
@@ -5064,10 +5226,10 @@
         <v>18</v>
       </c>
       <c r="AI38" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="AJ38" s="10">
-        <v>160</v>
+        <v>116</v>
       </c>
     </row>
     <row r="39" spans="9:36" x14ac:dyDescent="0.2">
@@ -5093,10 +5255,10 @@
       <c r="AD39" s="10"/>
       <c r="AF39" s="10"/>
       <c r="AI39" t="s">
-        <v>89</v>
+        <v>112</v>
       </c>
       <c r="AJ39" s="10">
-        <v>30</v>
+        <v>140</v>
       </c>
     </row>
     <row r="40" spans="9:36" x14ac:dyDescent="0.2">
@@ -5107,7 +5269,7 @@
         <v>152</v>
       </c>
       <c r="Q40" t="s">
-        <v>504</v>
+        <v>499</v>
       </c>
       <c r="R40" s="10">
         <v>6.9</v>
@@ -5116,10 +5278,10 @@
       <c r="AD40" s="10"/>
       <c r="AF40" s="10"/>
       <c r="AI40" t="s">
-        <v>505</v>
+        <v>109</v>
       </c>
       <c r="AJ40" s="10">
-        <v>140</v>
+        <v>160</v>
       </c>
     </row>
     <row r="41" spans="9:36" x14ac:dyDescent="0.2">
@@ -5130,7 +5292,7 @@
         <v>152</v>
       </c>
       <c r="Q41" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="R41" s="10">
         <v>5.4</v>
@@ -5139,15 +5301,15 @@
       <c r="AD41" s="10"/>
       <c r="AF41" s="10"/>
       <c r="AI41" t="s">
-        <v>506</v>
+        <v>89</v>
       </c>
       <c r="AJ41" s="10">
-        <v>140</v>
+        <v>30</v>
       </c>
     </row>
     <row r="42" spans="9:36" x14ac:dyDescent="0.2">
       <c r="Q42" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="R42" s="10">
         <v>3</v>
@@ -5156,10 +5318,10 @@
       <c r="AD42" s="10"/>
       <c r="AF42" s="10"/>
       <c r="AI42" t="s">
-        <v>507</v>
+        <v>500</v>
       </c>
       <c r="AJ42" s="10">
-        <v>113</v>
+        <v>140</v>
       </c>
     </row>
     <row r="43" spans="9:36" x14ac:dyDescent="0.2">
@@ -5173,15 +5335,15 @@
       <c r="AD43" s="10"/>
       <c r="AF43" s="10"/>
       <c r="AI43" t="s">
-        <v>519</v>
+        <v>501</v>
       </c>
       <c r="AJ43" s="10">
-        <v>101</v>
+        <v>140</v>
       </c>
     </row>
     <row r="44" spans="9:36" x14ac:dyDescent="0.2">
       <c r="Q44" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="R44" s="10">
         <v>6.9</v>
@@ -5190,30 +5352,30 @@
       <c r="AD44" s="10"/>
       <c r="AF44" s="10"/>
       <c r="AI44" t="s">
-        <v>509</v>
+        <v>514</v>
       </c>
       <c r="AJ44" s="10">
-        <v>145</v>
+        <v>101</v>
       </c>
     </row>
     <row r="45" spans="9:36" x14ac:dyDescent="0.2">
       <c r="Q45" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="R45" s="10">
         <v>5.3</v>
       </c>
       <c r="AF45" s="10"/>
       <c r="AI45" t="s">
-        <v>508</v>
+        <v>502</v>
       </c>
       <c r="AJ45" s="10">
-        <v>154</v>
+        <v>113</v>
       </c>
     </row>
     <row r="46" spans="9:36" x14ac:dyDescent="0.2">
       <c r="Q46" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="R46" s="10">
         <v>7.1</v>
@@ -5228,7 +5390,7 @@
     </row>
     <row r="47" spans="9:36" x14ac:dyDescent="0.2">
       <c r="Q47" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="R47" s="10">
         <v>8.6999999999999993</v>
@@ -5242,13 +5404,13 @@
     </row>
     <row r="48" spans="9:36" x14ac:dyDescent="0.2">
       <c r="Q48" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="R48" s="10">
         <v>10</v>
       </c>
       <c r="AI48" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="AJ48" s="10">
         <v>152</v>
@@ -5256,7 +5418,7 @@
     </row>
     <row r="49" spans="17:36" x14ac:dyDescent="0.2">
       <c r="Q49" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="R49" s="10">
         <v>3.3</v>
@@ -5270,7 +5432,7 @@
     </row>
     <row r="50" spans="17:36" x14ac:dyDescent="0.2">
       <c r="Q50" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="R50" s="10">
         <v>1.9</v>
@@ -5289,12 +5451,6 @@
       <c r="R51" s="10">
         <v>2.1</v>
       </c>
-      <c r="AI51" t="s">
-        <v>493</v>
-      </c>
-      <c r="AJ51" s="10">
-        <v>20</v>
-      </c>
     </row>
     <row r="52" spans="17:36" x14ac:dyDescent="0.2">
       <c r="Q52" t="s">
@@ -5325,7 +5481,7 @@
     </row>
     <row r="55" spans="17:36" x14ac:dyDescent="0.2">
       <c r="Q55" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="R55" s="10">
         <v>1.8</v>
@@ -5334,7 +5490,7 @@
     </row>
     <row r="56" spans="17:36" x14ac:dyDescent="0.2">
       <c r="Q56" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="R56" s="10">
         <v>2.4</v>
@@ -5343,7 +5499,7 @@
     </row>
     <row r="57" spans="17:36" x14ac:dyDescent="0.2">
       <c r="Q57" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="R57" s="10">
         <v>4.25</v>
@@ -5352,7 +5508,7 @@
     </row>
     <row r="58" spans="17:36" x14ac:dyDescent="0.2">
       <c r="Q58" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="R58" s="10">
         <v>2.4</v>
@@ -5368,7 +5524,7 @@
     </row>
     <row r="60" spans="17:36" x14ac:dyDescent="0.2">
       <c r="Q60" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="R60" s="10">
         <v>5</v>
@@ -5391,8 +5547,8 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="Y3:Z19">
-    <sortCondition ref="Y2:Y19"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="E2:F29">
+    <sortCondition ref="E2:E29"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="K1" r:id="rId1" xr:uid="{03BE3EB4-1121-B34D-96B6-1846C769CE18}"/>

</xml_diff>

<commit_message>
backup all ongoing .txt and .pdf files
</commit_message>
<xml_diff>
--- a/Ingredients and Types.xlsx
+++ b/Ingredients and Types.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Matthew/Documents/Coding/PersonalProjects/recipeConverter/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FBA2120-66E0-D94C-BD0F-70DD710A93F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0445A23-8AA1-CE45-8353-FDFFFF89C245}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="1900" windowWidth="39780" windowHeight="23260" xr2:uid="{2D2F75AA-471C-5F46-928E-911BD0472A90}"/>
+    <workbookView xWindow="60" yWindow="500" windowWidth="26760" windowHeight="23260" xr2:uid="{2D2F75AA-471C-5F46-928E-911BD0472A90}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="547">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="615">
   <si>
     <t>Baked Goods, Dry</t>
   </si>
@@ -1677,6 +1677,210 @@
   </si>
   <si>
     <t>?done</t>
+  </si>
+  <si>
+    <t>Pasta</t>
+  </si>
+  <si>
+    <t>angel hair, Cooked</t>
+  </si>
+  <si>
+    <t>angel hair, dry</t>
+  </si>
+  <si>
+    <t>bucatini, cooked</t>
+  </si>
+  <si>
+    <t>bucatini, dry</t>
+  </si>
+  <si>
+    <t>Spaghetti, cooked</t>
+  </si>
+  <si>
+    <t>Spaghetti, dry</t>
+  </si>
+  <si>
+    <t>conchiglie, cooked</t>
+  </si>
+  <si>
+    <t>conchiglie, dry</t>
+  </si>
+  <si>
+    <t>ditalini, cooked</t>
+  </si>
+  <si>
+    <t>ditalini, dry</t>
+  </si>
+  <si>
+    <t>farfalle, cooked</t>
+  </si>
+  <si>
+    <t>farfalle, dry</t>
+  </si>
+  <si>
+    <t>fettuccine, cooked</t>
+  </si>
+  <si>
+    <t>fettuccine, dry</t>
+  </si>
+  <si>
+    <t>fusilli, cooked</t>
+  </si>
+  <si>
+    <t>fusilli, dry</t>
+  </si>
+  <si>
+    <t>gemelli, cooked</t>
+  </si>
+  <si>
+    <t>gemelli, dry</t>
+  </si>
+  <si>
+    <t>lasagn, cooked</t>
+  </si>
+  <si>
+    <t>lasagn, dry</t>
+  </si>
+  <si>
+    <t>linguine, cooked</t>
+  </si>
+  <si>
+    <t>linguine, dry</t>
+  </si>
+  <si>
+    <t>macaroni, cooked</t>
+  </si>
+  <si>
+    <t>macaroni, dry</t>
+  </si>
+  <si>
+    <t>orecchiette, cooked</t>
+  </si>
+  <si>
+    <t>orecchiette, dry</t>
+  </si>
+  <si>
+    <t>orzo, cooked</t>
+  </si>
+  <si>
+    <t>orzo, dry</t>
+  </si>
+  <si>
+    <t>pappardelle, cooked</t>
+  </si>
+  <si>
+    <t>pappardelle, dry</t>
+  </si>
+  <si>
+    <t>penne, cooked</t>
+  </si>
+  <si>
+    <t>penne, dry</t>
+  </si>
+  <si>
+    <t>rigatoni, cooked</t>
+  </si>
+  <si>
+    <t>rigatoni, dry</t>
+  </si>
+  <si>
+    <t>rotini, cooked</t>
+  </si>
+  <si>
+    <t>rotini, dry</t>
+  </si>
+  <si>
+    <t>tagliatelle, cooked</t>
+  </si>
+  <si>
+    <t>tagliatelle, dry</t>
+  </si>
+  <si>
+    <t>ziti, cooked</t>
+  </si>
+  <si>
+    <t>ziti, dry</t>
+  </si>
+  <si>
+    <t>cavatelli, cooked</t>
+  </si>
+  <si>
+    <t>cavatelli, dry</t>
+  </si>
+  <si>
+    <t>https://d3ldzx7fxfvsfy.cloudfront.net/kraftwc/article/pdf/pastameasuringchart.pdf</t>
+  </si>
+  <si>
+    <t>vermicelli, cooked</t>
+  </si>
+  <si>
+    <t>Campanelle, cooked</t>
+  </si>
+  <si>
+    <t>Campanelle, Dry</t>
+  </si>
+  <si>
+    <t>Cellentani, cooked</t>
+  </si>
+  <si>
+    <t>Cellentani, dry</t>
+  </si>
+  <si>
+    <t>elbows, cooked</t>
+  </si>
+  <si>
+    <t>Elbows, dry</t>
+  </si>
+  <si>
+    <t>c cooked / cup dry</t>
+  </si>
+  <si>
+    <t>vermicelli, dry</t>
+  </si>
+  <si>
+    <t>Pumpkin</t>
+  </si>
+  <si>
+    <t>Pumpkin Puree</t>
+  </si>
+  <si>
+    <t>Salt, Maldon</t>
+  </si>
+  <si>
+    <t>Salt, Kosher</t>
+  </si>
+  <si>
+    <t>Pumpin Pie Mix</t>
+  </si>
+  <si>
+    <t>Pumpkin Spice</t>
+  </si>
+  <si>
+    <t>Parsley, Fresh</t>
+  </si>
+  <si>
+    <t>Parsley, Dry</t>
+  </si>
+  <si>
+    <t>Olives, Black</t>
+  </si>
+  <si>
+    <t>Olives, Green</t>
+  </si>
+  <si>
+    <t>Olives, Kalamata</t>
+  </si>
+  <si>
+    <t>Broth</t>
+  </si>
+  <si>
+    <t>Mustard, Dijon</t>
+  </si>
+  <si>
+    <t>Vinegar, Champaign</t>
+  </si>
+  <si>
+    <t>Vinegar, White</t>
   </si>
 </sst>
 </file>
@@ -1686,7 +1890,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1743,6 +1947,12 @@
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1829,7 +2039,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1839,7 +2049,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1852,6 +2061,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -2192,10 +2405,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AS62"/>
+  <dimension ref="A1:AS65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="AF48" sqref="AF48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2234,8 +2447,8 @@
     <col min="34" max="34" width="11.5" customWidth="1"/>
     <col min="35" max="35" width="24.5" customWidth="1"/>
     <col min="36" max="36" width="11.5" customWidth="1"/>
-    <col min="37" max="37" width="15.1640625" customWidth="1"/>
-    <col min="38" max="38" width="20.5" customWidth="1"/>
+    <col min="37" max="37" width="27.1640625" customWidth="1"/>
+    <col min="38" max="38" width="11.6640625" style="18" customWidth="1"/>
     <col min="39" max="39" width="14.1640625" customWidth="1"/>
     <col min="40" max="40" width="16.6640625" customWidth="1"/>
     <col min="41" max="41" width="10.83203125" customWidth="1"/>
@@ -2258,13 +2471,13 @@
       <c r="H1" s="8" t="s">
         <v>370</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="11" t="s">
         <v>6</v>
       </c>
       <c r="J1" s="8" t="s">
         <v>370</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="K1" s="12" t="s">
         <v>229</v>
       </c>
       <c r="L1" s="8" t="s">
@@ -2294,10 +2507,10 @@
       <c r="T1" s="8" t="s">
         <v>370</v>
       </c>
-      <c r="U1" s="14" t="s">
+      <c r="U1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="V1" s="15" t="s">
+      <c r="V1" s="14" t="s">
         <v>370</v>
       </c>
       <c r="W1" s="1" t="s">
@@ -2330,10 +2543,10 @@
       <c r="AF1" t="s">
         <v>371</v>
       </c>
-      <c r="AG1" s="14" t="s">
+      <c r="AG1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="AH1" s="15" t="s">
+      <c r="AH1" s="14" t="s">
         <v>370</v>
       </c>
       <c r="AI1" s="1" t="s">
@@ -2342,7 +2555,15 @@
       <c r="AJ1" s="8" t="s">
         <v>370</v>
       </c>
-      <c r="AK1" s="1"/>
+      <c r="AK1" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="AL1" s="18" t="s">
+        <v>370</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>598</v>
+      </c>
       <c r="AQ1" s="1"/>
       <c r="AS1" s="1"/>
     </row>
@@ -2354,7 +2575,7 @@
       <c r="E2" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="11">
+      <c r="F2" s="10">
         <f>220.8/16</f>
         <v>13.8</v>
       </c>
@@ -2367,77 +2588,83 @@
       <c r="I2" t="s">
         <v>390</v>
       </c>
-      <c r="J2" s="10">
+      <c r="J2" s="9">
         <v>112</v>
       </c>
-      <c r="K2" s="13" t="s">
+      <c r="K2" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="L2" s="11">
+      <c r="L2" s="10">
         <v>130</v>
       </c>
       <c r="M2" t="s">
         <v>509</v>
       </c>
-      <c r="N2" s="11">
+      <c r="N2" s="10">
         <v>125</v>
       </c>
       <c r="O2" t="s">
         <v>68</v>
       </c>
-      <c r="P2" s="11">
+      <c r="P2" s="10">
         <v>245</v>
       </c>
       <c r="Q2" t="s">
         <v>241</v>
       </c>
-      <c r="R2" s="10">
+      <c r="R2" s="9">
         <v>6</v>
       </c>
       <c r="S2" t="s">
         <v>331</v>
       </c>
-      <c r="T2" s="10">
+      <c r="T2" s="9">
         <v>197</v>
       </c>
-      <c r="U2" s="16" t="s">
+      <c r="U2" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="V2" s="16"/>
+      <c r="V2" s="15"/>
       <c r="Y2" t="s">
         <v>344</v>
       </c>
-      <c r="Z2" s="10" t="s">
+      <c r="Z2" s="9" t="s">
         <v>461</v>
       </c>
       <c r="AA2" t="s">
         <v>527</v>
       </c>
-      <c r="AB2" s="10">
+      <c r="AB2" s="9">
         <f>16*16</f>
         <v>256</v>
       </c>
       <c r="AC2" t="s">
         <v>12</v>
       </c>
-      <c r="AD2" s="10">
+      <c r="AD2" s="9">
         <v>13.75</v>
       </c>
       <c r="AE2" t="s">
         <v>293</v>
       </c>
-      <c r="AF2" s="10">
+      <c r="AF2" s="9">
         <v>17</v>
       </c>
-      <c r="AG2" s="16" t="s">
+      <c r="AG2" s="15" t="s">
         <v>360</v>
       </c>
-      <c r="AH2" s="17"/>
+      <c r="AH2" s="16"/>
       <c r="AI2" t="s">
         <v>102</v>
       </c>
-      <c r="AJ2" s="10">
+      <c r="AJ2" s="9">
         <v>168</v>
+      </c>
+      <c r="AK2" s="17" t="s">
+        <v>548</v>
+      </c>
+      <c r="AL2" s="10">
+        <v>220</v>
       </c>
     </row>
     <row r="3" spans="2:45" x14ac:dyDescent="0.2">
@@ -2448,89 +2675,95 @@
       <c r="E3" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="11">
+      <c r="F3" s="10">
         <f>220.8/16</f>
         <v>13.8</v>
       </c>
       <c r="G3" t="s">
         <v>520</v>
       </c>
-      <c r="H3" s="10">
+      <c r="H3" s="9">
         <v>248.8</v>
       </c>
       <c r="I3" t="s">
         <v>207</v>
       </c>
-      <c r="J3" s="10">
+      <c r="J3" s="9">
         <v>245.43799999999999</v>
       </c>
       <c r="K3" t="s">
         <v>16</v>
       </c>
-      <c r="L3" s="11">
+      <c r="L3" s="10">
         <v>96</v>
       </c>
       <c r="M3" t="s">
         <v>401</v>
       </c>
-      <c r="N3" s="11">
+      <c r="N3" s="10">
         <v>190</v>
       </c>
       <c r="O3" t="s">
         <v>59</v>
       </c>
-      <c r="P3" s="11">
+      <c r="P3" s="10">
         <v>157</v>
       </c>
       <c r="Q3" t="s">
         <v>248</v>
       </c>
-      <c r="R3" s="10">
+      <c r="R3" s="9">
         <v>6.7</v>
       </c>
       <c r="S3" t="s">
         <v>334</v>
       </c>
-      <c r="T3" s="10">
+      <c r="T3" s="9">
         <v>140</v>
       </c>
-      <c r="U3" s="16" t="s">
+      <c r="U3" s="15" t="s">
         <v>139</v>
       </c>
-      <c r="V3" s="16"/>
+      <c r="V3" s="15"/>
       <c r="Y3" t="s">
-        <v>349</v>
-      </c>
-      <c r="Z3" s="10">
-        <v>180</v>
+        <v>611</v>
+      </c>
+      <c r="Z3" s="9">
+        <v>240</v>
       </c>
       <c r="AA3" t="s">
         <v>302</v>
       </c>
-      <c r="AB3" s="10">
+      <c r="AB3" s="9">
         <v>138</v>
       </c>
       <c r="AC3" t="s">
         <v>475</v>
       </c>
-      <c r="AD3" s="10">
+      <c r="AD3" s="9">
         <v>13.625</v>
       </c>
       <c r="AE3" t="s">
         <v>297</v>
       </c>
-      <c r="AF3" s="10">
+      <c r="AF3" s="9">
         <v>14.08</v>
       </c>
-      <c r="AG3" s="16" t="s">
+      <c r="AG3" s="15" t="s">
         <v>185</v>
       </c>
-      <c r="AH3" s="17"/>
+      <c r="AH3" s="16"/>
       <c r="AI3" t="s">
         <v>488</v>
       </c>
-      <c r="AJ3" s="10">
+      <c r="AJ3" s="9">
         <v>20</v>
+      </c>
+      <c r="AK3" s="17" t="s">
+        <v>549</v>
+      </c>
+      <c r="AL3" s="10">
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="2:45" x14ac:dyDescent="0.2">
@@ -2541,88 +2774,94 @@
       <c r="E4" t="s">
         <v>316</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="10" t="s">
         <v>379</v>
       </c>
       <c r="G4" t="s">
         <v>521</v>
       </c>
-      <c r="H4" s="10">
+      <c r="H4" s="9">
         <v>247</v>
       </c>
       <c r="I4" t="s">
         <v>221</v>
       </c>
-      <c r="J4" s="10">
+      <c r="J4" s="9">
         <v>232</v>
       </c>
       <c r="K4" t="s">
         <v>473</v>
       </c>
-      <c r="L4" s="11">
+      <c r="L4" s="10">
         <v>103</v>
       </c>
       <c r="M4" t="s">
         <v>400</v>
       </c>
-      <c r="N4" s="11">
+      <c r="N4" s="10">
         <v>150</v>
       </c>
       <c r="O4" t="s">
         <v>63</v>
       </c>
-      <c r="P4" s="11">
+      <c r="P4" s="10">
         <v>170</v>
       </c>
       <c r="Q4" t="s">
         <v>420</v>
       </c>
-      <c r="R4" s="10">
+      <c r="R4" s="9">
         <v>2.1</v>
       </c>
       <c r="S4" t="s">
         <v>444</v>
       </c>
-      <c r="T4" s="10">
+      <c r="T4" s="9">
         <v>194</v>
       </c>
-      <c r="U4" s="16" t="s">
+      <c r="U4" s="15" t="s">
         <v>270</v>
       </c>
-      <c r="V4" s="16"/>
+      <c r="V4" s="15"/>
       <c r="Y4" t="s">
-        <v>345</v>
-      </c>
-      <c r="Z4" s="10" t="s">
-        <v>462</v>
+        <v>349</v>
+      </c>
+      <c r="Z4" s="9">
+        <v>180</v>
       </c>
       <c r="AA4" t="s">
         <v>321</v>
       </c>
-      <c r="AB4" s="10">
+      <c r="AB4" s="9">
         <v>120</v>
       </c>
       <c r="AC4" t="s">
         <v>481</v>
       </c>
-      <c r="AD4" s="10">
+      <c r="AD4" s="9">
         <v>13.625</v>
       </c>
       <c r="AE4" t="s">
         <v>277</v>
       </c>
-      <c r="AF4" s="10">
+      <c r="AF4" s="9">
         <v>17</v>
       </c>
-      <c r="AG4" s="16" t="s">
+      <c r="AG4" s="15" t="s">
         <v>177</v>
       </c>
-      <c r="AH4" s="17"/>
+      <c r="AH4" s="16"/>
       <c r="AI4" t="s">
         <v>99</v>
       </c>
-      <c r="AJ4" s="10">
+      <c r="AJ4" s="9">
         <v>134</v>
+      </c>
+      <c r="AK4" s="17" t="s">
+        <v>550</v>
+      </c>
+      <c r="AL4" s="10">
+        <v>240</v>
       </c>
     </row>
     <row r="5" spans="2:45" x14ac:dyDescent="0.2">
@@ -2633,88 +2872,94 @@
       <c r="E5" t="s">
         <v>541</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="9" t="s">
         <v>542</v>
       </c>
       <c r="G5" t="s">
         <v>534</v>
       </c>
-      <c r="H5" s="10">
+      <c r="H5" s="9">
         <v>304</v>
       </c>
       <c r="I5" t="s">
         <v>56</v>
       </c>
-      <c r="J5" s="10">
+      <c r="J5" s="9">
         <v>226</v>
       </c>
       <c r="K5" t="s">
         <v>372</v>
       </c>
-      <c r="L5" s="11">
+      <c r="L5" s="10">
         <v>128</v>
       </c>
       <c r="M5" t="s">
         <v>402</v>
       </c>
-      <c r="N5" s="11">
+      <c r="N5" s="10">
         <v>250</v>
       </c>
       <c r="O5" t="s">
         <v>71</v>
       </c>
-      <c r="P5" s="11">
+      <c r="P5" s="10">
         <v>160</v>
       </c>
       <c r="Q5" t="s">
         <v>421</v>
       </c>
-      <c r="R5" s="10">
+      <c r="R5" s="9">
         <v>1.5</v>
       </c>
       <c r="S5" t="s">
         <v>443</v>
       </c>
-      <c r="T5" s="10">
+      <c r="T5" s="9">
         <v>172</v>
       </c>
-      <c r="U5" s="16" t="s">
+      <c r="U5" s="15" t="s">
         <v>152</v>
       </c>
-      <c r="V5" s="16"/>
+      <c r="V5" s="15"/>
       <c r="Y5" t="s">
-        <v>343</v>
-      </c>
-      <c r="Z5" s="10">
-        <v>80</v>
+        <v>345</v>
+      </c>
+      <c r="Z5" s="9" t="s">
+        <v>462</v>
       </c>
       <c r="AA5" t="s">
         <v>465</v>
       </c>
-      <c r="AB5" s="10">
+      <c r="AB5" s="9">
         <v>133</v>
       </c>
       <c r="AC5" t="s">
         <v>476</v>
       </c>
-      <c r="AD5" s="10">
+      <c r="AD5" s="9">
         <v>13.456</v>
       </c>
       <c r="AE5" t="s">
         <v>281</v>
       </c>
-      <c r="AF5" s="10">
+      <c r="AF5" s="9">
         <v>14.1</v>
       </c>
-      <c r="AG5" s="16" t="s">
+      <c r="AG5" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="AH5" s="17"/>
+      <c r="AH5" s="16"/>
       <c r="AI5" t="s">
         <v>98</v>
       </c>
-      <c r="AJ5" s="10">
+      <c r="AJ5" s="9">
         <v>136</v>
+      </c>
+      <c r="AK5" s="17" t="s">
+        <v>551</v>
+      </c>
+      <c r="AL5" s="10">
+        <v>160</v>
       </c>
     </row>
     <row r="6" spans="2:45" x14ac:dyDescent="0.2">
@@ -2725,90 +2970,99 @@
       <c r="E6" t="s">
         <v>532</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="9" t="s">
         <v>535</v>
       </c>
       <c r="G6" t="s">
         <v>318</v>
       </c>
-      <c r="H6" s="11">
+      <c r="H6" s="10">
         <v>218</v>
       </c>
       <c r="I6" t="s">
         <v>211</v>
       </c>
-      <c r="J6" s="10">
+      <c r="J6" s="9">
         <v>244</v>
       </c>
       <c r="K6" t="s">
         <v>416</v>
       </c>
-      <c r="L6" s="11">
+      <c r="L6" s="10">
         <v>85</v>
       </c>
       <c r="M6" t="s">
         <v>510</v>
       </c>
-      <c r="N6" s="11">
+      <c r="N6" s="10">
         <v>220</v>
       </c>
       <c r="O6" t="s">
         <v>65</v>
       </c>
-      <c r="P6" s="11">
+      <c r="P6" s="10">
         <v>173</v>
       </c>
       <c r="Q6" t="s">
         <v>239</v>
       </c>
-      <c r="R6" s="10">
+      <c r="R6" s="9">
         <v>1.8</v>
       </c>
       <c r="S6" t="s">
         <v>446</v>
       </c>
-      <c r="T6" s="10">
+      <c r="T6" s="9">
         <v>202</v>
       </c>
-      <c r="U6" s="16" t="s">
+      <c r="U6" s="15" t="s">
         <v>271</v>
       </c>
-      <c r="V6" s="16"/>
+      <c r="V6" s="15"/>
       <c r="Y6" t="s">
-        <v>341</v>
-      </c>
-      <c r="Z6" s="10">
+        <v>343</v>
+      </c>
+      <c r="Z6" s="9">
         <v>80</v>
       </c>
       <c r="AA6" t="s">
         <v>528</v>
       </c>
-      <c r="AB6" s="10">
+      <c r="AB6" s="9">
         <f>16*16</f>
         <v>256</v>
       </c>
       <c r="AC6" t="s">
         <v>543</v>
       </c>
-      <c r="AD6" s="10">
+      <c r="AD6" s="9">
         <f xml:space="preserve"> 282/16</f>
         <v>17.625</v>
       </c>
       <c r="AE6" t="s">
         <v>284</v>
       </c>
-      <c r="AF6" s="10">
+      <c r="AF6" s="9">
         <v>15</v>
       </c>
-      <c r="AG6" s="16" t="s">
+      <c r="AG6" s="15" t="s">
         <v>361</v>
       </c>
-      <c r="AH6" s="17"/>
+      <c r="AH6" s="16"/>
       <c r="AI6" t="s">
         <v>88</v>
       </c>
-      <c r="AJ6" s="10">
+      <c r="AJ6" s="9">
         <v>149</v>
+      </c>
+      <c r="AK6" s="17" t="s">
+        <v>592</v>
+      </c>
+      <c r="AL6" s="10">
+        <v>235</v>
+      </c>
+      <c r="AM6">
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="2:45" x14ac:dyDescent="0.2">
@@ -2819,88 +3073,97 @@
       <c r="E7" t="s">
         <v>533</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="9" t="s">
         <v>536</v>
       </c>
       <c r="G7" t="s">
         <v>52</v>
       </c>
-      <c r="H7" s="11">
+      <c r="H7" s="10">
         <v>260</v>
       </c>
       <c r="I7" t="s">
         <v>205</v>
       </c>
-      <c r="J7" s="10">
+      <c r="J7" s="9">
         <v>113</v>
       </c>
       <c r="K7" t="s">
         <v>19</v>
       </c>
-      <c r="L7" s="11">
+      <c r="L7" s="10">
         <v>139</v>
       </c>
       <c r="M7" t="s">
         <v>133</v>
       </c>
-      <c r="N7" s="11">
+      <c r="N7" s="10">
         <v>144</v>
       </c>
       <c r="O7" t="s">
         <v>78</v>
       </c>
-      <c r="P7" s="11">
+      <c r="P7" s="10">
         <v>240</v>
       </c>
       <c r="Q7" t="s">
         <v>230</v>
       </c>
-      <c r="R7" s="10">
+      <c r="R7" s="9">
         <v>6.9</v>
       </c>
       <c r="S7" t="s">
         <v>445</v>
       </c>
-      <c r="T7" s="10">
+      <c r="T7" s="9">
         <v>179</v>
       </c>
-      <c r="U7" s="16" t="s">
+      <c r="U7" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="V7" s="16"/>
+      <c r="V7" s="15"/>
       <c r="Y7" t="s">
-        <v>469</v>
-      </c>
-      <c r="Z7" s="10">
-        <v>120</v>
+        <v>341</v>
+      </c>
+      <c r="Z7" s="9">
+        <v>80</v>
       </c>
       <c r="AA7" t="s">
         <v>303</v>
       </c>
-      <c r="AB7" s="10">
+      <c r="AB7" s="9">
         <v>137</v>
       </c>
       <c r="AC7" t="s">
         <v>123</v>
       </c>
-      <c r="AD7" s="10">
+      <c r="AD7" s="9">
         <v>13.625</v>
       </c>
       <c r="AE7" t="s">
         <v>280</v>
       </c>
-      <c r="AF7" s="10">
+      <c r="AF7" s="9">
         <v>15</v>
       </c>
-      <c r="AG7" s="16" t="s">
+      <c r="AG7" s="15" t="s">
         <v>173</v>
       </c>
-      <c r="AH7" s="17"/>
+      <c r="AH7" s="16"/>
       <c r="AI7" t="s">
         <v>90</v>
       </c>
-      <c r="AJ7" s="10">
+      <c r="AJ7" s="9">
         <v>88</v>
+      </c>
+      <c r="AK7" s="17" t="s">
+        <v>593</v>
+      </c>
+      <c r="AL7" s="10">
+        <v>155</v>
+      </c>
+      <c r="AM7">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:45" x14ac:dyDescent="0.2">
@@ -2911,89 +3174,95 @@
       <c r="E8" t="s">
         <v>540</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="9" t="s">
         <v>538</v>
       </c>
       <c r="G8" t="s">
         <v>51</v>
       </c>
-      <c r="H8" s="11">
+      <c r="H8" s="10">
         <v>241</v>
       </c>
       <c r="I8" t="s">
         <v>209</v>
       </c>
-      <c r="J8" s="10">
+      <c r="J8" s="9">
         <v>226.667</v>
       </c>
       <c r="K8" t="s">
         <v>43</v>
       </c>
-      <c r="L8" s="11">
+      <c r="L8" s="10">
         <v>120</v>
       </c>
       <c r="M8" t="s">
         <v>126</v>
       </c>
-      <c r="N8" s="11">
+      <c r="N8" s="10">
         <v>148</v>
       </c>
       <c r="O8" t="s">
         <v>77</v>
       </c>
-      <c r="P8" s="11">
+      <c r="P8" s="10">
         <v>176</v>
       </c>
       <c r="Q8" t="s">
         <v>422</v>
       </c>
-      <c r="R8" s="10">
+      <c r="R8" s="9">
         <v>6.7</v>
       </c>
       <c r="S8" t="s">
         <v>447</v>
       </c>
-      <c r="T8" s="10">
+      <c r="T8" s="9">
         <v>200</v>
       </c>
-      <c r="U8" s="16" t="s">
+      <c r="U8" s="15" t="s">
         <v>146</v>
       </c>
-      <c r="V8" s="16"/>
+      <c r="V8" s="15"/>
       <c r="Y8" t="s">
-        <v>352</v>
-      </c>
-      <c r="Z8" s="10" t="s">
-        <v>463</v>
+        <v>469</v>
+      </c>
+      <c r="Z8" s="9">
+        <v>120</v>
       </c>
       <c r="AA8" t="s">
         <v>13</v>
       </c>
-      <c r="AB8" s="10">
+      <c r="AB8" s="9">
         <f>12*16</f>
         <v>192</v>
       </c>
       <c r="AC8" t="s">
         <v>482</v>
       </c>
-      <c r="AD8" s="10">
+      <c r="AD8" s="9">
         <v>13.5</v>
       </c>
       <c r="AE8" t="s">
         <v>296</v>
       </c>
-      <c r="AF8" s="10">
+      <c r="AF8" s="9">
         <v>16.5</v>
       </c>
-      <c r="AG8" s="16" t="s">
+      <c r="AG8" s="15" t="s">
         <v>194</v>
       </c>
-      <c r="AH8" s="17"/>
+      <c r="AH8" s="16"/>
       <c r="AI8" t="s">
         <v>486</v>
       </c>
-      <c r="AJ8" s="10">
+      <c r="AJ8" s="9">
         <v>40</v>
+      </c>
+      <c r="AK8" s="17" t="s">
+        <v>588</v>
+      </c>
+      <c r="AL8" s="10">
+        <v>225</v>
       </c>
     </row>
     <row r="9" spans="2:45" x14ac:dyDescent="0.2">
@@ -3004,88 +3273,94 @@
       <c r="E9" t="s">
         <v>537</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F9" s="9" t="s">
         <v>539</v>
       </c>
       <c r="G9" t="s">
         <v>54</v>
       </c>
-      <c r="H9" s="11">
+      <c r="H9" s="10">
         <v>308</v>
       </c>
       <c r="I9" t="s">
         <v>216</v>
       </c>
-      <c r="J9" s="10">
+      <c r="J9" s="9">
         <v>120</v>
       </c>
       <c r="K9" t="s">
         <v>20</v>
       </c>
-      <c r="L9" s="11">
+      <c r="L9" s="10">
         <v>137</v>
       </c>
       <c r="M9" t="s">
         <v>398</v>
       </c>
-      <c r="N9" s="11">
+      <c r="N9" s="10">
         <v>156</v>
       </c>
       <c r="O9" t="s">
         <v>67</v>
       </c>
-      <c r="P9" s="11">
+      <c r="P9" s="10">
         <v>240</v>
       </c>
       <c r="Q9" t="s">
         <v>238</v>
       </c>
-      <c r="R9" s="10">
+      <c r="R9" s="9">
         <v>5.8</v>
       </c>
       <c r="S9" t="s">
         <v>448</v>
       </c>
-      <c r="T9" s="10">
+      <c r="T9" s="9">
         <v>164</v>
       </c>
-      <c r="U9" s="16" t="s">
+      <c r="U9" s="15" t="s">
         <v>272</v>
       </c>
-      <c r="V9" s="16"/>
+      <c r="V9" s="15"/>
       <c r="Y9" t="s">
-        <v>340</v>
-      </c>
-      <c r="Z9" s="10">
-        <v>80</v>
+        <v>352</v>
+      </c>
+      <c r="Z9" s="9" t="s">
+        <v>463</v>
       </c>
       <c r="AA9" t="s">
         <v>468</v>
       </c>
-      <c r="AB9" s="10">
+      <c r="AB9" s="9">
         <v>93</v>
       </c>
       <c r="AC9" t="s">
         <v>36</v>
       </c>
-      <c r="AD9" s="10">
+      <c r="AD9" s="9">
         <v>20.5</v>
       </c>
       <c r="AE9" t="s">
         <v>118</v>
       </c>
-      <c r="AF9" s="10">
+      <c r="AF9" s="9">
         <v>18</v>
       </c>
-      <c r="AG9" s="16" t="s">
+      <c r="AG9" s="15" t="s">
         <v>192</v>
       </c>
-      <c r="AH9" s="17"/>
+      <c r="AH9" s="16"/>
       <c r="AI9" t="s">
         <v>101</v>
       </c>
-      <c r="AJ9" s="10">
+      <c r="AJ9" s="9">
         <v>88</v>
+      </c>
+      <c r="AK9" s="17" t="s">
+        <v>589</v>
+      </c>
+      <c r="AL9" s="10">
+        <v>150</v>
       </c>
     </row>
     <row r="10" spans="2:45" x14ac:dyDescent="0.2">
@@ -3096,89 +3371,98 @@
       <c r="E10" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="F10" s="10" t="s">
         <v>378</v>
       </c>
       <c r="G10" t="s">
         <v>386</v>
       </c>
-      <c r="H10" s="11">
+      <c r="H10" s="10">
         <f>H11-H12</f>
         <v>38</v>
       </c>
       <c r="I10" t="s">
         <v>200</v>
       </c>
-      <c r="J10" s="10">
+      <c r="J10" s="9">
         <v>225</v>
       </c>
       <c r="K10" t="s">
         <v>393</v>
       </c>
-      <c r="L10" s="11">
+      <c r="L10" s="10">
         <v>92</v>
       </c>
       <c r="M10" t="s">
         <v>130</v>
       </c>
-      <c r="N10" s="11">
+      <c r="N10" s="10">
         <v>103</v>
       </c>
       <c r="O10" t="s">
         <v>72</v>
       </c>
-      <c r="P10" s="11">
+      <c r="P10" s="10">
         <v>243</v>
       </c>
       <c r="Q10" t="s">
         <v>254</v>
       </c>
-      <c r="R10" s="10">
+      <c r="R10" s="9">
         <v>12.6</v>
       </c>
       <c r="S10" t="s">
         <v>115</v>
       </c>
-      <c r="T10" s="10">
+      <c r="T10" s="9">
         <v>155</v>
       </c>
-      <c r="U10" s="16" t="s">
+      <c r="U10" s="15" t="s">
         <v>148</v>
       </c>
-      <c r="V10" s="16"/>
+      <c r="V10" s="15"/>
       <c r="Y10" t="s">
-        <v>347</v>
-      </c>
-      <c r="Z10" s="10">
-        <v>155</v>
+        <v>340</v>
+      </c>
+      <c r="Z10" s="9">
+        <v>80</v>
       </c>
       <c r="AA10" t="s">
         <v>33</v>
       </c>
-      <c r="AB10" s="10">
+      <c r="AB10" s="9">
         <v>168</v>
       </c>
       <c r="AC10" t="s">
         <v>477</v>
       </c>
-      <c r="AD10" s="10">
+      <c r="AD10" s="9">
         <v>13.625</v>
       </c>
       <c r="AE10" t="s">
         <v>294</v>
       </c>
-      <c r="AF10" s="10">
+      <c r="AF10" s="9">
         <v>32</v>
       </c>
-      <c r="AG10" s="16" t="s">
+      <c r="AG10" s="15" t="s">
         <v>183</v>
       </c>
-      <c r="AH10" s="17"/>
+      <c r="AH10" s="16"/>
       <c r="AI10" t="s">
         <v>87</v>
       </c>
-      <c r="AJ10" s="10">
+      <c r="AJ10" s="9">
         <v>110</v>
+      </c>
+      <c r="AK10" s="17" t="s">
+        <v>594</v>
+      </c>
+      <c r="AL10" s="10">
+        <v>230</v>
+      </c>
+      <c r="AM10">
+        <v>1.9</v>
       </c>
     </row>
     <row r="11" spans="2:45" x14ac:dyDescent="0.2">
@@ -3192,88 +3476,97 @@
       <c r="E11" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="F11" s="10" t="s">
         <v>519</v>
       </c>
       <c r="G11" t="s">
         <v>387</v>
       </c>
-      <c r="H11" s="11">
+      <c r="H11" s="10">
         <v>56</v>
       </c>
       <c r="I11" t="s">
         <v>208</v>
       </c>
-      <c r="J11" s="10">
+      <c r="J11" s="9">
         <v>228</v>
       </c>
       <c r="K11" t="s">
         <v>22</v>
       </c>
-      <c r="L11" s="11">
+      <c r="L11" s="10">
         <v>144</v>
       </c>
       <c r="M11" t="s">
         <v>515</v>
       </c>
-      <c r="N11" s="11">
+      <c r="N11" s="10">
         <v>90</v>
       </c>
       <c r="O11" t="s">
         <v>75</v>
       </c>
-      <c r="P11" s="11">
+      <c r="P11" s="10">
         <v>122</v>
       </c>
       <c r="Q11" t="s">
         <v>244</v>
       </c>
-      <c r="R11" s="10">
+      <c r="R11" s="9">
         <v>6.5</v>
       </c>
       <c r="S11" t="s">
         <v>449</v>
       </c>
-      <c r="T11" s="10">
+      <c r="T11" s="9">
         <v>150</v>
       </c>
-      <c r="U11" s="16" t="s">
+      <c r="U11" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="V11" s="16"/>
+      <c r="V11" s="15"/>
       <c r="Y11" t="s">
-        <v>348</v>
-      </c>
-      <c r="Z11" s="10">
-        <v>240</v>
+        <v>608</v>
+      </c>
+      <c r="Z11" s="9">
+        <v>135</v>
       </c>
       <c r="AA11" t="s">
         <v>529</v>
       </c>
-      <c r="AB11" s="10">
+      <c r="AB11" s="9">
         <v>224</v>
       </c>
       <c r="AC11" t="s">
         <v>478</v>
       </c>
-      <c r="AD11" s="10">
+      <c r="AD11" s="9">
         <v>13.625</v>
       </c>
       <c r="AE11" t="s">
         <v>298</v>
       </c>
-      <c r="AF11" s="10">
+      <c r="AF11" s="9">
         <v>14.2</v>
       </c>
-      <c r="AG11" s="16" t="s">
+      <c r="AG11" s="15" t="s">
         <v>191</v>
       </c>
-      <c r="AH11" s="17"/>
+      <c r="AH11" s="16"/>
       <c r="AI11" t="s">
         <v>94</v>
       </c>
-      <c r="AJ11" s="10">
+      <c r="AJ11" s="9">
         <v>107</v>
+      </c>
+      <c r="AK11" s="17" t="s">
+        <v>595</v>
+      </c>
+      <c r="AL11" s="10">
+        <v>145</v>
+      </c>
+      <c r="AM11">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="2:45" x14ac:dyDescent="0.2">
@@ -3284,90 +3577,96 @@
       <c r="E12" t="s">
         <v>24</v>
       </c>
-      <c r="F12" s="11">
+      <c r="F12" s="10">
         <f>128/16</f>
         <v>8</v>
       </c>
       <c r="G12" t="s">
         <v>388</v>
       </c>
-      <c r="H12" s="11">
+      <c r="H12" s="10">
         <v>18</v>
       </c>
       <c r="I12" t="s">
         <v>391</v>
       </c>
-      <c r="J12" s="10">
+      <c r="J12" s="9">
         <v>114</v>
       </c>
       <c r="K12" t="s">
         <v>369</v>
       </c>
-      <c r="L12" s="11">
+      <c r="L12" s="10">
         <v>114</v>
       </c>
       <c r="M12" t="s">
         <v>511</v>
       </c>
-      <c r="N12" s="11">
+      <c r="N12" s="10">
         <v>90</v>
       </c>
       <c r="O12" t="s">
         <v>73</v>
       </c>
-      <c r="P12" s="11">
+      <c r="P12" s="10">
         <v>156</v>
       </c>
       <c r="Q12" t="s">
         <v>260</v>
       </c>
-      <c r="R12" s="10">
+      <c r="R12" s="9">
         <v>1.9</v>
       </c>
       <c r="S12" t="s">
         <v>450</v>
       </c>
-      <c r="T12" s="10">
+      <c r="T12" s="9">
         <v>150</v>
       </c>
-      <c r="U12" s="16" t="s">
+      <c r="U12" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="V12" s="16"/>
-      <c r="X12" s="10"/>
+      <c r="V12" s="15"/>
+      <c r="X12" s="9"/>
       <c r="Y12" t="s">
-        <v>114</v>
-      </c>
-      <c r="Z12" s="10">
-        <v>80</v>
+        <v>609</v>
+      </c>
+      <c r="Z12" s="9">
+        <v>133</v>
       </c>
       <c r="AA12" t="s">
         <v>308</v>
       </c>
-      <c r="AB12" s="10">
+      <c r="AB12" s="9">
         <v>135</v>
       </c>
       <c r="AC12" t="s">
         <v>479</v>
       </c>
-      <c r="AD12" s="10">
+      <c r="AD12" s="9">
         <v>13.625</v>
       </c>
       <c r="AE12" t="s">
         <v>282</v>
       </c>
-      <c r="AF12" s="10">
+      <c r="AF12" s="9">
         <v>16</v>
       </c>
-      <c r="AG12" s="16" t="s">
+      <c r="AG12" s="15" t="s">
         <v>178</v>
       </c>
-      <c r="AH12" s="17"/>
+      <c r="AH12" s="16"/>
       <c r="AI12" t="s">
         <v>92</v>
       </c>
-      <c r="AJ12" s="10">
+      <c r="AJ12" s="9">
         <v>120</v>
+      </c>
+      <c r="AK12" s="17" t="s">
+        <v>554</v>
+      </c>
+      <c r="AL12" s="10">
+        <v>240</v>
       </c>
     </row>
     <row r="13" spans="2:45" x14ac:dyDescent="0.2">
@@ -3378,90 +3677,96 @@
       <c r="E13" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="11">
+      <c r="F13" s="10">
         <f>144/16</f>
         <v>9</v>
       </c>
       <c r="G13" t="s">
         <v>53</v>
       </c>
-      <c r="H13" s="11">
+      <c r="H13" s="10">
         <v>240</v>
       </c>
       <c r="I13" t="s">
         <v>203</v>
       </c>
-      <c r="J13" s="10">
+      <c r="J13" s="9">
         <v>112</v>
       </c>
       <c r="K13" t="s">
         <v>42</v>
       </c>
-      <c r="L13" s="11">
+      <c r="L13" s="10">
         <v>148</v>
       </c>
       <c r="M13" t="s">
         <v>468</v>
       </c>
-      <c r="N13" s="11">
+      <c r="N13" s="10">
         <v>75</v>
       </c>
       <c r="O13" t="s">
         <v>74</v>
       </c>
-      <c r="P13" s="11">
+      <c r="P13" s="10">
         <v>160</v>
       </c>
       <c r="Q13" t="s">
         <v>257</v>
       </c>
-      <c r="R13" s="10">
+      <c r="R13" s="9">
         <v>5.4</v>
       </c>
       <c r="S13" t="s">
         <v>451</v>
       </c>
-      <c r="T13" s="10">
+      <c r="T13" s="9">
         <v>200</v>
       </c>
-      <c r="U13" s="16" t="s">
+      <c r="U13" s="15" t="s">
         <v>157</v>
       </c>
-      <c r="V13" s="16"/>
-      <c r="X13" s="10"/>
+      <c r="V13" s="15"/>
+      <c r="X13" s="9"/>
       <c r="Y13" t="s">
-        <v>339</v>
-      </c>
-      <c r="Z13" s="10">
-        <v>257.60000000000002</v>
+        <v>610</v>
+      </c>
+      <c r="Z13" s="9">
+        <v>130</v>
       </c>
       <c r="AA13" t="s">
         <v>322</v>
       </c>
-      <c r="AB13" s="10">
+      <c r="AB13" s="9">
         <v>115</v>
       </c>
       <c r="AC13" t="s">
         <v>311</v>
       </c>
-      <c r="AD13" s="10">
+      <c r="AD13" s="9">
         <v>13.625</v>
       </c>
       <c r="AE13" t="s">
         <v>276</v>
       </c>
-      <c r="AF13" s="10">
+      <c r="AF13" s="9">
         <v>15</v>
       </c>
-      <c r="AG13" s="16" t="s">
+      <c r="AG13" s="15" t="s">
         <v>193</v>
       </c>
-      <c r="AH13" s="17"/>
+      <c r="AH13" s="16"/>
       <c r="AI13" t="s">
         <v>107</v>
       </c>
-      <c r="AJ13" s="10">
+      <c r="AJ13" s="9">
         <v>36</v>
+      </c>
+      <c r="AK13" s="17" t="s">
+        <v>555</v>
+      </c>
+      <c r="AL13" s="10">
+        <v>165</v>
       </c>
     </row>
     <row r="14" spans="2:45" x14ac:dyDescent="0.2">
@@ -3472,7 +3777,7 @@
       <c r="E14" t="s">
         <v>48</v>
       </c>
-      <c r="F14" s="11">
+      <c r="F14" s="10">
         <f>160/16</f>
         <v>10</v>
       </c>
@@ -3485,77 +3790,86 @@
       <c r="I14" t="s">
         <v>467</v>
       </c>
-      <c r="J14" s="10">
+      <c r="J14" s="9">
         <v>113</v>
       </c>
       <c r="K14" t="s">
         <v>368</v>
       </c>
-      <c r="L14" s="11">
+      <c r="L14" s="10">
         <v>122</v>
       </c>
       <c r="M14" t="s">
         <v>396</v>
       </c>
-      <c r="N14" s="11">
+      <c r="N14" s="10">
         <v>147</v>
       </c>
       <c r="O14" t="s">
         <v>80</v>
       </c>
-      <c r="P14" s="11">
+      <c r="P14" s="10">
         <v>177</v>
       </c>
       <c r="Q14" t="s">
         <v>233</v>
       </c>
-      <c r="R14" s="10">
+      <c r="R14" s="9">
         <v>8.1</v>
       </c>
       <c r="S14" t="s">
         <v>452</v>
       </c>
-      <c r="T14" s="10">
+      <c r="T14" s="9">
         <v>164</v>
       </c>
-      <c r="U14" s="16" t="s">
+      <c r="U14" s="15" t="s">
         <v>154</v>
       </c>
-      <c r="V14" s="16"/>
-      <c r="X14" s="10"/>
+      <c r="V14" s="15"/>
+      <c r="X14" s="9"/>
       <c r="Y14" t="s">
-        <v>337</v>
-      </c>
-      <c r="Z14" s="10">
-        <v>166</v>
+        <v>347</v>
+      </c>
+      <c r="Z14" s="9">
+        <v>155</v>
       </c>
       <c r="AA14" t="s">
         <v>74</v>
       </c>
-      <c r="AB14" s="10">
+      <c r="AB14" s="9">
         <v>160</v>
       </c>
       <c r="AC14" t="s">
         <v>516</v>
       </c>
-      <c r="AD14" s="10">
+      <c r="AD14" s="9">
         <v>13.625</v>
       </c>
       <c r="AE14" t="s">
         <v>273</v>
       </c>
-      <c r="AF14" s="10">
+      <c r="AF14" s="9">
         <v>17</v>
       </c>
-      <c r="AG14" s="16" t="s">
+      <c r="AG14" s="15" t="s">
         <v>195</v>
       </c>
-      <c r="AH14" s="17"/>
+      <c r="AH14" s="16"/>
       <c r="AI14" t="s">
         <v>504</v>
       </c>
-      <c r="AJ14" s="10">
+      <c r="AJ14" s="9">
         <v>145</v>
+      </c>
+      <c r="AK14" s="17" t="s">
+        <v>556</v>
+      </c>
+      <c r="AL14" s="10">
+        <v>215</v>
+      </c>
+      <c r="AM14">
+        <v>2.8</v>
       </c>
     </row>
     <row r="15" spans="2:45" x14ac:dyDescent="0.2">
@@ -3566,89 +3880,98 @@
       <c r="E15" t="s">
         <v>350</v>
       </c>
-      <c r="F15" s="11">
+      <c r="F15" s="10">
         <v>7.85</v>
       </c>
       <c r="G15" t="s">
         <v>522</v>
       </c>
-      <c r="H15" s="10">
+      <c r="H15" s="9">
         <v>241.2</v>
       </c>
       <c r="I15" t="s">
         <v>215</v>
       </c>
-      <c r="J15" s="10">
+      <c r="J15" s="9">
         <v>216.56299999999999</v>
       </c>
       <c r="K15" t="s">
         <v>374</v>
       </c>
-      <c r="L15" s="11">
+      <c r="L15" s="10">
         <v>114</v>
       </c>
       <c r="M15" t="s">
         <v>512</v>
       </c>
-      <c r="N15" s="11">
+      <c r="N15" s="10">
         <v>227</v>
       </c>
       <c r="O15" t="s">
         <v>64</v>
       </c>
-      <c r="P15" s="11">
+      <c r="P15" s="10">
         <v>103</v>
       </c>
       <c r="Q15" t="s">
         <v>255</v>
       </c>
-      <c r="R15" s="10">
+      <c r="R15" s="9">
         <v>6.9</v>
       </c>
       <c r="S15" t="s">
         <v>329</v>
       </c>
-      <c r="T15" s="10">
+      <c r="T15" s="9">
         <v>160</v>
       </c>
-      <c r="U15" s="16" t="s">
+      <c r="U15" s="15" t="s">
         <v>165</v>
       </c>
-      <c r="V15" s="16"/>
-      <c r="X15" s="10"/>
+      <c r="V15" s="15"/>
+      <c r="X15" s="9"/>
       <c r="Y15" t="s">
-        <v>338</v>
-      </c>
-      <c r="Z15" s="10">
-        <v>250</v>
+        <v>348</v>
+      </c>
+      <c r="Z15" s="9">
+        <v>240</v>
       </c>
       <c r="AA15" t="s">
         <v>314</v>
       </c>
-      <c r="AB15" s="10">
+      <c r="AB15" s="9">
         <v>32</v>
       </c>
       <c r="AC15" t="s">
         <v>37</v>
       </c>
-      <c r="AD15" s="10">
+      <c r="AD15" s="9">
         <v>21.117999999999999</v>
       </c>
       <c r="AE15" t="s">
         <v>285</v>
       </c>
-      <c r="AF15" s="10">
+      <c r="AF15" s="9">
         <v>15</v>
       </c>
-      <c r="AG15" s="16" t="s">
+      <c r="AG15" s="15" t="s">
         <v>182</v>
       </c>
-      <c r="AH15" s="17"/>
+      <c r="AH15" s="16"/>
       <c r="AI15" t="s">
         <v>503</v>
       </c>
-      <c r="AJ15" s="10">
+      <c r="AJ15" s="9">
         <v>154</v>
+      </c>
+      <c r="AK15" s="17" t="s">
+        <v>557</v>
+      </c>
+      <c r="AL15" s="10">
+        <v>135</v>
+      </c>
+      <c r="AM15">
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="2:45" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -3659,445 +3982,499 @@
       <c r="E16" t="s">
         <v>373</v>
       </c>
-      <c r="F16" s="11">
+      <c r="F16" s="10">
         <f>48/16</f>
         <v>3</v>
       </c>
       <c r="G16" t="s">
-        <v>523</v>
-      </c>
-      <c r="H16" s="10">
-        <v>240</v>
+        <v>604</v>
+      </c>
+      <c r="H16" s="9">
+        <v>270</v>
       </c>
       <c r="I16" t="s">
         <v>220</v>
       </c>
-      <c r="J16" s="10">
+      <c r="J16" s="9">
         <v>112</v>
       </c>
       <c r="K16" t="s">
         <v>417</v>
       </c>
-      <c r="L16" s="11">
+      <c r="L16" s="10">
         <v>119</v>
       </c>
       <c r="M16" t="s">
         <v>135</v>
       </c>
-      <c r="N16" s="11">
+      <c r="N16" s="10">
         <v>145</v>
       </c>
       <c r="O16" t="s">
         <v>76</v>
       </c>
-      <c r="P16" s="11">
+      <c r="P16" s="10">
         <v>85</v>
       </c>
       <c r="Q16" t="s">
         <v>235</v>
       </c>
-      <c r="R16" s="10">
+      <c r="R16" s="9">
         <v>7.8</v>
       </c>
       <c r="S16" t="s">
         <v>453</v>
       </c>
-      <c r="T16" s="10">
+      <c r="T16" s="9">
         <v>184</v>
       </c>
-      <c r="U16" s="16" t="s">
+      <c r="U16" s="15" t="s">
         <v>155</v>
       </c>
-      <c r="V16" s="16"/>
+      <c r="V16" s="15"/>
       <c r="Y16" t="s">
-        <v>525</v>
-      </c>
-      <c r="Z16" s="10" t="s">
-        <v>526</v>
+        <v>114</v>
+      </c>
+      <c r="Z16" s="9">
+        <v>80</v>
       </c>
       <c r="AA16" t="s">
         <v>309</v>
       </c>
-      <c r="AB16" s="10">
+      <c r="AB16" s="9">
         <v>134</v>
       </c>
       <c r="AC16" t="s">
         <v>319</v>
       </c>
-      <c r="AD16" s="10">
+      <c r="AD16" s="9">
         <v>14</v>
       </c>
       <c r="AE16" t="s">
         <v>365</v>
       </c>
-      <c r="AF16" s="10">
+      <c r="AF16" s="9">
         <v>15</v>
       </c>
-      <c r="AG16" s="16" t="s">
+      <c r="AG16" s="15" t="s">
         <v>169</v>
       </c>
-      <c r="AH16" s="17"/>
+      <c r="AH16" s="16"/>
       <c r="AI16" t="s">
         <v>93</v>
       </c>
-      <c r="AJ16" s="10">
+      <c r="AJ16" s="9">
         <v>119</v>
       </c>
-    </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK16" s="17" t="s">
+        <v>596</v>
+      </c>
+      <c r="AL16" s="10">
+        <v>220</v>
+      </c>
+      <c r="AM16">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:39" x14ac:dyDescent="0.2">
       <c r="E17" t="s">
         <v>358</v>
       </c>
-      <c r="F17" s="11">
+      <c r="F17" s="10">
         <f>128/16</f>
         <v>8</v>
       </c>
       <c r="G17" t="s">
-        <v>524</v>
-      </c>
-      <c r="H17" s="10">
-        <v>243</v>
+        <v>523</v>
+      </c>
+      <c r="H17" s="9">
+        <v>240</v>
       </c>
       <c r="I17" t="s">
         <v>226</v>
       </c>
-      <c r="J17" s="10">
+      <c r="J17" s="9">
         <v>238.4</v>
       </c>
       <c r="K17" t="s">
         <v>26</v>
       </c>
-      <c r="L17" s="11">
+      <c r="L17" s="10">
         <v>104</v>
       </c>
       <c r="M17" t="s">
         <v>403</v>
       </c>
-      <c r="N17" s="11">
+      <c r="N17" s="10">
         <v>230</v>
       </c>
       <c r="O17" t="s">
         <v>58</v>
       </c>
-      <c r="P17" s="11">
+      <c r="P17" s="10">
         <v>81</v>
       </c>
       <c r="Q17" t="s">
         <v>236</v>
       </c>
-      <c r="R17" s="10">
+      <c r="R17" s="9">
         <v>6.5</v>
       </c>
       <c r="S17" t="s">
         <v>454</v>
       </c>
-      <c r="T17" s="10">
+      <c r="T17" s="9">
         <v>177</v>
       </c>
-      <c r="U17" s="16" t="s">
+      <c r="U17" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="V17" s="16"/>
-      <c r="X17" s="10"/>
+      <c r="V17" s="15"/>
+      <c r="X17" s="9"/>
       <c r="Y17" t="s">
-        <v>342</v>
-      </c>
-      <c r="Z17" s="10">
-        <v>80</v>
+        <v>339</v>
+      </c>
+      <c r="Z17" s="9">
+        <v>257.60000000000002</v>
       </c>
       <c r="AA17" t="s">
         <v>323</v>
       </c>
-      <c r="AB17" s="10">
+      <c r="AB17" s="9">
         <v>120</v>
       </c>
       <c r="AC17" t="s">
         <v>50</v>
       </c>
-      <c r="AD17" s="10">
+      <c r="AD17" s="9">
         <v>20.7</v>
       </c>
       <c r="AE17" t="s">
         <v>275</v>
       </c>
-      <c r="AF17" s="10">
+      <c r="AF17" s="9">
         <v>13.8</v>
       </c>
-      <c r="AG17" s="16" t="s">
+      <c r="AG17" s="15" t="s">
         <v>187</v>
       </c>
-      <c r="AH17" s="17"/>
+      <c r="AH17" s="16"/>
       <c r="AI17" t="s">
         <v>113</v>
       </c>
-      <c r="AJ17" s="10">
+      <c r="AJ17" s="9">
         <v>154</v>
       </c>
-    </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK17" s="17" t="s">
+        <v>597</v>
+      </c>
+      <c r="AL17" s="10">
+        <v>145</v>
+      </c>
+      <c r="AM17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:39" x14ac:dyDescent="0.2">
       <c r="E18" t="s">
         <v>351</v>
       </c>
-      <c r="F18" s="11">
+      <c r="F18" s="10">
         <f>48/16</f>
         <v>3</v>
       </c>
       <c r="G18" t="s">
-        <v>55</v>
-      </c>
-      <c r="H18" s="11">
-        <v>306</v>
+        <v>524</v>
+      </c>
+      <c r="H18" s="9">
+        <v>243</v>
       </c>
       <c r="I18" t="s">
         <v>210</v>
       </c>
-      <c r="J18" s="10">
+      <c r="J18" s="9">
         <v>248</v>
       </c>
       <c r="K18" t="s">
         <v>27</v>
       </c>
-      <c r="L18" s="11">
+      <c r="L18" s="10">
         <v>105</v>
       </c>
       <c r="M18" t="s">
         <v>267</v>
       </c>
-      <c r="N18" s="11">
+      <c r="N18" s="10">
         <v>92</v>
       </c>
       <c r="O18" t="s">
         <v>66</v>
       </c>
-      <c r="P18" s="11">
+      <c r="P18" s="10">
         <v>163</v>
       </c>
       <c r="Q18" t="s">
         <v>234</v>
       </c>
-      <c r="R18" s="10">
+      <c r="R18" s="9">
         <v>5</v>
       </c>
       <c r="S18" t="s">
         <v>456</v>
       </c>
-      <c r="T18" s="10">
+      <c r="T18" s="9">
         <v>195</v>
       </c>
-      <c r="U18" s="16" t="s">
+      <c r="U18" s="15" t="s">
         <v>153</v>
       </c>
-      <c r="V18" s="16"/>
-      <c r="X18" s="10"/>
+      <c r="V18" s="15"/>
+      <c r="X18" s="9"/>
       <c r="Y18" t="s">
-        <v>346</v>
-      </c>
-      <c r="Z18" s="10" t="s">
-        <v>464</v>
+        <v>337</v>
+      </c>
+      <c r="Z18" s="9">
+        <v>166</v>
       </c>
       <c r="AA18" t="s">
         <v>530</v>
       </c>
-      <c r="AB18" s="10">
+      <c r="AB18" s="9">
         <v>256</v>
       </c>
       <c r="AC18" t="s">
         <v>38</v>
       </c>
-      <c r="AD18" s="10">
+      <c r="AD18" s="9">
         <v>19.667999999999999</v>
       </c>
       <c r="AE18" t="s">
         <v>292</v>
       </c>
-      <c r="AF18" s="10">
+      <c r="AF18" s="9">
         <v>15</v>
       </c>
-      <c r="AG18" s="16" t="s">
+      <c r="AG18" s="15" t="s">
         <v>171</v>
       </c>
-      <c r="AH18" s="17"/>
+      <c r="AH18" s="16"/>
       <c r="AI18" t="s">
         <v>105</v>
       </c>
-      <c r="AJ18" s="10">
+      <c r="AJ18" s="9">
         <v>82</v>
       </c>
-    </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK18" s="17" t="s">
+        <v>558</v>
+      </c>
+      <c r="AL18" s="10">
+        <v>230</v>
+      </c>
+      <c r="AM18">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:39" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>517</v>
       </c>
       <c r="E19" t="s">
         <v>376</v>
       </c>
-      <c r="F19" s="11">
+      <c r="F19" s="10">
         <v>7.5</v>
       </c>
       <c r="G19" t="s">
-        <v>32</v>
-      </c>
-      <c r="H19" s="11" t="s">
-        <v>389</v>
+        <v>55</v>
+      </c>
+      <c r="H19" s="10">
+        <v>306</v>
       </c>
       <c r="I19" t="s">
         <v>218</v>
       </c>
-      <c r="J19" s="10">
+      <c r="J19" s="9">
         <v>134</v>
       </c>
       <c r="K19" t="s">
         <v>366</v>
       </c>
-      <c r="L19" s="11">
+      <c r="L19" s="10">
         <v>116</v>
       </c>
       <c r="M19" t="s">
         <v>404</v>
       </c>
-      <c r="N19" s="11">
+      <c r="N19" s="10">
         <v>165</v>
       </c>
       <c r="O19" t="s">
         <v>60</v>
       </c>
-      <c r="P19" s="11">
+      <c r="P19" s="10">
         <v>170</v>
       </c>
       <c r="Q19" t="s">
         <v>231</v>
       </c>
-      <c r="R19" s="10">
+      <c r="R19" s="9">
         <v>6</v>
       </c>
       <c r="S19" t="s">
         <v>455</v>
       </c>
-      <c r="T19" s="10">
+      <c r="T19" s="9">
         <v>198</v>
       </c>
-      <c r="U19" s="16" t="s">
+      <c r="U19" s="15" t="s">
         <v>269</v>
       </c>
-      <c r="V19" s="16"/>
-      <c r="X19" s="10"/>
+      <c r="V19" s="15"/>
+      <c r="X19" s="9"/>
+      <c r="Y19" t="s">
+        <v>338</v>
+      </c>
+      <c r="Z19" s="9">
+        <v>250</v>
+      </c>
       <c r="AA19" t="s">
         <v>310</v>
       </c>
-      <c r="AB19" s="10">
+      <c r="AB19" s="9">
         <v>146</v>
       </c>
       <c r="AC19" t="s">
         <v>480</v>
       </c>
-      <c r="AD19" s="10">
+      <c r="AD19" s="9">
         <v>14</v>
       </c>
       <c r="AE19" t="s">
         <v>274</v>
       </c>
-      <c r="AF19" s="10">
+      <c r="AF19" s="9">
         <v>15</v>
       </c>
-      <c r="AG19" s="16" t="s">
+      <c r="AG19" s="15" t="s">
         <v>180</v>
       </c>
-      <c r="AH19" s="17"/>
+      <c r="AH19" s="16"/>
       <c r="AI19" t="s">
         <v>487</v>
       </c>
-      <c r="AJ19" s="10">
+      <c r="AJ19" s="9">
         <v>87</v>
       </c>
-    </row>
-    <row r="20" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK19" s="17" t="s">
+        <v>559</v>
+      </c>
+      <c r="AL19" s="10">
+        <v>150</v>
+      </c>
+      <c r="AM19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:39" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>518</v>
       </c>
       <c r="E20" t="s">
-        <v>377</v>
-      </c>
-      <c r="F20" s="11">
-        <v>12</v>
+        <v>603</v>
+      </c>
+      <c r="F20" s="10">
+        <v>14.4</v>
       </c>
       <c r="G20" t="s">
-        <v>513</v>
-      </c>
-      <c r="H20" s="10">
-        <v>236.58799999999999</v>
+        <v>32</v>
+      </c>
+      <c r="H20" s="10" t="s">
+        <v>389</v>
       </c>
       <c r="I20" t="s">
         <v>212</v>
       </c>
-      <c r="J20" s="10">
+      <c r="J20" s="9">
         <v>240</v>
       </c>
       <c r="K20" t="s">
         <v>45</v>
       </c>
-      <c r="L20" s="11">
+      <c r="L20" s="10">
         <v>170</v>
       </c>
       <c r="M20" t="s">
         <v>397</v>
       </c>
-      <c r="N20" s="11">
+      <c r="N20" s="10">
         <v>170</v>
       </c>
       <c r="O20" t="s">
         <v>79</v>
       </c>
-      <c r="P20" s="11">
+      <c r="P20" s="10">
         <v>140</v>
       </c>
       <c r="Q20" t="s">
         <v>262</v>
       </c>
-      <c r="R20" s="10">
+      <c r="R20" s="9">
         <v>0.375</v>
       </c>
       <c r="S20" t="s">
         <v>458</v>
       </c>
-      <c r="T20" s="10">
+      <c r="T20" s="9">
         <v>178</v>
       </c>
-      <c r="U20" s="16" t="s">
+      <c r="U20" s="15" t="s">
         <v>158</v>
       </c>
-      <c r="V20" s="16"/>
-      <c r="X20" s="10"/>
+      <c r="V20" s="15"/>
+      <c r="X20" s="9"/>
+      <c r="Y20" t="s">
+        <v>525</v>
+      </c>
+      <c r="Z20" s="9" t="s">
+        <v>526</v>
+      </c>
       <c r="AA20" t="s">
         <v>470</v>
       </c>
-      <c r="AB20" s="10">
+      <c r="AB20" s="9">
         <v>180</v>
       </c>
       <c r="AC20" t="s">
         <v>39</v>
       </c>
-      <c r="AD20" s="10">
+      <c r="AD20" s="9">
         <f>337/16</f>
         <v>21.0625</v>
       </c>
       <c r="AE20" t="s">
-        <v>289</v>
-      </c>
-      <c r="AF20" s="10">
-        <v>18</v>
-      </c>
-      <c r="AG20" s="16" t="s">
+        <v>612</v>
+      </c>
+      <c r="AF20" s="9">
+        <v>15</v>
+      </c>
+      <c r="AG20" s="15" t="s">
         <v>174</v>
       </c>
-      <c r="AH20" s="17"/>
+      <c r="AH20" s="16"/>
       <c r="AI20" t="s">
         <v>84</v>
       </c>
-      <c r="AJ20" s="10">
+      <c r="AJ20" s="9">
         <v>136</v>
       </c>
-    </row>
-    <row r="21" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK20" s="17" t="s">
+        <v>560</v>
+      </c>
+      <c r="AL20" s="10">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="21" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>544</v>
       </c>
@@ -4109,83 +4486,100 @@
         <v>20</v>
       </c>
       <c r="E21" t="s">
-        <v>375</v>
-      </c>
-      <c r="F21" s="11">
-        <v>18.25</v>
+        <v>377</v>
+      </c>
+      <c r="F21" s="10">
+        <v>12</v>
+      </c>
+      <c r="G21" t="s">
+        <v>513</v>
+      </c>
+      <c r="H21" s="9">
+        <v>236.58799999999999</v>
       </c>
       <c r="I21" t="s">
         <v>198</v>
       </c>
-      <c r="J21" s="10">
+      <c r="J21" s="9">
         <v>244</v>
       </c>
       <c r="K21" t="s">
         <v>472</v>
       </c>
-      <c r="L21" s="11">
+      <c r="L21" s="10">
         <v>106</v>
       </c>
       <c r="M21" t="s">
         <v>266</v>
       </c>
-      <c r="N21" s="11">
+      <c r="N21" s="10">
         <v>177</v>
       </c>
       <c r="O21" t="s">
         <v>82</v>
       </c>
-      <c r="P21" s="11">
+      <c r="P21" s="10">
         <v>190</v>
       </c>
       <c r="Q21" t="s">
         <v>246</v>
       </c>
-      <c r="R21" s="10">
+      <c r="R21" s="9">
         <v>6.3</v>
       </c>
       <c r="S21" t="s">
         <v>457</v>
       </c>
-      <c r="T21" s="10">
+      <c r="T21" s="9">
         <v>188</v>
       </c>
-      <c r="U21" s="16" t="s">
+      <c r="U21" s="15" t="s">
         <v>141</v>
       </c>
-      <c r="V21" s="16"/>
-      <c r="X21" s="10"/>
+      <c r="V21" s="15"/>
+      <c r="X21" s="9"/>
+      <c r="Y21" t="s">
+        <v>342</v>
+      </c>
+      <c r="Z21" s="9">
+        <v>80</v>
+      </c>
       <c r="AA21" t="s">
         <v>324</v>
       </c>
-      <c r="AB21" s="10">
+      <c r="AB21" s="9">
         <v>144</v>
       </c>
       <c r="AC21" t="s">
         <v>121</v>
       </c>
-      <c r="AD21" s="10">
+      <c r="AD21" s="9">
         <v>13.5</v>
       </c>
       <c r="AE21" t="s">
-        <v>291</v>
-      </c>
-      <c r="AF21" s="10">
-        <f>244/16</f>
-        <v>15.25</v>
-      </c>
-      <c r="AG21" s="16" t="s">
+        <v>289</v>
+      </c>
+      <c r="AF21" s="9">
+        <v>18</v>
+      </c>
+      <c r="AG21" s="15" t="s">
         <v>184</v>
       </c>
-      <c r="AH21" s="17"/>
+      <c r="AH21" s="16"/>
       <c r="AI21" t="s">
         <v>96</v>
       </c>
-      <c r="AJ21" s="10">
+      <c r="AJ21" s="9">
         <v>100</v>
       </c>
-    </row>
-    <row r="22" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK21" s="17" t="s">
+        <v>561</v>
+      </c>
+      <c r="AL21" s="10">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="22" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>545</v>
       </c>
@@ -4194,82 +4588,95 @@
         <v>65</v>
       </c>
       <c r="E22" t="s">
-        <v>354</v>
-      </c>
-      <c r="F22" s="11" t="s">
-        <v>381</v>
+        <v>602</v>
+      </c>
+      <c r="F22" s="9">
+        <v>16</v>
       </c>
       <c r="I22" t="s">
         <v>196</v>
       </c>
-      <c r="J22" s="10">
+      <c r="J22" s="9">
         <v>244</v>
       </c>
       <c r="K22" t="s">
         <v>395</v>
       </c>
-      <c r="L22" s="11">
+      <c r="L22" s="10">
         <v>137</v>
       </c>
       <c r="M22" t="s">
         <v>399</v>
       </c>
-      <c r="N22" s="11">
+      <c r="N22" s="10">
         <v>212</v>
       </c>
       <c r="O22" t="s">
         <v>57</v>
       </c>
-      <c r="P22" s="11">
+      <c r="P22" s="10">
         <v>185</v>
       </c>
       <c r="Q22" t="s">
         <v>261</v>
       </c>
-      <c r="R22" s="10">
+      <c r="R22" s="9">
         <v>6.6</v>
       </c>
       <c r="S22" t="s">
         <v>330</v>
       </c>
-      <c r="T22" s="10">
+      <c r="T22" s="9">
         <v>207</v>
       </c>
-      <c r="U22" s="16" t="s">
+      <c r="U22" s="15" t="s">
         <v>163</v>
       </c>
-      <c r="V22" s="16"/>
-      <c r="X22" s="10"/>
+      <c r="V22" s="15"/>
+      <c r="X22" s="9"/>
+      <c r="Y22" t="s">
+        <v>346</v>
+      </c>
+      <c r="Z22" s="9" t="s">
+        <v>464</v>
+      </c>
       <c r="AA22" t="s">
         <v>307</v>
       </c>
-      <c r="AB22" s="10">
+      <c r="AB22" s="9">
         <v>99</v>
       </c>
       <c r="AC22" t="s">
         <v>484</v>
       </c>
-      <c r="AD22" s="10">
+      <c r="AD22" s="9">
         <v>13.5</v>
       </c>
       <c r="AE22" t="s">
-        <v>283</v>
-      </c>
-      <c r="AF22" s="10">
-        <v>15</v>
-      </c>
-      <c r="AG22" s="16" t="s">
+        <v>291</v>
+      </c>
+      <c r="AF22" s="9">
+        <f>244/16</f>
+        <v>15.25</v>
+      </c>
+      <c r="AG22" s="15" t="s">
         <v>167</v>
       </c>
-      <c r="AH22" s="17"/>
+      <c r="AH22" s="16"/>
       <c r="AI22" t="s">
         <v>108</v>
       </c>
-      <c r="AJ22" s="10">
+      <c r="AJ22" s="9">
         <v>130</v>
       </c>
-    </row>
-    <row r="23" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK22" s="17" t="s">
+        <v>562</v>
+      </c>
+      <c r="AL22" s="10">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="23" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>546</v>
       </c>
@@ -4278,1277 +4685,1551 @@
         <v>455</v>
       </c>
       <c r="E23" t="s">
-        <v>357</v>
-      </c>
-      <c r="F23" s="11" t="s">
-        <v>382</v>
+        <v>375</v>
+      </c>
+      <c r="F23" s="10">
+        <v>18.25</v>
       </c>
       <c r="I23" t="s">
         <v>197</v>
       </c>
-      <c r="J23" s="10">
+      <c r="J23" s="9">
         <v>244</v>
       </c>
       <c r="K23" t="s">
         <v>394</v>
       </c>
-      <c r="L23" s="11">
+      <c r="L23" s="10">
         <v>155</v>
       </c>
       <c r="M23" t="s">
         <v>268</v>
       </c>
-      <c r="N23" s="11">
+      <c r="N23" s="10">
         <v>180</v>
       </c>
       <c r="O23" t="s">
         <v>81</v>
       </c>
-      <c r="P23" s="11">
+      <c r="P23" s="10">
         <v>160</v>
       </c>
       <c r="Q23" t="s">
         <v>423</v>
       </c>
-      <c r="R23" s="10">
+      <c r="R23" s="9">
         <v>3.1</v>
       </c>
       <c r="S23" t="s">
         <v>442</v>
       </c>
-      <c r="T23" s="10">
+      <c r="T23" s="9">
         <v>104</v>
       </c>
-      <c r="U23" s="16" t="s">
+      <c r="U23" s="15" t="s">
         <v>164</v>
       </c>
-      <c r="V23" s="16"/>
-      <c r="X23" s="10"/>
+      <c r="V23" s="15"/>
+      <c r="X23" s="9"/>
       <c r="AA23" t="s">
         <v>325</v>
       </c>
-      <c r="AB23" s="10">
+      <c r="AB23" s="9">
         <v>109</v>
       </c>
       <c r="AC23" t="s">
         <v>317</v>
       </c>
-      <c r="AD23" s="10">
+      <c r="AD23" s="9">
         <f>237/16</f>
         <v>14.8125</v>
       </c>
       <c r="AE23" t="s">
-        <v>288</v>
-      </c>
-      <c r="AF23" s="10">
+        <v>283</v>
+      </c>
+      <c r="AF23" s="9">
         <v>15</v>
       </c>
-      <c r="AG23" s="16" t="s">
+      <c r="AG23" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="AH23" s="17"/>
+      <c r="AH23" s="16"/>
       <c r="AI23" t="s">
         <v>103</v>
       </c>
-      <c r="AJ23" s="10">
+      <c r="AJ23" s="9">
         <v>21</v>
       </c>
-    </row>
-    <row r="24" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK23" s="17" t="s">
+        <v>563</v>
+      </c>
+      <c r="AL23" s="10">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="24" spans="1:39" x14ac:dyDescent="0.2">
       <c r="E24" t="s">
-        <v>356</v>
-      </c>
-      <c r="F24" s="11" t="s">
-        <v>383</v>
+        <v>354</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>381</v>
       </c>
       <c r="I24" t="s">
         <v>219</v>
       </c>
-      <c r="J24" s="10">
+      <c r="J24" s="9">
         <v>113</v>
       </c>
       <c r="K24" t="s">
         <v>367</v>
       </c>
-      <c r="L24" s="11">
+      <c r="L24" s="10">
         <v>108</v>
       </c>
       <c r="M24" t="s">
         <v>405</v>
       </c>
-      <c r="N24" s="11">
+      <c r="N24" s="10">
         <v>190</v>
       </c>
       <c r="O24" t="s">
         <v>62</v>
       </c>
-      <c r="P24" s="11">
+      <c r="P24" s="10">
         <v>169</v>
       </c>
       <c r="Q24" t="s">
         <v>106</v>
       </c>
-      <c r="R24" s="10">
+      <c r="R24" s="9">
         <v>5.8</v>
       </c>
       <c r="S24" t="s">
         <v>328</v>
       </c>
-      <c r="T24" s="10">
+      <c r="T24" s="9">
         <v>208</v>
       </c>
-      <c r="U24" s="16" t="s">
+      <c r="U24" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="V24" s="16"/>
-      <c r="X24" s="10"/>
+      <c r="V24" s="15"/>
+      <c r="X24" s="9"/>
       <c r="AA24" t="s">
         <v>313</v>
       </c>
-      <c r="AB24" s="10">
+      <c r="AB24" s="9">
         <v>135</v>
       </c>
       <c r="AC24" t="s">
         <v>471</v>
       </c>
-      <c r="AD24" s="10">
+      <c r="AD24" s="9">
         <v>13.53</v>
       </c>
       <c r="AE24" t="s">
-        <v>287</v>
-      </c>
-      <c r="AF24" s="10">
-        <v>18</v>
-      </c>
-      <c r="AG24" s="16" t="s">
+        <v>288</v>
+      </c>
+      <c r="AF24" s="9">
+        <v>15</v>
+      </c>
+      <c r="AG24" s="15" t="s">
         <v>175</v>
       </c>
-      <c r="AH24" s="17"/>
+      <c r="AH24" s="16"/>
       <c r="AI24" t="s">
         <v>110</v>
       </c>
-      <c r="AJ24" s="10">
+      <c r="AJ24" s="9">
         <v>135</v>
       </c>
-    </row>
-    <row r="25" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK24" s="17" t="s">
+        <v>564</v>
+      </c>
+      <c r="AL24" s="10">
+        <v>240</v>
+      </c>
+      <c r="AM24">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:39" x14ac:dyDescent="0.2">
       <c r="E25" t="s">
-        <v>353</v>
-      </c>
-      <c r="F25" s="11" t="s">
-        <v>384</v>
+        <v>357</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>382</v>
       </c>
       <c r="I25" t="s">
         <v>204</v>
       </c>
-      <c r="J25" s="10">
+      <c r="J25" s="9">
         <v>113</v>
       </c>
       <c r="K25" t="s">
         <v>28</v>
       </c>
-      <c r="L25" s="11">
+      <c r="L25" s="10">
         <v>125</v>
       </c>
       <c r="M25" t="s">
         <v>415</v>
       </c>
-      <c r="N25" s="11">
+      <c r="N25" s="10">
         <v>165</v>
       </c>
       <c r="O25" t="s">
         <v>69</v>
       </c>
-      <c r="P25" s="11">
+      <c r="P25" s="10">
         <v>174</v>
       </c>
       <c r="Q25" t="s">
         <v>251</v>
       </c>
-      <c r="R25" s="10">
+      <c r="R25" s="9">
         <v>11.1</v>
       </c>
       <c r="S25" t="s">
         <v>459</v>
       </c>
-      <c r="T25" s="10">
+      <c r="T25" s="9">
         <v>193</v>
       </c>
-      <c r="U25" s="16" t="s">
+      <c r="U25" s="15" t="s">
         <v>160</v>
       </c>
-      <c r="V25" s="16"/>
-      <c r="X25" s="10"/>
+      <c r="V25" s="15"/>
+      <c r="X25" s="9"/>
       <c r="AA25" t="s">
         <v>304</v>
       </c>
-      <c r="AB25" s="10">
+      <c r="AB25" s="9">
         <v>123</v>
       </c>
       <c r="AC25" t="s">
         <v>483</v>
       </c>
-      <c r="AD25" s="10">
+      <c r="AD25" s="9">
         <v>13.625</v>
       </c>
       <c r="AE25" t="s">
-        <v>299</v>
-      </c>
-      <c r="AF25" s="10">
-        <v>15</v>
-      </c>
-      <c r="AG25" s="16" t="s">
+        <v>287</v>
+      </c>
+      <c r="AF25" s="9">
+        <v>18</v>
+      </c>
+      <c r="AG25" s="15" t="s">
         <v>181</v>
       </c>
-      <c r="AH25" s="17"/>
+      <c r="AH25" s="16"/>
       <c r="AI25" t="s">
         <v>100</v>
       </c>
-      <c r="AJ25" s="10">
+      <c r="AJ25" s="9">
         <v>89</v>
       </c>
-    </row>
-    <row r="26" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK25" s="17" t="s">
+        <v>565</v>
+      </c>
+      <c r="AL25" s="10">
+        <v>160</v>
+      </c>
+      <c r="AM25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:39" x14ac:dyDescent="0.2">
       <c r="E26" t="s">
-        <v>364</v>
-      </c>
-      <c r="F26" s="11" t="s">
-        <v>380</v>
+        <v>356</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>383</v>
       </c>
       <c r="I26" t="s">
         <v>506</v>
       </c>
-      <c r="J26" s="10">
+      <c r="J26" s="9">
         <v>240</v>
       </c>
       <c r="K26" t="s">
         <v>29</v>
       </c>
-      <c r="L26" s="11">
+      <c r="L26" s="10">
         <v>167</v>
       </c>
       <c r="M26" t="s">
         <v>137</v>
       </c>
-      <c r="N26" s="11">
+      <c r="N26" s="10">
         <v>196</v>
       </c>
       <c r="O26" t="s">
         <v>70</v>
       </c>
-      <c r="P26" s="11">
+      <c r="P26" s="10">
         <v>193</v>
       </c>
       <c r="Q26" t="s">
         <v>498</v>
       </c>
-      <c r="R26" s="10">
+      <c r="R26" s="9">
         <v>9.6999999999999993</v>
       </c>
       <c r="S26" t="s">
         <v>460</v>
       </c>
-      <c r="T26" s="10">
+      <c r="T26" s="9">
         <v>171</v>
       </c>
-      <c r="U26" s="16" t="s">
+      <c r="U26" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="V26" s="16"/>
-      <c r="X26" s="10"/>
+      <c r="V26" s="15"/>
+      <c r="X26" s="9"/>
       <c r="AA26" t="s">
         <v>326</v>
       </c>
-      <c r="AB26" s="10">
+      <c r="AB26" s="9">
         <v>133</v>
       </c>
       <c r="AC26" t="s">
         <v>40</v>
       </c>
-      <c r="AD26" s="10">
+      <c r="AD26" s="9">
         <v>13.625</v>
       </c>
       <c r="AE26" t="s">
-        <v>116</v>
-      </c>
-      <c r="AF26" s="10">
-        <v>16</v>
-      </c>
-      <c r="AG26" s="16" t="s">
+        <v>299</v>
+      </c>
+      <c r="AF26" s="9">
+        <v>15</v>
+      </c>
+      <c r="AG26" s="15" t="s">
         <v>186</v>
       </c>
-      <c r="AH26" s="17"/>
+      <c r="AH26" s="16"/>
       <c r="AI26" t="s">
         <v>489</v>
       </c>
-      <c r="AJ26" s="10">
+      <c r="AJ26" s="9">
         <v>55</v>
       </c>
-    </row>
-    <row r="27" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK26" s="17" t="s">
+        <v>566</v>
+      </c>
+      <c r="AL26" s="10">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="27" spans="1:39" x14ac:dyDescent="0.2">
       <c r="E27" t="s">
-        <v>355</v>
-      </c>
-      <c r="F27" s="11" t="s">
-        <v>383</v>
+        <v>353</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>384</v>
       </c>
       <c r="I27" t="s">
         <v>214</v>
       </c>
-      <c r="J27" s="10">
+      <c r="J27" s="9">
         <v>122</v>
       </c>
       <c r="K27" t="s">
         <v>47</v>
       </c>
-      <c r="L27" s="11">
+      <c r="L27" s="10">
         <v>121</v>
       </c>
       <c r="M27" t="s">
         <v>134</v>
       </c>
-      <c r="N27" s="11">
+      <c r="N27" s="10">
         <v>140</v>
       </c>
       <c r="O27" t="s">
         <v>61</v>
       </c>
-      <c r="P27" s="11">
+      <c r="P27" s="10">
         <v>192</v>
       </c>
       <c r="Q27" t="s">
         <v>508</v>
       </c>
-      <c r="R27" s="10">
+      <c r="R27" s="9">
         <f>149/16</f>
         <v>9.3125</v>
       </c>
       <c r="S27" t="s">
         <v>336</v>
       </c>
-      <c r="T27" s="10">
+      <c r="T27" s="9">
         <v>150</v>
       </c>
-      <c r="U27" s="16" t="s">
+      <c r="U27" s="15" t="s">
         <v>166</v>
       </c>
-      <c r="V27" s="16"/>
-      <c r="X27" s="10"/>
+      <c r="V27" s="15"/>
+      <c r="X27" s="9"/>
       <c r="AA27" t="s">
         <v>34</v>
       </c>
-      <c r="AB27" s="10">
+      <c r="AB27" s="9">
         <v>140.80000000000001</v>
       </c>
       <c r="AC27" t="s">
         <v>120</v>
       </c>
-      <c r="AD27" s="10">
+      <c r="AD27" s="9">
         <v>13.5</v>
       </c>
       <c r="AE27" t="s">
+        <v>116</v>
+      </c>
+      <c r="AF27" s="9">
+        <v>16</v>
+      </c>
+      <c r="AG27" s="15" t="s">
+        <v>362</v>
+      </c>
+      <c r="AH27" s="16"/>
+      <c r="AI27" t="s">
+        <v>491</v>
+      </c>
+      <c r="AJ27" s="9">
+        <v>57</v>
+      </c>
+      <c r="AK27" s="17" t="s">
+        <v>567</v>
+      </c>
+      <c r="AL27" s="10">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="28" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="E28" t="s">
+        <v>364</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>380</v>
+      </c>
+      <c r="I28" t="s">
+        <v>392</v>
+      </c>
+      <c r="J28" s="9">
+        <v>100</v>
+      </c>
+      <c r="K28" t="s">
+        <v>44</v>
+      </c>
+      <c r="L28" s="10">
+        <v>120</v>
+      </c>
+      <c r="M28" t="s">
+        <v>406</v>
+      </c>
+      <c r="N28" s="10">
+        <v>143</v>
+      </c>
+      <c r="O28" t="s">
+        <v>418</v>
+      </c>
+      <c r="P28" s="10">
+        <v>64</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>507</v>
+      </c>
+      <c r="R28" s="9">
+        <v>14</v>
+      </c>
+      <c r="S28" t="s">
+        <v>333</v>
+      </c>
+      <c r="T28" s="9">
+        <v>256</v>
+      </c>
+      <c r="U28" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="V28" s="15"/>
+      <c r="X28" s="9"/>
+      <c r="AA28" t="s">
+        <v>306</v>
+      </c>
+      <c r="AB28" s="9">
+        <v>122</v>
+      </c>
+      <c r="AC28" t="s">
+        <v>466</v>
+      </c>
+      <c r="AD28" s="9">
+        <v>14</v>
+      </c>
+      <c r="AE28" t="s">
         <v>279</v>
       </c>
-      <c r="AF27" s="10">
+      <c r="AF28" s="9">
         <f>6.5*3</f>
         <v>19.5</v>
       </c>
-      <c r="AG27" s="16" t="s">
-        <v>362</v>
-      </c>
-      <c r="AH27" s="17"/>
-      <c r="AI27" t="s">
-        <v>491</v>
-      </c>
-      <c r="AJ27" s="10">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="28" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="E28" t="s">
-        <v>49</v>
-      </c>
-      <c r="F28" s="11">
-        <v>6.9</v>
-      </c>
-      <c r="I28" t="s">
-        <v>392</v>
-      </c>
-      <c r="J28" s="10">
-        <v>100</v>
-      </c>
-      <c r="K28" t="s">
-        <v>44</v>
-      </c>
-      <c r="L28" s="11">
-        <v>120</v>
-      </c>
-      <c r="M28" t="s">
-        <v>406</v>
-      </c>
-      <c r="N28" s="11">
-        <v>143</v>
-      </c>
-      <c r="O28" t="s">
-        <v>418</v>
-      </c>
-      <c r="P28" s="11">
-        <v>64</v>
-      </c>
-      <c r="Q28" t="s">
-        <v>507</v>
-      </c>
-      <c r="R28" s="10">
-        <v>14</v>
-      </c>
-      <c r="S28" t="s">
-        <v>333</v>
-      </c>
-      <c r="T28" s="10">
-        <v>256</v>
-      </c>
-      <c r="U28" s="16" t="s">
-        <v>161</v>
-      </c>
-      <c r="V28" s="16"/>
-      <c r="X28" s="10"/>
-      <c r="AA28" t="s">
-        <v>306</v>
-      </c>
-      <c r="AB28" s="10">
-        <v>122</v>
-      </c>
-      <c r="AC28" t="s">
-        <v>466</v>
-      </c>
-      <c r="AD28" s="10">
-        <v>14</v>
-      </c>
-      <c r="AE28" t="s">
-        <v>290</v>
-      </c>
-      <c r="AF28" s="10">
-        <v>10</v>
-      </c>
-      <c r="AG28" s="16" t="s">
+      <c r="AG28" s="15" t="s">
         <v>188</v>
       </c>
-      <c r="AH28" s="17"/>
+      <c r="AH28" s="16"/>
       <c r="AI28" t="s">
         <v>490</v>
       </c>
-      <c r="AJ28" s="10">
+      <c r="AJ28" s="9">
         <v>35</v>
       </c>
-    </row>
-    <row r="29" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK28" s="17" t="s">
+        <v>568</v>
+      </c>
+      <c r="AL28" s="10">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="29" spans="1:39" x14ac:dyDescent="0.2">
       <c r="E29" t="s">
-        <v>31</v>
-      </c>
-      <c r="F29" s="11">
-        <v>10</v>
+        <v>355</v>
+      </c>
+      <c r="F29" s="10" t="s">
+        <v>383</v>
       </c>
       <c r="I29" t="s">
         <v>213</v>
       </c>
-      <c r="J29" s="10">
+      <c r="J29" s="9">
         <v>245.43799999999999</v>
       </c>
       <c r="K29" t="s">
         <v>46</v>
       </c>
-      <c r="L29" s="11">
+      <c r="L29" s="10">
         <v>120</v>
       </c>
       <c r="M29" t="s">
         <v>407</v>
       </c>
-      <c r="N29" s="11">
+      <c r="N29" s="10">
         <v>217</v>
       </c>
       <c r="O29" t="s">
         <v>419</v>
       </c>
-      <c r="P29" s="11">
+      <c r="P29" s="10">
         <f>28*4</f>
         <v>112</v>
       </c>
       <c r="Q29" t="s">
         <v>424</v>
       </c>
-      <c r="R29" s="10">
+      <c r="R29" s="9">
         <v>5.2</v>
       </c>
       <c r="S29" t="s">
         <v>332</v>
       </c>
-      <c r="T29" s="10">
+      <c r="T29" s="9">
         <v>197</v>
       </c>
-      <c r="U29" s="16" t="s">
+      <c r="U29" s="15" t="s">
         <v>149</v>
       </c>
-      <c r="V29" s="16"/>
-      <c r="X29" s="10"/>
+      <c r="V29" s="15"/>
+      <c r="X29" s="9"/>
       <c r="AA29" t="s">
         <v>315</v>
       </c>
-      <c r="AB29" s="10">
+      <c r="AB29" s="9">
         <f>28*4</f>
         <v>112</v>
       </c>
       <c r="AC29" t="s">
         <v>124</v>
       </c>
-      <c r="AD29" s="10">
+      <c r="AD29" s="9">
         <v>13.5</v>
       </c>
       <c r="AE29" t="s">
-        <v>278</v>
-      </c>
-      <c r="AF29" s="10">
-        <v>18</v>
-      </c>
-      <c r="AG29" s="16" t="s">
+        <v>290</v>
+      </c>
+      <c r="AF29" s="9">
+        <v>10</v>
+      </c>
+      <c r="AG29" s="15" t="s">
         <v>189</v>
       </c>
-      <c r="AH29" s="17"/>
+      <c r="AH29" s="16"/>
       <c r="AI29" t="s">
         <v>493</v>
       </c>
-      <c r="AJ29" s="10">
+      <c r="AJ29" s="9">
         <v>87</v>
       </c>
-    </row>
-    <row r="30" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK29" s="17" t="s">
+        <v>569</v>
+      </c>
+      <c r="AL29" s="10">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="30" spans="1:39" x14ac:dyDescent="0.2">
       <c r="D30">
         <v>30</v>
       </c>
-      <c r="F30" s="9"/>
+      <c r="E30" t="s">
+        <v>49</v>
+      </c>
+      <c r="F30" s="10">
+        <v>6.9</v>
+      </c>
       <c r="I30" t="s">
         <v>224</v>
       </c>
-      <c r="J30" s="10">
+      <c r="J30" s="9">
         <v>118</v>
       </c>
       <c r="K30" t="s">
         <v>30</v>
       </c>
-      <c r="L30" s="11">
+      <c r="L30" s="10">
         <v>135</v>
       </c>
       <c r="M30" t="s">
         <v>408</v>
       </c>
-      <c r="N30" s="11">
+      <c r="N30" s="10">
         <v>140</v>
       </c>
-      <c r="P30" s="11"/>
+      <c r="P30" s="10"/>
       <c r="Q30" t="s">
         <v>425</v>
       </c>
-      <c r="R30" s="10">
+      <c r="R30" s="9">
         <v>6</v>
       </c>
       <c r="S30" t="s">
         <v>335</v>
       </c>
-      <c r="T30" s="10">
+      <c r="T30" s="9">
         <v>105</v>
       </c>
-      <c r="U30" s="16" t="s">
+      <c r="U30" s="15" t="s">
         <v>144</v>
       </c>
-      <c r="V30" s="16"/>
-      <c r="X30" s="10"/>
+      <c r="V30" s="15"/>
+      <c r="X30" s="9"/>
       <c r="AA30" t="s">
         <v>35</v>
       </c>
-      <c r="AB30" s="10">
+      <c r="AB30" s="9">
         <v>128</v>
       </c>
       <c r="AC30" t="s">
         <v>122</v>
       </c>
-      <c r="AD30" s="10">
+      <c r="AD30" s="9">
         <v>13.625</v>
       </c>
       <c r="AE30" t="s">
-        <v>119</v>
-      </c>
-      <c r="AF30" s="10">
-        <v>16.5</v>
-      </c>
-      <c r="AG30" s="16" t="s">
+        <v>278</v>
+      </c>
+      <c r="AF30" s="9">
+        <v>18</v>
+      </c>
+      <c r="AG30" s="15" t="s">
         <v>179</v>
       </c>
-      <c r="AH30" s="17"/>
+      <c r="AH30" s="16"/>
       <c r="AI30" t="s">
         <v>492</v>
       </c>
-      <c r="AJ30" s="10">
+      <c r="AJ30" s="9">
         <v>54</v>
       </c>
-    </row>
-    <row r="31" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK30" s="17" t="s">
+        <v>570</v>
+      </c>
+      <c r="AL30" s="10">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="31" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="E31" t="s">
+        <v>31</v>
+      </c>
+      <c r="F31" s="10">
+        <v>10</v>
+      </c>
       <c r="I31" t="s">
         <v>223</v>
       </c>
-      <c r="J31" s="10">
+      <c r="J31" s="9">
         <v>122</v>
       </c>
       <c r="M31" t="s">
         <v>136</v>
       </c>
-      <c r="N31" s="11">
+      <c r="N31" s="10">
         <v>236</v>
       </c>
-      <c r="P31" s="11"/>
+      <c r="P31" s="10"/>
       <c r="Q31" t="s">
         <v>252</v>
       </c>
-      <c r="R31" s="10">
+      <c r="R31" s="9">
         <v>6.9</v>
       </c>
-      <c r="T31" s="10"/>
-      <c r="U31" s="16" t="s">
+      <c r="T31" s="9"/>
+      <c r="U31" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="V31" s="16"/>
-      <c r="X31" s="10"/>
+      <c r="V31" s="15"/>
+      <c r="X31" s="9"/>
       <c r="AA31" t="s">
         <v>531</v>
       </c>
-      <c r="AB31" s="10">
+      <c r="AB31" s="9">
         <v>256</v>
       </c>
       <c r="AC31" t="s">
         <v>312</v>
       </c>
-      <c r="AD31" s="10">
+      <c r="AD31" s="9">
         <v>13.625</v>
       </c>
       <c r="AE31" t="s">
-        <v>286</v>
-      </c>
-      <c r="AF31" s="10">
-        <v>15</v>
-      </c>
-      <c r="AG31" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="AF31" s="9">
+        <v>16.5</v>
+      </c>
+      <c r="AG31" s="15" t="s">
         <v>176</v>
       </c>
-      <c r="AH31" s="17"/>
+      <c r="AH31" s="16"/>
       <c r="AI31" t="s">
         <v>494</v>
       </c>
-      <c r="AJ31" s="10">
+      <c r="AJ31" s="9">
         <v>66</v>
       </c>
-    </row>
-    <row r="32" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="AK31" s="17" t="s">
+        <v>571</v>
+      </c>
+      <c r="AL31" s="10">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="32" spans="1:39" x14ac:dyDescent="0.2">
       <c r="I32" t="s">
         <v>202</v>
       </c>
-      <c r="J32" s="10">
+      <c r="J32" s="9">
         <v>227</v>
       </c>
       <c r="M32" t="s">
         <v>410</v>
       </c>
-      <c r="N32" s="11">
+      <c r="N32" s="10">
         <v>154</v>
       </c>
       <c r="Q32" t="s">
         <v>259</v>
       </c>
-      <c r="R32" s="10">
+      <c r="R32" s="9">
         <v>2.8</v>
       </c>
-      <c r="T32" s="10"/>
-      <c r="U32" s="16" t="s">
+      <c r="T32" s="9"/>
+      <c r="U32" s="15" t="s">
         <v>142</v>
       </c>
-      <c r="V32" s="16"/>
-      <c r="X32" s="10"/>
+      <c r="V32" s="15"/>
+      <c r="X32" s="9"/>
       <c r="AA32" t="s">
         <v>305</v>
       </c>
-      <c r="AB32" s="10">
+      <c r="AB32" s="9">
         <v>46</v>
       </c>
-      <c r="AD32" s="10"/>
+      <c r="AD32" s="9"/>
       <c r="AE32" t="s">
-        <v>41</v>
-      </c>
-      <c r="AF32" s="10">
-        <v>14.9</v>
-      </c>
-      <c r="AG32" s="16" t="s">
+        <v>286</v>
+      </c>
+      <c r="AF32" s="9">
+        <v>15</v>
+      </c>
+      <c r="AG32" s="15" t="s">
         <v>190</v>
       </c>
-      <c r="AH32" s="17"/>
+      <c r="AH32" s="16"/>
       <c r="AI32" t="s">
         <v>495</v>
       </c>
-      <c r="AJ32" s="10">
+      <c r="AJ32" s="9">
         <v>86</v>
       </c>
-    </row>
-    <row r="33" spans="9:36" x14ac:dyDescent="0.2">
+      <c r="AK32" t="s">
+        <v>572</v>
+      </c>
+      <c r="AL32" s="10">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="33" spans="9:39" x14ac:dyDescent="0.2">
       <c r="I33" t="s">
         <v>222</v>
       </c>
-      <c r="J33" s="10">
+      <c r="J33" s="9">
         <v>122</v>
       </c>
       <c r="M33" t="s">
         <v>409</v>
       </c>
-      <c r="N33" s="11">
+      <c r="N33" s="10">
         <v>150</v>
       </c>
       <c r="Q33" t="s">
         <v>249</v>
       </c>
-      <c r="R33" s="10">
+      <c r="R33" s="9">
         <v>6</v>
       </c>
-      <c r="T33" s="10"/>
-      <c r="U33" s="16" t="s">
+      <c r="T33" s="9"/>
+      <c r="U33" s="15" t="s">
         <v>162</v>
       </c>
-      <c r="V33" s="16"/>
+      <c r="V33" s="15"/>
       <c r="AA33" t="s">
         <v>320</v>
       </c>
-      <c r="AB33" s="10">
+      <c r="AB33" s="9">
         <v>120</v>
       </c>
-      <c r="AD33" s="10"/>
+      <c r="AD33" s="9"/>
       <c r="AE33" t="s">
-        <v>300</v>
-      </c>
-      <c r="AF33" s="10">
-        <v>14.938000000000001</v>
-      </c>
-      <c r="AG33" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="AF33" s="9">
+        <v>14.9</v>
+      </c>
+      <c r="AG33" s="15" t="s">
         <v>168</v>
       </c>
-      <c r="AH33" s="17"/>
+      <c r="AH33" s="16"/>
       <c r="AI33" t="s">
         <v>496</v>
       </c>
-      <c r="AJ33" s="10">
+      <c r="AJ33" s="9">
         <v>89</v>
       </c>
-    </row>
-    <row r="34" spans="9:36" x14ac:dyDescent="0.2">
+      <c r="AK33" t="s">
+        <v>573</v>
+      </c>
+      <c r="AL33" s="10">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="34" spans="9:39" x14ac:dyDescent="0.2">
       <c r="I34" t="s">
         <v>217</v>
       </c>
-      <c r="J34" s="10">
+      <c r="J34" s="9">
         <v>245</v>
       </c>
       <c r="M34" t="s">
         <v>412</v>
       </c>
-      <c r="N34" s="11">
+      <c r="N34" s="10">
         <v>168</v>
       </c>
       <c r="Q34" t="s">
         <v>250</v>
       </c>
-      <c r="R34" s="10">
+      <c r="R34" s="9">
         <v>6</v>
       </c>
-      <c r="T34" s="10"/>
-      <c r="U34" s="16" t="s">
+      <c r="T34" s="9"/>
+      <c r="U34" s="15" t="s">
         <v>156</v>
       </c>
-      <c r="V34" s="16"/>
+      <c r="V34" s="15"/>
       <c r="AA34" t="s">
         <v>327</v>
       </c>
-      <c r="AB34" s="10">
+      <c r="AB34" s="9">
         <v>120</v>
       </c>
-      <c r="AD34" s="10"/>
+      <c r="AD34" s="9"/>
       <c r="AE34" t="s">
-        <v>301</v>
-      </c>
-      <c r="AF34" s="10">
-        <v>15.938000000000001</v>
-      </c>
-      <c r="AH34" s="10"/>
+        <v>300</v>
+      </c>
+      <c r="AF34" s="9">
+        <v>14.938000000000001</v>
+      </c>
+      <c r="AH34" s="9"/>
       <c r="AI34" t="s">
         <v>497</v>
       </c>
-      <c r="AJ34" s="10">
+      <c r="AJ34" s="9">
         <v>96</v>
       </c>
-    </row>
-    <row r="35" spans="9:36" x14ac:dyDescent="0.2">
+      <c r="AK34" s="17" t="s">
+        <v>574</v>
+      </c>
+      <c r="AL34" s="10">
+        <v>210</v>
+      </c>
+      <c r="AM34">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="35" spans="9:39" x14ac:dyDescent="0.2">
       <c r="I35" t="s">
         <v>201</v>
       </c>
-      <c r="J35" s="10">
+      <c r="J35" s="9">
         <v>248</v>
       </c>
       <c r="M35" t="s">
         <v>411</v>
       </c>
-      <c r="N35" s="11">
+      <c r="N35" s="10">
         <v>173.25</v>
       </c>
       <c r="Q35" t="s">
         <v>247</v>
       </c>
-      <c r="R35" s="10">
+      <c r="R35" s="9">
         <v>5.2</v>
       </c>
-      <c r="T35" s="10"/>
+      <c r="T35" s="9"/>
       <c r="AA35" t="s">
         <v>440</v>
       </c>
-      <c r="AB35" s="10">
+      <c r="AB35" s="9">
         <v>62</v>
       </c>
-      <c r="AD35" s="10"/>
+      <c r="AD35" s="9"/>
       <c r="AE35" t="s">
-        <v>359</v>
-      </c>
-      <c r="AF35" s="10">
-        <v>14.938000000000001</v>
-      </c>
-      <c r="AH35" s="10"/>
+        <v>301</v>
+      </c>
+      <c r="AF35" s="9">
+        <v>15.938000000000001</v>
+      </c>
+      <c r="AH35" s="9"/>
       <c r="AI35" t="s">
         <v>104</v>
       </c>
-      <c r="AJ35" s="10">
+      <c r="AJ35" s="9">
         <v>100</v>
       </c>
-    </row>
-    <row r="36" spans="9:36" x14ac:dyDescent="0.2">
+      <c r="AK35" s="17" t="s">
+        <v>575</v>
+      </c>
+      <c r="AL35" s="10">
+        <v>160</v>
+      </c>
+      <c r="AM35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="9:39" x14ac:dyDescent="0.2">
       <c r="I36" t="s">
         <v>225</v>
       </c>
-      <c r="J36" s="10">
+      <c r="J36" s="9">
         <f>28*8</f>
         <v>224</v>
       </c>
       <c r="M36" t="s">
         <v>413</v>
       </c>
-      <c r="N36" s="11">
+      <c r="N36" s="10">
         <v>150</v>
       </c>
       <c r="Q36" t="s">
         <v>242</v>
       </c>
-      <c r="R36" s="10">
+      <c r="R36" s="9">
         <v>1.7</v>
       </c>
-      <c r="T36" s="10"/>
-      <c r="AD36" s="10"/>
+      <c r="T36" s="9"/>
+      <c r="AD36" s="9"/>
       <c r="AE36" t="s">
-        <v>363</v>
-      </c>
-      <c r="AF36" s="10">
-        <v>14.938000000000001</v>
-      </c>
-      <c r="AH36" s="10"/>
+        <v>613</v>
+      </c>
+      <c r="AF36" s="9">
+        <v>14</v>
+      </c>
+      <c r="AH36" s="9"/>
       <c r="AI36" t="s">
         <v>83</v>
       </c>
-      <c r="AJ36" s="10">
+      <c r="AJ36" s="9">
         <v>142</v>
       </c>
-    </row>
-    <row r="37" spans="9:36" x14ac:dyDescent="0.2">
+      <c r="AK36" s="17" t="s">
+        <v>576</v>
+      </c>
+      <c r="AL36" s="10">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="37" spans="9:39" x14ac:dyDescent="0.2">
       <c r="I37" t="s">
         <v>206</v>
       </c>
-      <c r="J37" s="10">
+      <c r="J37" s="9">
         <v>113</v>
       </c>
       <c r="M37" t="s">
         <v>414</v>
       </c>
-      <c r="N37" s="11">
+      <c r="N37" s="10">
         <v>174</v>
       </c>
       <c r="Q37" t="s">
         <v>265</v>
       </c>
-      <c r="R37" s="10">
+      <c r="R37" s="9">
         <v>6</v>
       </c>
-      <c r="T37" s="10"/>
-      <c r="AD37" s="10"/>
+      <c r="T37" s="9"/>
+      <c r="AD37" s="9"/>
       <c r="AE37" t="s">
-        <v>117</v>
-      </c>
-      <c r="AF37" s="10">
-        <v>17.117999999999999</v>
+        <v>359</v>
+      </c>
+      <c r="AF37" s="9">
+        <v>14.938000000000001</v>
       </c>
       <c r="AI37" t="s">
         <v>85</v>
       </c>
-      <c r="AJ37" s="10">
+      <c r="AJ37" s="9">
         <v>150</v>
       </c>
-    </row>
-    <row r="38" spans="9:36" x14ac:dyDescent="0.2">
+      <c r="AK37" s="17" t="s">
+        <v>577</v>
+      </c>
+      <c r="AL37" s="10">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="38" spans="9:39" x14ac:dyDescent="0.2">
       <c r="I38" t="s">
         <v>227</v>
       </c>
-      <c r="J38" s="10">
+      <c r="J38" s="9">
         <v>240</v>
       </c>
       <c r="M38" t="s">
         <v>132</v>
       </c>
-      <c r="N38" s="11">
+      <c r="N38" s="10">
         <v>134</v>
       </c>
       <c r="Q38" t="s">
         <v>245</v>
       </c>
-      <c r="R38" s="10">
+      <c r="R38" s="9">
         <v>6.2</v>
       </c>
-      <c r="T38" s="10"/>
-      <c r="AD38" s="10"/>
+      <c r="T38" s="9"/>
+      <c r="AD38" s="9"/>
       <c r="AE38" t="s">
-        <v>295</v>
-      </c>
-      <c r="AF38" s="10">
-        <v>18</v>
+        <v>363</v>
+      </c>
+      <c r="AF38" s="9">
+        <v>14.938000000000001</v>
       </c>
       <c r="AI38" t="s">
-        <v>97</v>
-      </c>
-      <c r="AJ38" s="10">
+        <v>600</v>
+      </c>
+      <c r="AJ38" s="9">
         <v>116</v>
       </c>
-    </row>
-    <row r="39" spans="9:36" x14ac:dyDescent="0.2">
+      <c r="AK38" s="17" t="s">
+        <v>578</v>
+      </c>
+      <c r="AL38" s="10">
+        <v>220</v>
+      </c>
+      <c r="AM38">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="39" spans="9:39" x14ac:dyDescent="0.2">
       <c r="I39" t="s">
         <v>199</v>
       </c>
-      <c r="J39" s="10">
+      <c r="J39" s="9">
         <v>245</v>
       </c>
       <c r="M39" t="s">
         <v>131</v>
       </c>
-      <c r="N39" s="11">
+      <c r="N39" s="10">
         <v>120</v>
       </c>
       <c r="Q39" t="s">
         <v>237</v>
       </c>
-      <c r="R39" s="10">
+      <c r="R39" s="9">
         <v>6.8</v>
       </c>
-      <c r="T39" s="10"/>
-      <c r="AD39" s="10"/>
-      <c r="AF39" s="10"/>
+      <c r="T39" s="9"/>
+      <c r="AD39" s="9"/>
+      <c r="AE39" t="s">
+        <v>614</v>
+      </c>
+      <c r="AF39" s="9">
+        <v>15</v>
+      </c>
       <c r="AI39" t="s">
-        <v>112</v>
-      </c>
-      <c r="AJ39" s="10">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="40" spans="9:36" x14ac:dyDescent="0.2">
+        <v>601</v>
+      </c>
+      <c r="AJ39" s="9">
+        <v>260</v>
+      </c>
+      <c r="AK39" s="17" t="s">
+        <v>579</v>
+      </c>
+      <c r="AL39" s="10">
+        <v>145</v>
+      </c>
+      <c r="AM39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="9:39" x14ac:dyDescent="0.2">
       <c r="M40" t="s">
         <v>125</v>
       </c>
-      <c r="N40" s="11">
+      <c r="N40" s="10">
         <v>152</v>
       </c>
       <c r="Q40" t="s">
         <v>499</v>
       </c>
-      <c r="R40" s="10">
+      <c r="R40" s="9">
         <v>6.9</v>
       </c>
-      <c r="T40" s="10"/>
-      <c r="AD40" s="10"/>
-      <c r="AF40" s="10"/>
+      <c r="T40" s="9"/>
+      <c r="AD40" s="9"/>
+      <c r="AE40" t="s">
+        <v>117</v>
+      </c>
+      <c r="AF40" s="9">
+        <v>17.117999999999999</v>
+      </c>
       <c r="AI40" t="s">
-        <v>109</v>
-      </c>
-      <c r="AJ40" s="10">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="41" spans="9:36" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+      <c r="AJ40" s="9">
+        <v>116</v>
+      </c>
+      <c r="AK40" s="17" t="s">
+        <v>580</v>
+      </c>
+      <c r="AL40" s="10">
+        <v>235</v>
+      </c>
+      <c r="AM40">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="41" spans="9:39" x14ac:dyDescent="0.2">
       <c r="M41" t="s">
         <v>127</v>
       </c>
-      <c r="N41" s="11">
+      <c r="N41" s="10">
         <v>152</v>
       </c>
       <c r="Q41" t="s">
         <v>426</v>
       </c>
-      <c r="R41" s="10">
+      <c r="R41" s="9">
         <v>5.4</v>
       </c>
-      <c r="T41" s="10"/>
-      <c r="AD41" s="10"/>
-      <c r="AF41" s="10"/>
+      <c r="T41" s="9"/>
+      <c r="AD41" s="9"/>
+      <c r="AE41" t="s">
+        <v>295</v>
+      </c>
+      <c r="AF41" s="9">
+        <v>18</v>
+      </c>
       <c r="AI41" t="s">
-        <v>89</v>
-      </c>
-      <c r="AJ41" s="10">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="42" spans="9:36" x14ac:dyDescent="0.2">
+        <v>112</v>
+      </c>
+      <c r="AJ41" s="9">
+        <v>140</v>
+      </c>
+      <c r="AK41" s="17" t="s">
+        <v>581</v>
+      </c>
+      <c r="AL41" s="10">
+        <v>155</v>
+      </c>
+      <c r="AM41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="9:39" x14ac:dyDescent="0.2">
       <c r="Q42" t="s">
         <v>427</v>
       </c>
-      <c r="R42" s="10">
+      <c r="R42" s="9">
         <v>3</v>
       </c>
-      <c r="T42" s="10"/>
-      <c r="AD42" s="10"/>
-      <c r="AF42" s="10"/>
+      <c r="T42" s="9"/>
+      <c r="AD42" s="9"/>
+      <c r="AF42" s="9"/>
       <c r="AI42" t="s">
-        <v>500</v>
-      </c>
-      <c r="AJ42" s="10">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="43" spans="9:36" x14ac:dyDescent="0.2">
+        <v>109</v>
+      </c>
+      <c r="AJ42" s="9">
+        <v>160</v>
+      </c>
+      <c r="AK42" s="17" t="s">
+        <v>582</v>
+      </c>
+      <c r="AL42" s="10">
+        <v>220</v>
+      </c>
+      <c r="AM42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="9:39" x14ac:dyDescent="0.2">
       <c r="Q43" t="s">
         <v>232</v>
       </c>
-      <c r="R43" s="10">
+      <c r="R43" s="9">
         <v>6.85</v>
       </c>
-      <c r="T43" s="10"/>
-      <c r="AD43" s="10"/>
-      <c r="AF43" s="10"/>
+      <c r="T43" s="9"/>
+      <c r="AD43" s="9"/>
+      <c r="AF43" s="9"/>
       <c r="AI43" t="s">
+        <v>89</v>
+      </c>
+      <c r="AJ43" s="9">
+        <v>30</v>
+      </c>
+      <c r="AK43" s="17" t="s">
+        <v>583</v>
+      </c>
+      <c r="AL43" s="10">
+        <v>140</v>
+      </c>
+      <c r="AM43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="9:39" x14ac:dyDescent="0.2">
+      <c r="Q44" t="s">
+        <v>607</v>
+      </c>
+      <c r="R44" s="9">
+        <v>1.6</v>
+      </c>
+      <c r="T44" s="9"/>
+      <c r="AD44" s="9"/>
+      <c r="AF44" s="9"/>
+      <c r="AI44" t="s">
+        <v>500</v>
+      </c>
+      <c r="AJ44" s="9">
+        <v>140</v>
+      </c>
+      <c r="AK44" s="17" t="s">
+        <v>552</v>
+      </c>
+      <c r="AL44" s="10">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="45" spans="9:39" x14ac:dyDescent="0.2">
+      <c r="Q45" t="s">
+        <v>606</v>
+      </c>
+      <c r="R45" s="9">
+        <v>3.8</v>
+      </c>
+      <c r="AF45" s="9"/>
+      <c r="AI45" t="s">
         <v>501</v>
       </c>
-      <c r="AJ43" s="10">
+      <c r="AJ45" s="9">
         <v>140</v>
       </c>
-    </row>
-    <row r="44" spans="9:36" x14ac:dyDescent="0.2">
-      <c r="Q44" t="s">
+      <c r="AK45" s="17" t="s">
+        <v>553</v>
+      </c>
+      <c r="AL45" s="10">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="46" spans="9:39" x14ac:dyDescent="0.2">
+      <c r="Q46" t="s">
         <v>430</v>
       </c>
-      <c r="R44" s="10">
+      <c r="R46" s="9">
         <v>6.9</v>
       </c>
-      <c r="T44" s="10"/>
-      <c r="AD44" s="10"/>
-      <c r="AF44" s="10"/>
-      <c r="AI44" t="s">
+      <c r="AF46" s="9"/>
+      <c r="AI46" t="s">
         <v>514</v>
       </c>
-      <c r="AJ44" s="10">
+      <c r="AJ46" s="9">
         <v>101</v>
       </c>
-    </row>
-    <row r="45" spans="9:36" x14ac:dyDescent="0.2">
-      <c r="Q45" t="s">
+      <c r="AK46" s="17" t="s">
+        <v>584</v>
+      </c>
+      <c r="AL46" s="10">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="47" spans="9:39" x14ac:dyDescent="0.2">
+      <c r="Q47" t="s">
         <v>431</v>
       </c>
-      <c r="R45" s="10">
+      <c r="R47" s="9">
         <v>5.3</v>
       </c>
-      <c r="AF45" s="10"/>
-      <c r="AI45" t="s">
+      <c r="AI47" t="s">
         <v>502</v>
       </c>
-      <c r="AJ45" s="10">
+      <c r="AJ47" s="9">
         <v>113</v>
       </c>
-    </row>
-    <row r="46" spans="9:36" x14ac:dyDescent="0.2">
-      <c r="Q46" t="s">
+      <c r="AK47" s="17" t="s">
+        <v>585</v>
+      </c>
+      <c r="AL47" s="10">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="48" spans="9:39" x14ac:dyDescent="0.2">
+      <c r="Q48" t="s">
         <v>432</v>
       </c>
-      <c r="R46" s="10">
+      <c r="R48" s="9">
         <v>7.1</v>
       </c>
-      <c r="AF46" s="10"/>
-      <c r="AI46" t="s">
+      <c r="AI48" t="s">
         <v>95</v>
       </c>
-      <c r="AJ46" s="10">
+      <c r="AJ48" s="9">
         <v>133</v>
       </c>
-    </row>
-    <row r="47" spans="9:36" x14ac:dyDescent="0.2">
-      <c r="Q47" t="s">
+      <c r="AK48" s="17" t="s">
+        <v>591</v>
+      </c>
+      <c r="AL48" s="10">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="49" spans="17:39" x14ac:dyDescent="0.2">
+      <c r="Q49" t="s">
         <v>434</v>
       </c>
-      <c r="R47" s="10">
+      <c r="R49" s="9">
         <v>8.6999999999999993</v>
       </c>
-      <c r="AI47" t="s">
+      <c r="AI49" t="s">
         <v>86</v>
       </c>
-      <c r="AJ47" s="10">
+      <c r="AJ49" s="9">
         <v>180</v>
       </c>
-    </row>
-    <row r="48" spans="9:36" x14ac:dyDescent="0.2">
-      <c r="Q48" t="s">
+      <c r="AK49" s="17" t="s">
+        <v>599</v>
+      </c>
+      <c r="AL49" s="10">
+        <v>120</v>
+      </c>
+      <c r="AM49">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="50" spans="17:39" x14ac:dyDescent="0.2">
+      <c r="Q50" t="s">
         <v>433</v>
       </c>
-      <c r="R48" s="10">
+      <c r="R50" s="9">
         <v>10</v>
       </c>
-      <c r="AI48" t="s">
+      <c r="AI50" t="s">
         <v>505</v>
       </c>
-      <c r="AJ48" s="10">
+      <c r="AJ50" s="9">
         <v>152</v>
       </c>
-    </row>
-    <row r="49" spans="17:36" x14ac:dyDescent="0.2">
-      <c r="Q49" t="s">
+      <c r="AK50" s="17" t="s">
+        <v>586</v>
+      </c>
+      <c r="AL50" s="10">
+        <v>240</v>
+      </c>
+      <c r="AM50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="17:39" x14ac:dyDescent="0.2">
+      <c r="Q51" t="s">
+        <v>605</v>
+      </c>
+      <c r="R51" s="9">
+        <v>5.6</v>
+      </c>
+      <c r="AI51" t="s">
+        <v>111</v>
+      </c>
+      <c r="AJ51" s="9">
+        <v>130</v>
+      </c>
+      <c r="AK51" s="17" t="s">
+        <v>587</v>
+      </c>
+      <c r="AL51" s="10">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="52" spans="17:39" x14ac:dyDescent="0.2">
+      <c r="Q52" t="s">
         <v>429</v>
       </c>
-      <c r="R49" s="10">
+      <c r="R52" s="9">
         <v>3.3</v>
       </c>
-      <c r="AI49" t="s">
-        <v>111</v>
-      </c>
-      <c r="AJ49" s="10">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="50" spans="17:36" x14ac:dyDescent="0.2">
-      <c r="Q50" t="s">
+      <c r="AI52" t="s">
+        <v>91</v>
+      </c>
+      <c r="AJ52" s="9">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="53" spans="17:39" x14ac:dyDescent="0.2">
+      <c r="Q53" t="s">
         <v>428</v>
       </c>
-      <c r="R50" s="10">
+      <c r="R53" s="9">
         <v>1.9</v>
       </c>
-      <c r="AI50" t="s">
-        <v>91</v>
-      </c>
-      <c r="AJ50" s="10">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="51" spans="17:36" x14ac:dyDescent="0.2">
-      <c r="Q51" t="s">
+      <c r="AJ53" s="9"/>
+    </row>
+    <row r="54" spans="17:39" x14ac:dyDescent="0.2">
+      <c r="Q54" t="s">
         <v>240</v>
       </c>
-      <c r="R51" s="10">
+      <c r="R54" s="9">
         <v>2.1</v>
       </c>
-    </row>
-    <row r="52" spans="17:36" x14ac:dyDescent="0.2">
-      <c r="Q52" t="s">
+      <c r="AJ54" s="9"/>
+      <c r="AK54" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="55" spans="17:39" x14ac:dyDescent="0.2">
+      <c r="Q55" t="s">
         <v>243</v>
       </c>
-      <c r="R52" s="10">
+      <c r="R55" s="9">
         <v>2.1</v>
       </c>
-      <c r="AJ52" s="10"/>
-    </row>
-    <row r="53" spans="17:36" x14ac:dyDescent="0.2">
-      <c r="Q53" t="s">
+      <c r="AJ55" s="9"/>
+    </row>
+    <row r="56" spans="17:39" x14ac:dyDescent="0.2">
+      <c r="Q56" t="s">
         <v>253</v>
       </c>
-      <c r="R53" s="10">
+      <c r="R56" s="9">
         <v>8.1</v>
       </c>
-      <c r="AJ53" s="10"/>
-    </row>
-    <row r="54" spans="17:36" x14ac:dyDescent="0.2">
-      <c r="Q54" t="s">
+      <c r="AJ56" s="9"/>
+    </row>
+    <row r="57" spans="17:39" x14ac:dyDescent="0.2">
+      <c r="Q57" t="s">
         <v>258</v>
       </c>
-      <c r="R54" s="10">
+      <c r="R57" s="9">
         <v>7.5</v>
       </c>
-      <c r="AJ54" s="10"/>
-    </row>
-    <row r="55" spans="17:36" x14ac:dyDescent="0.2">
-      <c r="Q55" t="s">
+      <c r="AJ57" s="9"/>
+    </row>
+    <row r="58" spans="17:39" x14ac:dyDescent="0.2">
+      <c r="Q58" t="s">
         <v>435</v>
       </c>
-      <c r="R55" s="10">
+      <c r="R58" s="9">
         <v>1.8</v>
       </c>
-      <c r="AJ55" s="10"/>
-    </row>
-    <row r="56" spans="17:36" x14ac:dyDescent="0.2">
-      <c r="Q56" t="s">
+    </row>
+    <row r="59" spans="17:39" x14ac:dyDescent="0.2">
+      <c r="Q59" t="s">
         <v>436</v>
       </c>
-      <c r="R56" s="10">
+      <c r="R59" s="9">
         <v>2.4</v>
       </c>
-      <c r="AJ56" s="10"/>
-    </row>
-    <row r="57" spans="17:36" x14ac:dyDescent="0.2">
-      <c r="Q57" t="s">
+    </row>
+    <row r="60" spans="17:39" x14ac:dyDescent="0.2">
+      <c r="Q60" t="s">
         <v>437</v>
       </c>
-      <c r="R57" s="10">
+      <c r="R60" s="9">
         <v>4.25</v>
       </c>
-      <c r="AJ57" s="10"/>
-    </row>
-    <row r="58" spans="17:36" x14ac:dyDescent="0.2">
-      <c r="Q58" t="s">
+    </row>
+    <row r="61" spans="17:39" x14ac:dyDescent="0.2">
+      <c r="Q61" t="s">
         <v>438</v>
       </c>
-      <c r="R58" s="10">
+      <c r="R61" s="9">
         <v>2.4</v>
       </c>
     </row>
-    <row r="59" spans="17:36" x14ac:dyDescent="0.2">
-      <c r="Q59" t="s">
+    <row r="62" spans="17:39" x14ac:dyDescent="0.2">
+      <c r="Q62" t="s">
         <v>263</v>
       </c>
-      <c r="R59" s="10">
+      <c r="R62" s="9">
         <v>9.4</v>
       </c>
     </row>
-    <row r="60" spans="17:36" x14ac:dyDescent="0.2">
-      <c r="Q60" t="s">
+    <row r="63" spans="17:39" x14ac:dyDescent="0.2">
+      <c r="Q63" t="s">
         <v>439</v>
       </c>
-      <c r="R60" s="10">
+      <c r="R63" s="9">
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="17:36" x14ac:dyDescent="0.2">
-      <c r="Q61" t="s">
+    <row r="64" spans="17:39" x14ac:dyDescent="0.2">
+      <c r="Q64" t="s">
         <v>264</v>
       </c>
-      <c r="R61" s="10">
+      <c r="R64" s="9">
         <v>6</v>
       </c>
     </row>
-    <row r="62" spans="17:36" x14ac:dyDescent="0.2">
-      <c r="Q62" t="s">
+    <row r="65" spans="17:18" x14ac:dyDescent="0.2">
+      <c r="Q65" t="s">
         <v>256</v>
       </c>
-      <c r="R62" s="10">
+      <c r="R65" s="9">
         <v>4.2</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="E2:F29">
-    <sortCondition ref="E2:E29"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="AE2:AF41">
+    <sortCondition ref="AE2:AE41"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="K1" r:id="rId1" xr:uid="{03BE3EB4-1121-B34D-96B6-1846C769CE18}"/>

</xml_diff>